<commit_message>
day 5 data committed on day 6 morning
</commit_message>
<xml_diff>
--- a/Data acquisition/wing_leakage_data_samples_filt.xlsx
+++ b/Data acquisition/wing_leakage_data_samples_filt.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="31">
   <si>
     <t xml:space="preserve">sample_number</t>
   </si>
@@ -300,8 +300,8 @@
   </sheetPr>
   <dimension ref="A1:S2001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A272" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F280" activeCellId="0" sqref="F280"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A306" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F320" activeCellId="0" sqref="F320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13354,9 +13354,39 @@
       <c r="C280" s="1" t="n">
         <v>2850</v>
       </c>
+      <c r="F280" s="1" t="n">
+        <v>0.0149</v>
+      </c>
+      <c r="G280" s="1" t="n">
+        <v>0.0368</v>
+      </c>
+      <c r="H280" s="1" t="n">
+        <v>0.0624</v>
+      </c>
+      <c r="I280" s="1" t="n">
+        <v>0.0399</v>
+      </c>
+      <c r="J280" s="1" t="n">
+        <v>0.0373</v>
+      </c>
+      <c r="K280" s="1" t="n">
+        <v>0.0124</v>
+      </c>
+      <c r="L280" s="1" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="M280" s="1" t="n">
+        <v>0.0505</v>
+      </c>
+      <c r="N280" s="1" t="n">
+        <v>0.0356</v>
+      </c>
+      <c r="O280" s="1" t="n">
+        <v>0.0191</v>
+      </c>
       <c r="P280" s="1" t="n">
         <f aca="false">SUM(F280:O280)</f>
-        <v>0</v>
+        <v>0.3379</v>
       </c>
       <c r="R280" s="1" t="n">
         <v>5</v>
@@ -13381,9 +13411,39 @@
       <c r="E281" s="1" t="n">
         <v>1350</v>
       </c>
+      <c r="F281" s="1" t="n">
+        <v>0.0171</v>
+      </c>
+      <c r="G281" s="1" t="n">
+        <v>0.0396</v>
+      </c>
+      <c r="H281" s="1" t="n">
+        <v>0.0678</v>
+      </c>
+      <c r="I281" s="1" t="n">
+        <v>0.0591</v>
+      </c>
+      <c r="J281" s="1" t="n">
+        <v>0.0995</v>
+      </c>
+      <c r="K281" s="1" t="n">
+        <v>0.0151</v>
+      </c>
+      <c r="L281" s="1" t="n">
+        <v>0.0315</v>
+      </c>
+      <c r="M281" s="1" t="n">
+        <v>0.0565</v>
+      </c>
+      <c r="N281" s="1" t="n">
+        <v>0.0585</v>
+      </c>
+      <c r="O281" s="1" t="n">
+        <v>0.1891</v>
+      </c>
       <c r="P281" s="1" t="n">
         <f aca="false">SUM(F281:O281)</f>
-        <v>0</v>
+        <v>0.6338</v>
       </c>
       <c r="R281" s="1" t="n">
         <v>5</v>
@@ -13402,9 +13462,39 @@
       <c r="C282" s="1" t="n">
         <v>1350</v>
       </c>
+      <c r="F282" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G282" s="1" t="n">
+        <v>0.0117</v>
+      </c>
+      <c r="H282" s="1" t="n">
+        <v>0.0129</v>
+      </c>
+      <c r="I282" s="1" t="n">
+        <v>0.0256</v>
+      </c>
+      <c r="J282" s="1" t="n">
+        <v>0.0884</v>
+      </c>
+      <c r="K282" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L282" s="1" t="n">
+        <v>0.0097</v>
+      </c>
+      <c r="M282" s="1" t="n">
+        <v>0.0098</v>
+      </c>
+      <c r="N282" s="1" t="n">
+        <v>0.0287</v>
+      </c>
+      <c r="O282" s="1" t="n">
+        <v>0.1759</v>
+      </c>
       <c r="P282" s="1" t="n">
         <f aca="false">SUM(F282:O282)</f>
-        <v>0</v>
+        <v>0.3627</v>
       </c>
       <c r="R282" s="1" t="n">
         <v>5</v>
@@ -13429,9 +13519,39 @@
       <c r="E283" s="1" t="n">
         <v>4100</v>
       </c>
+      <c r="F283" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G283" s="1" t="n">
+        <v>0.0096</v>
+      </c>
+      <c r="H283" s="1" t="n">
+        <v>0.0161</v>
+      </c>
+      <c r="I283" s="1" t="n">
+        <v>0.0512</v>
+      </c>
+      <c r="J283" s="1" t="n">
+        <v>0.2598</v>
+      </c>
+      <c r="K283" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L283" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M283" s="1" t="n">
+        <v>0.0132</v>
+      </c>
+      <c r="N283" s="1" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="O283" s="1" t="n">
+        <v>0.2461</v>
+      </c>
       <c r="P283" s="1" t="n">
         <f aca="false">SUM(F283:O283)</f>
-        <v>0</v>
+        <v>0.644</v>
       </c>
       <c r="R283" s="1" t="n">
         <v>5</v>
@@ -13450,9 +13570,39 @@
       <c r="C284" s="1" t="n">
         <v>4100</v>
       </c>
+      <c r="F284" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G284" s="1" t="n">
+        <v>0.0025</v>
+      </c>
+      <c r="H284" s="1" t="n">
+        <v>0.0115</v>
+      </c>
+      <c r="I284" s="1" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="J284" s="1" t="n">
+        <v>0.2011</v>
+      </c>
+      <c r="K284" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L284" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M284" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N284" s="1" t="n">
+        <v>0.0251</v>
+      </c>
+      <c r="O284" s="1" t="n">
+        <v>0.0786</v>
+      </c>
       <c r="P284" s="1" t="n">
         <f aca="false">SUM(F284:O284)</f>
-        <v>0</v>
+        <v>0.3508</v>
       </c>
       <c r="R284" s="1" t="n">
         <v>5</v>
@@ -13477,9 +13627,39 @@
       <c r="E285" s="1" t="n">
         <v>2100</v>
       </c>
+      <c r="F285" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G285" s="1" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="H285" s="1" t="n">
+        <v>0.0156</v>
+      </c>
+      <c r="I285" s="1" t="n">
+        <v>0.0537</v>
+      </c>
+      <c r="J285" s="1" t="n">
+        <v>0.2748</v>
+      </c>
+      <c r="K285" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L285" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M285" s="1" t="n">
+        <v>0.0126</v>
+      </c>
+      <c r="N285" s="1" t="n">
+        <v>0.0488</v>
+      </c>
+      <c r="O285" s="1" t="n">
+        <v>0.2133</v>
+      </c>
       <c r="P285" s="1" t="n">
         <f aca="false">SUM(F285:O285)</f>
-        <v>0</v>
+        <v>0.6248</v>
       </c>
       <c r="R285" s="1" t="n">
         <v>5</v>
@@ -13498,9 +13678,39 @@
       <c r="C286" s="1" t="n">
         <v>2100</v>
       </c>
+      <c r="F286" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G286" s="1" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="H286" s="1" t="n">
+        <v>0.0114</v>
+      </c>
+      <c r="I286" s="1" t="n">
+        <v>0.0276</v>
+      </c>
+      <c r="J286" s="1" t="n">
+        <v>0.1033</v>
+      </c>
+      <c r="K286" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L286" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M286" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N286" s="1" t="n">
+        <v>0.0288</v>
+      </c>
+      <c r="O286" s="1" t="n">
+        <v>0.142</v>
+      </c>
       <c r="P286" s="1" t="n">
         <f aca="false">SUM(F286:O286)</f>
-        <v>0</v>
+        <v>0.3147</v>
       </c>
       <c r="R286" s="1" t="n">
         <v>5</v>
@@ -13525,9 +13735,39 @@
       <c r="E287" s="1" t="n">
         <v>350</v>
       </c>
+      <c r="F287" s="1" t="n">
+        <v>0.0362</v>
+      </c>
+      <c r="G287" s="1" t="n">
+        <v>0.0374</v>
+      </c>
+      <c r="H287" s="1" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="I287" s="1" t="n">
+        <v>0.0331</v>
+      </c>
+      <c r="J287" s="1" t="n">
+        <v>0.1051</v>
+      </c>
+      <c r="K287" s="1" t="n">
+        <v>0.0812</v>
+      </c>
+      <c r="L287" s="1" t="n">
+        <v>0.1097</v>
+      </c>
+      <c r="M287" s="1" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N287" s="1" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="O287" s="1" t="n">
+        <v>0.1441</v>
+      </c>
       <c r="P287" s="1" t="n">
         <f aca="false">SUM(F287:O287)</f>
-        <v>0</v>
+        <v>0.6378</v>
       </c>
       <c r="R287" s="1" t="n">
         <v>5</v>
@@ -13546,9 +13786,39 @@
       <c r="C288" s="1" t="n">
         <v>350</v>
       </c>
+      <c r="F288" s="1" t="n">
+        <v>0.0364</v>
+      </c>
+      <c r="G288" s="1" t="n">
+        <v>0.0369</v>
+      </c>
+      <c r="H288" s="1" t="n">
+        <v>0.0224</v>
+      </c>
+      <c r="I288" s="1" t="n">
+        <v>0.0128</v>
+      </c>
+      <c r="J288" s="1" t="n">
+        <v>0.0294</v>
+      </c>
+      <c r="K288" s="1" t="n">
+        <v>0.0814</v>
+      </c>
+      <c r="L288" s="1" t="n">
+        <v>0.109</v>
+      </c>
+      <c r="M288" s="1" t="n">
+        <v>0.0258</v>
+      </c>
+      <c r="N288" s="1" t="n">
+        <v>0.0128</v>
+      </c>
+      <c r="O288" s="1" t="n">
+        <v>0.0098</v>
+      </c>
       <c r="P288" s="1" t="n">
         <f aca="false">SUM(F288:O288)</f>
-        <v>0</v>
+        <v>0.3767</v>
       </c>
       <c r="R288" s="1" t="n">
         <v>5</v>
@@ -13573,9 +13843,39 @@
       <c r="E289" s="1" t="n">
         <v>4100</v>
       </c>
+      <c r="F289" s="1" t="n">
+        <v>0.0464</v>
+      </c>
+      <c r="G289" s="1" t="n">
+        <v>0.067</v>
+      </c>
+      <c r="H289" s="1" t="n">
+        <v>0.1219</v>
+      </c>
+      <c r="I289" s="1" t="n">
+        <v>0.0553</v>
+      </c>
+      <c r="J289" s="1" t="n">
+        <v>0.0389</v>
+      </c>
+      <c r="K289" s="1" t="n">
+        <v>0.0904</v>
+      </c>
+      <c r="L289" s="1" t="n">
+        <v>0.1252</v>
+      </c>
+      <c r="M289" s="1" t="n">
+        <v>0.0544</v>
+      </c>
+      <c r="N289" s="1" t="n">
+        <v>0.0356</v>
+      </c>
+      <c r="O289" s="1" t="n">
+        <v>0.0198</v>
+      </c>
       <c r="P289" s="1" t="n">
         <f aca="false">SUM(F289:O289)</f>
-        <v>0</v>
+        <v>0.6549</v>
       </c>
       <c r="R289" s="1" t="n">
         <v>5</v>
@@ -13594,9 +13894,39 @@
       <c r="C290" s="1" t="n">
         <v>4100</v>
       </c>
+      <c r="F290" s="1" t="n">
+        <v>0.0159</v>
+      </c>
+      <c r="G290" s="1" t="n">
+        <v>0.0383</v>
+      </c>
+      <c r="H290" s="1" t="n">
+        <v>0.1065</v>
+      </c>
+      <c r="I290" s="1" t="n">
+        <v>0.0492</v>
+      </c>
+      <c r="J290" s="1" t="n">
+        <v>0.0371</v>
+      </c>
+      <c r="K290" s="1" t="n">
+        <v>0.0133</v>
+      </c>
+      <c r="L290" s="1" t="n">
+        <v>0.0228</v>
+      </c>
+      <c r="M290" s="1" t="n">
+        <v>0.0324</v>
+      </c>
+      <c r="N290" s="1" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="O290" s="1" t="n">
+        <v>0.0174</v>
+      </c>
       <c r="P290" s="1" t="n">
         <f aca="false">SUM(F290:O290)</f>
-        <v>0</v>
+        <v>0.3619</v>
       </c>
       <c r="R290" s="1" t="n">
         <v>5</v>
@@ -13621,9 +13951,39 @@
       <c r="E291" s="1" t="n">
         <v>2100</v>
       </c>
+      <c r="F291" s="1" t="n">
+        <v>0.0158</v>
+      </c>
+      <c r="G291" s="1" t="n">
+        <v>0.0412</v>
+      </c>
+      <c r="H291" s="1" t="n">
+        <v>0.1174</v>
+      </c>
+      <c r="I291" s="1" t="n">
+        <v>0.0883</v>
+      </c>
+      <c r="J291" s="1" t="n">
+        <v>0.0937</v>
+      </c>
+      <c r="K291" s="1" t="n">
+        <v>0.0127</v>
+      </c>
+      <c r="L291" s="1" t="n">
+        <v>0.0256</v>
+      </c>
+      <c r="M291" s="1" t="n">
+        <v>0.0458</v>
+      </c>
+      <c r="N291" s="1" t="n">
+        <v>0.0861</v>
+      </c>
+      <c r="O291" s="1" t="n">
+        <v>0.1109</v>
+      </c>
       <c r="P291" s="1" t="n">
         <f aca="false">SUM(F291:O291)</f>
-        <v>0</v>
+        <v>0.6375</v>
       </c>
       <c r="R291" s="1" t="n">
         <v>5</v>
@@ -13666,9 +14026,39 @@
       <c r="E293" s="1" t="n">
         <v>1100</v>
       </c>
+      <c r="F293" s="1" t="n">
+        <v>0.0095</v>
+      </c>
+      <c r="G293" s="1" t="n">
+        <v>0.0194</v>
+      </c>
+      <c r="H293" s="1" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="I293" s="1" t="n">
+        <v>0.0826</v>
+      </c>
+      <c r="J293" s="1" t="n">
+        <v>0.117</v>
+      </c>
+      <c r="K293" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L293" s="1" t="n">
+        <v>0.0168</v>
+      </c>
+      <c r="M293" s="1" t="n">
+        <v>0.0424</v>
+      </c>
+      <c r="N293" s="1" t="n">
+        <v>0.2085</v>
+      </c>
+      <c r="O293" s="1" t="n">
+        <v>0.1709</v>
+      </c>
       <c r="P293" s="1" t="n">
         <f aca="false">SUM(F293:O293)</f>
-        <v>0</v>
+        <v>0.7021</v>
       </c>
       <c r="R293" s="1" t="n">
         <v>5</v>
@@ -13687,9 +14077,39 @@
       <c r="C294" s="1" t="n">
         <v>1100</v>
       </c>
+      <c r="F294" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G294" s="1" t="n">
+        <v>0.0141</v>
+      </c>
+      <c r="H294" s="1" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="I294" s="1" t="n">
+        <v>0.042</v>
+      </c>
+      <c r="J294" s="1" t="n">
+        <v>0.0614</v>
+      </c>
+      <c r="K294" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L294" s="1" t="n">
+        <v>0.0122</v>
+      </c>
+      <c r="M294" s="1" t="n">
+        <v>0.0274</v>
+      </c>
+      <c r="N294" s="1" t="n">
+        <v>0.1489</v>
+      </c>
+      <c r="O294" s="1" t="n">
+        <v>0.0774</v>
+      </c>
       <c r="P294" s="1" t="n">
         <f aca="false">SUM(F294:O294)</f>
-        <v>0</v>
+        <v>0.4054</v>
       </c>
       <c r="R294" s="1" t="n">
         <v>5</v>
@@ -13714,9 +14134,39 @@
       <c r="E295" s="1" t="n">
         <v>850</v>
       </c>
+      <c r="F295" s="1" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="G295" s="1" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="H295" s="1" t="n">
+        <v>0.0441</v>
+      </c>
+      <c r="I295" s="1" t="n">
+        <v>0.0639</v>
+      </c>
+      <c r="J295" s="1" t="n">
+        <v>0.0698</v>
+      </c>
+      <c r="K295" s="1" t="n">
+        <v>0.0119</v>
+      </c>
+      <c r="L295" s="1" t="n">
+        <v>0.0276</v>
+      </c>
+      <c r="M295" s="1" t="n">
+        <v>0.1015</v>
+      </c>
+      <c r="N295" s="1" t="n">
+        <v>0.196</v>
+      </c>
+      <c r="O295" s="1" t="n">
+        <v>0.0856</v>
+      </c>
       <c r="P295" s="1" t="n">
         <f aca="false">SUM(F295:O295)</f>
-        <v>0</v>
+        <v>0.6404</v>
       </c>
       <c r="R295" s="1" t="n">
         <v>5</v>
@@ -13759,9 +14209,39 @@
       <c r="E297" s="1" t="n">
         <v>850</v>
       </c>
+      <c r="F297" s="1" t="n">
+        <v>0.0126</v>
+      </c>
+      <c r="G297" s="1" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="H297" s="1" t="n">
+        <v>0.0422</v>
+      </c>
+      <c r="I297" s="1" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="J297" s="1" t="n">
+        <v>0.0736</v>
+      </c>
+      <c r="K297" s="1" t="n">
+        <v>0.0114</v>
+      </c>
+      <c r="L297" s="1" t="n">
+        <v>0.0267</v>
+      </c>
+      <c r="M297" s="1" t="n">
+        <v>0.0979</v>
+      </c>
+      <c r="N297" s="1" t="n">
+        <v>0.174</v>
+      </c>
+      <c r="O297" s="1" t="n">
+        <v>0.106</v>
+      </c>
       <c r="P297" s="1" t="n">
         <f aca="false">SUM(F297:O297)</f>
-        <v>0</v>
+        <v>0.6329</v>
       </c>
       <c r="R297" s="1" t="n">
         <v>5</v>
@@ -13780,9 +14260,39 @@
       <c r="C298" s="1" t="n">
         <v>850</v>
       </c>
+      <c r="F298" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G298" s="1" t="n">
+        <v>0.0127</v>
+      </c>
+      <c r="H298" s="1" t="n">
+        <v>0.0176</v>
+      </c>
+      <c r="I298" s="1" t="n">
+        <v>0.0344</v>
+      </c>
+      <c r="J298" s="1" t="n">
+        <v>0.059</v>
+      </c>
+      <c r="K298" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L298" s="1" t="n">
+        <v>0.0106</v>
+      </c>
+      <c r="M298" s="1" t="n">
+        <v>0.0196</v>
+      </c>
+      <c r="N298" s="1" t="n">
+        <v>0.1017</v>
+      </c>
+      <c r="O298" s="1" t="n">
+        <v>0.0851</v>
+      </c>
       <c r="P298" s="1" t="n">
         <f aca="false">SUM(F298:O298)</f>
-        <v>0</v>
+        <v>0.3407</v>
       </c>
       <c r="R298" s="1" t="n">
         <v>5</v>
@@ -13807,9 +14317,39 @@
       <c r="E299" s="1" t="n">
         <v>4350</v>
       </c>
+      <c r="F299" s="1" t="n">
+        <v>0.0154</v>
+      </c>
+      <c r="G299" s="1" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H299" s="1" t="n">
+        <v>0.1376</v>
+      </c>
+      <c r="I299" s="1" t="n">
+        <v>0.0648</v>
+      </c>
+      <c r="J299" s="1" t="n">
+        <v>0.0673</v>
+      </c>
+      <c r="K299" s="1" t="n">
+        <v>0.0111</v>
+      </c>
+      <c r="L299" s="1" t="n">
+        <v>0.0246</v>
+      </c>
+      <c r="M299" s="1" t="n">
+        <v>0.0435</v>
+      </c>
+      <c r="N299" s="1" t="n">
+        <v>0.1191</v>
+      </c>
+      <c r="O299" s="1" t="n">
+        <v>0.0936</v>
+      </c>
       <c r="P299" s="1" t="n">
         <f aca="false">SUM(F299:O299)</f>
-        <v>0</v>
+        <v>0.627</v>
       </c>
       <c r="R299" s="1" t="n">
         <v>5</v>
@@ -13828,9 +14368,39 @@
       <c r="C300" s="1" t="n">
         <v>4350</v>
       </c>
+      <c r="F300" s="1" t="n">
+        <v>0.0167</v>
+      </c>
+      <c r="G300" s="1" t="n">
+        <v>0.0436</v>
+      </c>
+      <c r="H300" s="1" t="n">
+        <v>0.1276</v>
+      </c>
+      <c r="I300" s="1" t="n">
+        <v>0.0373</v>
+      </c>
+      <c r="J300" s="1" t="n">
+        <v>0.0346</v>
+      </c>
+      <c r="K300" s="1" t="n">
+        <v>0.0131</v>
+      </c>
+      <c r="L300" s="1" t="n">
+        <v>0.0224</v>
+      </c>
+      <c r="M300" s="1" t="n">
+        <v>0.0286</v>
+      </c>
+      <c r="N300" s="1" t="n">
+        <v>0.0233</v>
+      </c>
+      <c r="O300" s="1" t="n">
+        <v>0.0147</v>
+      </c>
       <c r="P300" s="1" t="n">
         <f aca="false">SUM(F300:O300)</f>
-        <v>0</v>
+        <v>0.3619</v>
       </c>
       <c r="R300" s="1" t="n">
         <v>5</v>
@@ -13855,9 +14425,42 @@
       <c r="E301" s="1" t="n">
         <v>4600</v>
       </c>
+      <c r="F301" s="1" t="n">
+        <v>0.0954</v>
+      </c>
+      <c r="G301" s="1" t="n">
+        <v>0.1314</v>
+      </c>
+      <c r="H301" s="1" t="n">
+        <v>0.1484</v>
+      </c>
+      <c r="I301" s="1" t="n">
+        <v>0.0428</v>
+      </c>
+      <c r="J301" s="1" t="n">
+        <v>0.0352</v>
+      </c>
+      <c r="K301" s="1" t="n">
+        <v>0.0475</v>
+      </c>
+      <c r="L301" s="1" t="n">
+        <v>0.0493</v>
+      </c>
+      <c r="M301" s="1" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="N301" s="1" t="n">
+        <v>0.0282</v>
+      </c>
+      <c r="O301" s="1" t="n">
+        <v>0.0156</v>
+      </c>
       <c r="P301" s="1" t="n">
         <f aca="false">SUM(F301:O301)</f>
-        <v>0</v>
+        <v>0.6368</v>
+      </c>
+      <c r="R301" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="S301" s="1" t="n">
         <v>2</v>
@@ -13873,9 +14476,42 @@
       <c r="C302" s="1" t="n">
         <v>4600</v>
       </c>
+      <c r="F302" s="1" t="n">
+        <v>0.0848</v>
+      </c>
+      <c r="G302" s="1" t="n">
+        <v>0.0966</v>
+      </c>
+      <c r="H302" s="1" t="n">
+        <v>0.0287</v>
+      </c>
+      <c r="I302" s="1" t="n">
+        <v>0.0129</v>
+      </c>
+      <c r="J302" s="1" t="n">
+        <v>0.0278</v>
+      </c>
+      <c r="K302" s="1" t="n">
+        <v>0.0385</v>
+      </c>
+      <c r="L302" s="1" t="n">
+        <v>0.0338</v>
+      </c>
+      <c r="M302" s="1" t="n">
+        <v>0.0193</v>
+      </c>
+      <c r="N302" s="1" t="n">
+        <v>0.0114</v>
+      </c>
+      <c r="O302" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P302" s="1" t="n">
         <f aca="false">SUM(F302:O302)</f>
-        <v>0</v>
+        <v>0.3538</v>
+      </c>
+      <c r="R302" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="S302" s="1" t="n">
         <v>1</v>
@@ -13901,6 +14537,12 @@
         <f aca="false">SUM(F303:O303)</f>
         <v>0</v>
       </c>
+      <c r="Q303" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R303" s="1" t="n">
+        <v>5</v>
+      </c>
       <c r="S303" s="1" t="n">
         <v>2</v>
       </c>
@@ -13919,6 +14561,12 @@
         <f aca="false">SUM(F304:O304)</f>
         <v>0</v>
       </c>
+      <c r="Q304" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R304" s="1" t="n">
+        <v>5</v>
+      </c>
       <c r="S304" s="1" t="n">
         <v>1</v>
       </c>
@@ -13943,6 +14591,12 @@
         <f aca="false">SUM(F305:O305)</f>
         <v>0</v>
       </c>
+      <c r="Q305" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R305" s="1" t="n">
+        <v>5</v>
+      </c>
       <c r="S305" s="1" t="n">
         <v>2</v>
       </c>
@@ -13957,9 +14611,42 @@
       <c r="C306" s="1" t="n">
         <v>600</v>
       </c>
+      <c r="F306" s="1" t="n">
+        <v>0.0453</v>
+      </c>
+      <c r="G306" s="1" t="n">
+        <v>0.0329</v>
+      </c>
+      <c r="H306" s="1" t="n">
+        <v>0.0162</v>
+      </c>
+      <c r="I306" s="1" t="n">
+        <v>0.0037</v>
+      </c>
+      <c r="J306" s="1" t="n">
+        <v>0.0254</v>
+      </c>
+      <c r="K306" s="1" t="n">
+        <v>0.1581</v>
+      </c>
+      <c r="L306" s="1" t="n">
+        <v>0.0404</v>
+      </c>
+      <c r="M306" s="1" t="n">
+        <v>0.0146</v>
+      </c>
+      <c r="N306" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O306" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P306" s="1" t="n">
         <f aca="false">SUM(F306:O306)</f>
-        <v>0</v>
+        <v>0.3366</v>
+      </c>
+      <c r="R306" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="S306" s="1" t="n">
         <v>1</v>
@@ -13981,9 +14668,42 @@
       <c r="E307" s="1" t="n">
         <v>1350</v>
       </c>
+      <c r="F307" s="1" t="n">
+        <v>0.088</v>
+      </c>
+      <c r="G307" s="1" t="n">
+        <v>0.0642</v>
+      </c>
+      <c r="H307" s="1" t="n">
+        <v>0.0288</v>
+      </c>
+      <c r="I307" s="1" t="n">
+        <v>0.0119</v>
+      </c>
+      <c r="J307" s="1" t="n">
+        <v>0.0251</v>
+      </c>
+      <c r="K307" s="1" t="n">
+        <v>0.2659</v>
+      </c>
+      <c r="L307" s="1" t="n">
+        <v>0.0924</v>
+      </c>
+      <c r="M307" s="1" t="n">
+        <v>0.0301</v>
+      </c>
+      <c r="N307" s="1" t="n">
+        <v>0.0118</v>
+      </c>
+      <c r="O307" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P307" s="1" t="n">
         <f aca="false">SUM(F307:O307)</f>
-        <v>0</v>
+        <v>0.6182</v>
+      </c>
+      <c r="R307" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="S307" s="1" t="n">
         <v>2</v>
@@ -13999,9 +14719,42 @@
       <c r="C308" s="1" t="n">
         <v>1350</v>
       </c>
+      <c r="F308" s="1" t="n">
+        <v>0.0507</v>
+      </c>
+      <c r="G308" s="1" t="n">
+        <v>0.0419</v>
+      </c>
+      <c r="H308" s="1" t="n">
+        <v>0.0214</v>
+      </c>
+      <c r="I308" s="1" t="n">
+        <v>0.0115</v>
+      </c>
+      <c r="J308" s="1" t="n">
+        <v>0.0259</v>
+      </c>
+      <c r="K308" s="1" t="n">
+        <v>0.1162</v>
+      </c>
+      <c r="L308" s="1" t="n">
+        <v>0.0592</v>
+      </c>
+      <c r="M308" s="1" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="N308" s="1" t="n">
+        <v>0.0106</v>
+      </c>
+      <c r="O308" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P308" s="1" t="n">
         <f aca="false">SUM(F308:O308)</f>
-        <v>0</v>
+        <v>0.3584</v>
+      </c>
+      <c r="R308" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="S308" s="1" t="n">
         <v>1</v>
@@ -14023,9 +14776,42 @@
       <c r="E309" s="1" t="n">
         <v>3100</v>
       </c>
+      <c r="F309" s="1" t="n">
+        <v>0.0504</v>
+      </c>
+      <c r="G309" s="1" t="n">
+        <v>0.0444</v>
+      </c>
+      <c r="H309" s="1" t="n">
+        <v>0.0335</v>
+      </c>
+      <c r="I309" s="1" t="n">
+        <v>0.0726</v>
+      </c>
+      <c r="J309" s="1" t="n">
+        <v>0.1297</v>
+      </c>
+      <c r="K309" s="1" t="n">
+        <v>0.1161</v>
+      </c>
+      <c r="L309" s="1" t="n">
+        <v>0.0616</v>
+      </c>
+      <c r="M309" s="1" t="n">
+        <v>0.0334</v>
+      </c>
+      <c r="N309" s="1" t="n">
+        <v>0.0556</v>
+      </c>
+      <c r="O309" s="1" t="n">
+        <v>0.0915</v>
+      </c>
       <c r="P309" s="1" t="n">
         <f aca="false">SUM(F309:O309)</f>
-        <v>0</v>
+        <v>0.6888</v>
+      </c>
+      <c r="R309" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="S309" s="1" t="n">
         <v>2</v>
@@ -14041,9 +14827,42 @@
       <c r="C310" s="1" t="n">
         <v>3100</v>
       </c>
+      <c r="F310" s="1" t="n">
+        <v>0.0105</v>
+      </c>
+      <c r="G310" s="1" t="n">
+        <v>0.0164</v>
+      </c>
+      <c r="H310" s="1" t="n">
+        <v>0.0224</v>
+      </c>
+      <c r="I310" s="1" t="n">
+        <v>0.0688</v>
+      </c>
+      <c r="J310" s="1" t="n">
+        <v>0.1282</v>
+      </c>
+      <c r="K310" s="1" t="n">
+        <v>0.0091</v>
+      </c>
+      <c r="L310" s="1" t="n">
+        <v>0.0127</v>
+      </c>
+      <c r="M310" s="1" t="n">
+        <v>0.0192</v>
+      </c>
+      <c r="N310" s="1" t="n">
+        <v>0.0513</v>
+      </c>
+      <c r="O310" s="1" t="n">
+        <v>0.094</v>
+      </c>
       <c r="P310" s="1" t="n">
         <f aca="false">SUM(F310:O310)</f>
-        <v>0</v>
+        <v>0.4326</v>
+      </c>
+      <c r="R310" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="S310" s="1" t="n">
         <v>1</v>
@@ -14065,9 +14884,42 @@
       <c r="E311" s="1" t="n">
         <v>600</v>
       </c>
+      <c r="F311" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G311" s="1" t="n">
+        <v>0.0154</v>
+      </c>
+      <c r="H311" s="1" t="n">
+        <v>0.0284</v>
+      </c>
+      <c r="I311" s="1" t="n">
+        <v>0.0864</v>
+      </c>
+      <c r="J311" s="1" t="n">
+        <v>0.1446</v>
+      </c>
+      <c r="K311" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L311" s="1" t="n">
+        <v>0.0126</v>
+      </c>
+      <c r="M311" s="1" t="n">
+        <v>0.0322</v>
+      </c>
+      <c r="N311" s="1" t="n">
+        <v>0.2154</v>
+      </c>
+      <c r="O311" s="1" t="n">
+        <v>0.1245</v>
+      </c>
       <c r="P311" s="1" t="n">
         <f aca="false">SUM(F311:O311)</f>
-        <v>0</v>
+        <v>0.6595</v>
+      </c>
+      <c r="R311" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="S311" s="1" t="n">
         <v>2</v>
@@ -14083,9 +14935,42 @@
       <c r="C312" s="1" t="n">
         <v>600</v>
       </c>
+      <c r="F312" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G312" s="1" t="n">
+        <v>0.0107</v>
+      </c>
+      <c r="H312" s="1" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="I312" s="1" t="n">
+        <v>0.0241</v>
+      </c>
+      <c r="J312" s="1" t="n">
+        <v>0.0427</v>
+      </c>
+      <c r="K312" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L312" s="1" t="n">
+        <v>0.0089</v>
+      </c>
+      <c r="M312" s="1" t="n">
+        <v>0.0178</v>
+      </c>
+      <c r="N312" s="1" t="n">
+        <v>0.1681</v>
+      </c>
+      <c r="O312" s="1" t="n">
+        <v>0.0404</v>
+      </c>
       <c r="P312" s="1" t="n">
         <f aca="false">SUM(F312:O312)</f>
-        <v>0</v>
+        <v>0.3267</v>
+      </c>
+      <c r="R312" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="S312" s="1" t="n">
         <v>1</v>
@@ -14107,9 +14992,42 @@
       <c r="E313" s="1" t="n">
         <v>1850</v>
       </c>
+      <c r="F313" s="1" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G313" s="1" t="n">
+        <v>0.0257</v>
+      </c>
+      <c r="H313" s="1" t="n">
+        <v>0.0468</v>
+      </c>
+      <c r="I313" s="1" t="n">
+        <v>0.0626</v>
+      </c>
+      <c r="J313" s="1" t="n">
+        <v>0.0604</v>
+      </c>
+      <c r="K313" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L313" s="1" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="M313" s="1" t="n">
+        <v>0.0773</v>
+      </c>
+      <c r="N313" s="1" t="n">
+        <v>0.2303</v>
+      </c>
+      <c r="O313" s="1" t="n">
+        <v>0.0629</v>
+      </c>
       <c r="P313" s="1" t="n">
         <f aca="false">SUM(F313:O313)</f>
-        <v>0</v>
+        <v>0.6</v>
+      </c>
+      <c r="R313" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="S313" s="1" t="n">
         <v>2</v>
@@ -14125,9 +15043,42 @@
       <c r="C314" s="1" t="n">
         <v>1850</v>
       </c>
+      <c r="F314" s="1" t="n">
+        <v>0.0116</v>
+      </c>
+      <c r="G314" s="1" t="n">
+        <v>0.0243</v>
+      </c>
+      <c r="H314" s="1" t="n">
+        <v>0.0391</v>
+      </c>
+      <c r="I314" s="1" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="J314" s="1" t="n">
+        <v>0.0427</v>
+      </c>
+      <c r="K314" s="1" t="n">
+        <v>0.0101</v>
+      </c>
+      <c r="L314" s="1" t="n">
+        <v>0.0227</v>
+      </c>
+      <c r="M314" s="1" t="n">
+        <v>0.0635</v>
+      </c>
+      <c r="N314" s="1" t="n">
+        <v>0.0648</v>
+      </c>
+      <c r="O314" s="1" t="n">
+        <v>0.0272</v>
+      </c>
       <c r="P314" s="1" t="n">
         <f aca="false">SUM(F314:O314)</f>
-        <v>0</v>
+        <v>0.35</v>
+      </c>
+      <c r="R314" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="S314" s="1" t="n">
         <v>1</v>
@@ -14149,9 +15100,42 @@
       <c r="E315" s="1" t="n">
         <v>2850</v>
       </c>
+      <c r="F315" s="1" t="n">
+        <v>0.0509</v>
+      </c>
+      <c r="G315" s="1" t="n">
+        <v>0.0871</v>
+      </c>
+      <c r="H315" s="1" t="n">
+        <v>0.0736</v>
+      </c>
+      <c r="I315" s="1" t="n">
+        <v>0.0567</v>
+      </c>
+      <c r="J315" s="1" t="n">
+        <v>0.0472</v>
+      </c>
+      <c r="K315" s="1" t="n">
+        <v>0.0484</v>
+      </c>
+      <c r="L315" s="1" t="n">
+        <v>0.0715</v>
+      </c>
+      <c r="M315" s="1" t="n">
+        <v>0.0952</v>
+      </c>
+      <c r="N315" s="1" t="n">
+        <v>0.0775</v>
+      </c>
+      <c r="O315" s="1" t="n">
+        <v>0.0323</v>
+      </c>
       <c r="P315" s="1" t="n">
         <f aca="false">SUM(F315:O315)</f>
-        <v>0</v>
+        <v>0.6404</v>
+      </c>
+      <c r="R315" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="S315" s="1" t="n">
         <v>2</v>
@@ -14167,9 +15151,42 @@
       <c r="C316" s="1" t="n">
         <v>2850</v>
       </c>
+      <c r="F316" s="1" t="n">
+        <v>0.0439</v>
+      </c>
+      <c r="G316" s="1" t="n">
+        <v>0.0696</v>
+      </c>
+      <c r="H316" s="1" t="n">
+        <v>0.0394</v>
+      </c>
+      <c r="I316" s="1" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="J316" s="1" t="n">
+        <v>0.0293</v>
+      </c>
+      <c r="K316" s="1" t="n">
+        <v>0.0406</v>
+      </c>
+      <c r="L316" s="1" t="n">
+        <v>0.054</v>
+      </c>
+      <c r="M316" s="1" t="n">
+        <v>0.0344</v>
+      </c>
+      <c r="N316" s="1" t="n">
+        <v>0.0155</v>
+      </c>
+      <c r="O316" s="1" t="n">
+        <v>0.0097</v>
+      </c>
       <c r="P316" s="1" t="n">
         <f aca="false">SUM(F316:O316)</f>
-        <v>0</v>
+        <v>0.3544</v>
+      </c>
+      <c r="R316" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="S316" s="1" t="n">
         <v>1</v>
@@ -14195,6 +15212,12 @@
         <f aca="false">SUM(F317:O317)</f>
         <v>0</v>
       </c>
+      <c r="Q317" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R317" s="1" t="n">
+        <v>5</v>
+      </c>
       <c r="S317" s="1" t="n">
         <v>2</v>
       </c>
@@ -14213,6 +15236,12 @@
         <f aca="false">SUM(F318:O318)</f>
         <v>0</v>
       </c>
+      <c r="Q318" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R318" s="1" t="n">
+        <v>5</v>
+      </c>
       <c r="S318" s="1" t="n">
         <v>1</v>
       </c>
@@ -14237,12 +15266,18 @@
         <f aca="false">SUM(F319:O319)</f>
         <v>0</v>
       </c>
+      <c r="Q319" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R319" s="1" t="n">
+        <v>5</v>
+      </c>
       <c r="S319" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A320" s="1" t="n">
+      <c r="A320" s="4" t="n">
         <v>318</v>
       </c>
       <c r="B320" s="1" t="n">
@@ -14254,6 +15289,9 @@
       <c r="P320" s="1" t="n">
         <f aca="false">SUM(F320:O320)</f>
         <v>0</v>
+      </c>
+      <c r="R320" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="S320" s="1" t="n">
         <v>1</v>
@@ -14279,6 +15317,9 @@
         <f aca="false">SUM(F321:O321)</f>
         <v>0</v>
       </c>
+      <c r="R321" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S321" s="1" t="n">
         <v>2</v>
       </c>
@@ -14297,6 +15338,9 @@
         <f aca="false">SUM(F322:O322)</f>
         <v>0</v>
       </c>
+      <c r="R322" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S322" s="1" t="n">
         <v>1</v>
       </c>
@@ -14321,6 +15365,9 @@
         <f aca="false">SUM(F323:O323)</f>
         <v>0</v>
       </c>
+      <c r="R323" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S323" s="1" t="n">
         <v>2</v>
       </c>
@@ -14339,6 +15386,9 @@
         <f aca="false">SUM(F324:O324)</f>
         <v>0</v>
       </c>
+      <c r="R324" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S324" s="1" t="n">
         <v>1</v>
       </c>
@@ -14363,6 +15413,9 @@
         <f aca="false">SUM(F325:O325)</f>
         <v>0</v>
       </c>
+      <c r="R325" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S325" s="1" t="n">
         <v>2</v>
       </c>
@@ -14381,6 +15434,9 @@
         <f aca="false">SUM(F326:O326)</f>
         <v>0</v>
       </c>
+      <c r="R326" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S326" s="1" t="n">
         <v>1</v>
       </c>
@@ -14405,6 +15461,9 @@
         <f aca="false">SUM(F327:O327)</f>
         <v>0</v>
       </c>
+      <c r="R327" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S327" s="1" t="n">
         <v>2</v>
       </c>
@@ -14423,6 +15482,9 @@
         <f aca="false">SUM(F328:O328)</f>
         <v>0</v>
       </c>
+      <c r="R328" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S328" s="1" t="n">
         <v>1</v>
       </c>
@@ -14447,6 +15509,9 @@
         <f aca="false">SUM(F329:O329)</f>
         <v>0</v>
       </c>
+      <c r="R329" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S329" s="1" t="n">
         <v>2</v>
       </c>
@@ -14465,6 +15530,9 @@
         <f aca="false">SUM(F330:O330)</f>
         <v>0</v>
       </c>
+      <c r="R330" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S330" s="1" t="n">
         <v>1</v>
       </c>
@@ -14489,6 +15557,9 @@
         <f aca="false">SUM(F331:O331)</f>
         <v>0</v>
       </c>
+      <c r="R331" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S331" s="1" t="n">
         <v>2</v>
       </c>
@@ -14507,6 +15578,9 @@
         <f aca="false">SUM(F332:O332)</f>
         <v>0</v>
       </c>
+      <c r="R332" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S332" s="1" t="n">
         <v>1</v>
       </c>
@@ -14531,6 +15605,9 @@
         <f aca="false">SUM(F333:O333)</f>
         <v>0</v>
       </c>
+      <c r="R333" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S333" s="1" t="n">
         <v>2</v>
       </c>
@@ -14549,6 +15626,9 @@
         <f aca="false">SUM(F334:O334)</f>
         <v>0</v>
       </c>
+      <c r="R334" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S334" s="1" t="n">
         <v>1</v>
       </c>
@@ -14573,6 +15653,9 @@
         <f aca="false">SUM(F335:O335)</f>
         <v>0</v>
       </c>
+      <c r="R335" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S335" s="1" t="n">
         <v>2</v>
       </c>
@@ -14591,6 +15674,9 @@
         <f aca="false">SUM(F336:O336)</f>
         <v>0</v>
       </c>
+      <c r="R336" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S336" s="1" t="n">
         <v>1</v>
       </c>
@@ -14615,6 +15701,9 @@
         <f aca="false">SUM(F337:O337)</f>
         <v>0</v>
       </c>
+      <c r="R337" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S337" s="1" t="n">
         <v>2</v>
       </c>
@@ -14633,6 +15722,9 @@
         <f aca="false">SUM(F338:O338)</f>
         <v>0</v>
       </c>
+      <c r="R338" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S338" s="1" t="n">
         <v>1</v>
       </c>
@@ -14657,6 +15749,9 @@
         <f aca="false">SUM(F339:O339)</f>
         <v>0</v>
       </c>
+      <c r="R339" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S339" s="1" t="n">
         <v>2</v>
       </c>
@@ -14675,6 +15770,9 @@
         <f aca="false">SUM(F340:O340)</f>
         <v>0</v>
       </c>
+      <c r="R340" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S340" s="1" t="n">
         <v>1</v>
       </c>
@@ -14699,6 +15797,9 @@
         <f aca="false">SUM(F341:O341)</f>
         <v>0</v>
       </c>
+      <c r="R341" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S341" s="1" t="n">
         <v>2</v>
       </c>
@@ -14717,6 +15818,9 @@
         <f aca="false">SUM(F342:O342)</f>
         <v>0</v>
       </c>
+      <c r="R342" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S342" s="1" t="n">
         <v>1</v>
       </c>
@@ -14741,6 +15845,9 @@
         <f aca="false">SUM(F343:O343)</f>
         <v>0</v>
       </c>
+      <c r="R343" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S343" s="1" t="n">
         <v>2</v>
       </c>
@@ -14759,6 +15866,9 @@
         <f aca="false">SUM(F344:O344)</f>
         <v>0</v>
       </c>
+      <c r="R344" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S344" s="1" t="n">
         <v>1</v>
       </c>
@@ -14783,6 +15893,9 @@
         <f aca="false">SUM(F345:O345)</f>
         <v>0</v>
       </c>
+      <c r="R345" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S345" s="1" t="n">
         <v>2</v>
       </c>
@@ -14801,6 +15914,9 @@
         <f aca="false">SUM(F346:O346)</f>
         <v>0</v>
       </c>
+      <c r="R346" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S346" s="1" t="n">
         <v>1</v>
       </c>
@@ -14825,6 +15941,9 @@
         <f aca="false">SUM(F347:O347)</f>
         <v>0</v>
       </c>
+      <c r="R347" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S347" s="1" t="n">
         <v>2</v>
       </c>
@@ -14843,6 +15962,9 @@
         <f aca="false">SUM(F348:O348)</f>
         <v>0</v>
       </c>
+      <c r="R348" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S348" s="1" t="n">
         <v>1</v>
       </c>
@@ -14867,6 +15989,9 @@
         <f aca="false">SUM(F349:O349)</f>
         <v>0</v>
       </c>
+      <c r="R349" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S349" s="1" t="n">
         <v>2</v>
       </c>
@@ -14885,6 +16010,9 @@
         <f aca="false">SUM(F350:O350)</f>
         <v>0</v>
       </c>
+      <c r="R350" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S350" s="1" t="n">
         <v>1</v>
       </c>
@@ -14909,6 +16037,9 @@
         <f aca="false">SUM(F351:O351)</f>
         <v>0</v>
       </c>
+      <c r="R351" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S351" s="1" t="n">
         <v>2</v>
       </c>
@@ -14927,6 +16058,9 @@
         <f aca="false">SUM(F352:O352)</f>
         <v>0</v>
       </c>
+      <c r="R352" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S352" s="1" t="n">
         <v>1</v>
       </c>
@@ -14951,6 +16085,9 @@
         <f aca="false">SUM(F353:O353)</f>
         <v>0</v>
       </c>
+      <c r="R353" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S353" s="1" t="n">
         <v>2</v>
       </c>
@@ -14969,6 +16106,9 @@
         <f aca="false">SUM(F354:O354)</f>
         <v>0</v>
       </c>
+      <c r="R354" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S354" s="1" t="n">
         <v>1</v>
       </c>
@@ -14993,6 +16133,9 @@
         <f aca="false">SUM(F355:O355)</f>
         <v>0</v>
       </c>
+      <c r="R355" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S355" s="1" t="n">
         <v>2</v>
       </c>
@@ -15008,6 +16151,9 @@
       <c r="Q356" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="R356" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S356" s="1" t="n">
         <v>1</v>
       </c>
@@ -15032,6 +16178,9 @@
         <f aca="false">SUM(F357:O357)</f>
         <v>0</v>
       </c>
+      <c r="R357" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S357" s="1" t="n">
         <v>2</v>
       </c>
@@ -15050,6 +16199,9 @@
         <f aca="false">SUM(F358:O358)</f>
         <v>0</v>
       </c>
+      <c r="R358" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S358" s="1" t="n">
         <v>1</v>
       </c>
@@ -15074,6 +16226,9 @@
         <f aca="false">SUM(F359:O359)</f>
         <v>0</v>
       </c>
+      <c r="R359" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S359" s="1" t="n">
         <v>2</v>
       </c>
@@ -15092,6 +16247,9 @@
         <f aca="false">SUM(F360:O360)</f>
         <v>0</v>
       </c>
+      <c r="R360" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S360" s="1" t="n">
         <v>1</v>
       </c>
@@ -15116,6 +16274,9 @@
         <f aca="false">SUM(F361:O361)</f>
         <v>0</v>
       </c>
+      <c r="R361" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S361" s="1" t="n">
         <v>2</v>
       </c>
@@ -15134,6 +16295,9 @@
         <f aca="false">SUM(F362:O362)</f>
         <v>0</v>
       </c>
+      <c r="R362" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S362" s="1" t="n">
         <v>1</v>
       </c>
@@ -15158,6 +16322,9 @@
         <f aca="false">SUM(F363:O363)</f>
         <v>0</v>
       </c>
+      <c r="R363" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S363" s="1" t="n">
         <v>2</v>
       </c>
@@ -15176,6 +16343,9 @@
         <f aca="false">SUM(F364:O364)</f>
         <v>0</v>
       </c>
+      <c r="R364" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S364" s="1" t="n">
         <v>1</v>
       </c>
@@ -15200,6 +16370,9 @@
         <f aca="false">SUM(F365:O365)</f>
         <v>0</v>
       </c>
+      <c r="R365" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S365" s="1" t="n">
         <v>2</v>
       </c>
@@ -15218,6 +16391,9 @@
         <f aca="false">SUM(F366:O366)</f>
         <v>0</v>
       </c>
+      <c r="R366" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S366" s="1" t="n">
         <v>1</v>
       </c>
@@ -15242,6 +16418,9 @@
         <f aca="false">SUM(F367:O367)</f>
         <v>0</v>
       </c>
+      <c r="R367" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S367" s="1" t="n">
         <v>2</v>
       </c>
@@ -15260,6 +16439,9 @@
         <f aca="false">SUM(F368:O368)</f>
         <v>0</v>
       </c>
+      <c r="R368" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S368" s="1" t="n">
         <v>1</v>
       </c>
@@ -15284,6 +16466,9 @@
         <f aca="false">SUM(F369:O369)</f>
         <v>0</v>
       </c>
+      <c r="R369" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S369" s="1" t="n">
         <v>2</v>
       </c>
@@ -15302,6 +16487,9 @@
         <f aca="false">SUM(F370:O370)</f>
         <v>0</v>
       </c>
+      <c r="R370" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S370" s="1" t="n">
         <v>1</v>
       </c>
@@ -15326,6 +16514,9 @@
         <f aca="false">SUM(F371:O371)</f>
         <v>0</v>
       </c>
+      <c r="R371" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S371" s="1" t="n">
         <v>2</v>
       </c>
@@ -15344,6 +16535,9 @@
         <f aca="false">SUM(F372:O372)</f>
         <v>0</v>
       </c>
+      <c r="R372" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S372" s="1" t="n">
         <v>1</v>
       </c>
@@ -15368,6 +16562,9 @@
         <f aca="false">SUM(F373:O373)</f>
         <v>0</v>
       </c>
+      <c r="R373" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S373" s="1" t="n">
         <v>2</v>
       </c>
@@ -15386,6 +16583,9 @@
         <f aca="false">SUM(F374:O374)</f>
         <v>0</v>
       </c>
+      <c r="R374" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S374" s="1" t="n">
         <v>1</v>
       </c>
@@ -15410,6 +16610,9 @@
         <f aca="false">SUM(F375:O375)</f>
         <v>0</v>
       </c>
+      <c r="R375" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S375" s="1" t="n">
         <v>2</v>
       </c>
@@ -15428,6 +16631,9 @@
         <f aca="false">SUM(F376:O376)</f>
         <v>0</v>
       </c>
+      <c r="R376" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S376" s="1" t="n">
         <v>1</v>
       </c>
@@ -15452,6 +16658,9 @@
         <f aca="false">SUM(F377:O377)</f>
         <v>0</v>
       </c>
+      <c r="R377" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S377" s="1" t="n">
         <v>2</v>
       </c>
@@ -15467,6 +16676,9 @@
       <c r="Q378" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="R378" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S378" s="1" t="n">
         <v>1</v>
       </c>
@@ -15491,6 +16703,9 @@
         <f aca="false">SUM(F379:O379)</f>
         <v>0</v>
       </c>
+      <c r="R379" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S379" s="1" t="n">
         <v>2</v>
       </c>
@@ -15509,6 +16724,9 @@
         <f aca="false">SUM(F380:O380)</f>
         <v>0</v>
       </c>
+      <c r="R380" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S380" s="1" t="n">
         <v>1</v>
       </c>
@@ -15533,6 +16751,9 @@
         <f aca="false">SUM(F381:O381)</f>
         <v>0</v>
       </c>
+      <c r="R381" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S381" s="1" t="n">
         <v>2</v>
       </c>
@@ -15551,6 +16772,9 @@
         <f aca="false">SUM(F382:O382)</f>
         <v>0</v>
       </c>
+      <c r="R382" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S382" s="1" t="n">
         <v>1</v>
       </c>
@@ -15575,6 +16799,9 @@
         <f aca="false">SUM(F383:O383)</f>
         <v>0</v>
       </c>
+      <c r="R383" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S383" s="1" t="n">
         <v>2</v>
       </c>
@@ -15593,6 +16820,9 @@
         <f aca="false">SUM(F384:O384)</f>
         <v>0</v>
       </c>
+      <c r="R384" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S384" s="1" t="n">
         <v>1</v>
       </c>
@@ -15617,6 +16847,9 @@
         <f aca="false">SUM(F385:O385)</f>
         <v>0</v>
       </c>
+      <c r="R385" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S385" s="1" t="n">
         <v>2</v>
       </c>
@@ -15632,6 +16865,9 @@
       <c r="Q386" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="R386" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S386" s="1" t="n">
         <v>1</v>
       </c>
@@ -15656,6 +16892,9 @@
         <f aca="false">SUM(F387:O387)</f>
         <v>0</v>
       </c>
+      <c r="R387" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S387" s="1" t="n">
         <v>2</v>
       </c>
@@ -15674,6 +16913,9 @@
         <f aca="false">SUM(F388:O388)</f>
         <v>0</v>
       </c>
+      <c r="R388" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S388" s="1" t="n">
         <v>1</v>
       </c>
@@ -15698,6 +16940,9 @@
         <f aca="false">SUM(F389:O389)</f>
         <v>0</v>
       </c>
+      <c r="R389" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S389" s="1" t="n">
         <v>2</v>
       </c>
@@ -15716,6 +16961,9 @@
         <f aca="false">SUM(F390:O390)</f>
         <v>0</v>
       </c>
+      <c r="R390" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S390" s="1" t="n">
         <v>1</v>
       </c>
@@ -15740,6 +16988,9 @@
         <f aca="false">SUM(F391:O391)</f>
         <v>0</v>
       </c>
+      <c r="R391" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S391" s="1" t="n">
         <v>2</v>
       </c>
@@ -15755,6 +17006,9 @@
       <c r="Q392" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="R392" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S392" s="1" t="n">
         <v>1</v>
       </c>
@@ -15779,6 +17033,9 @@
         <f aca="false">SUM(F393:O393)</f>
         <v>0</v>
       </c>
+      <c r="R393" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S393" s="1" t="n">
         <v>2</v>
       </c>
@@ -15797,6 +17054,9 @@
         <f aca="false">SUM(F394:O394)</f>
         <v>0</v>
       </c>
+      <c r="R394" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S394" s="1" t="n">
         <v>1</v>
       </c>
@@ -15821,6 +17081,9 @@
         <f aca="false">SUM(F395:O395)</f>
         <v>0</v>
       </c>
+      <c r="R395" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S395" s="1" t="n">
         <v>2</v>
       </c>
@@ -15839,6 +17102,9 @@
         <f aca="false">SUM(F396:O396)</f>
         <v>0</v>
       </c>
+      <c r="R396" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S396" s="1" t="n">
         <v>1</v>
       </c>
@@ -15863,6 +17129,9 @@
         <f aca="false">SUM(F397:O397)</f>
         <v>0</v>
       </c>
+      <c r="R397" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S397" s="1" t="n">
         <v>2</v>
       </c>
@@ -15881,6 +17150,9 @@
         <f aca="false">SUM(F398:O398)</f>
         <v>0</v>
       </c>
+      <c r="R398" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S398" s="1" t="n">
         <v>1</v>
       </c>
@@ -15905,6 +17177,9 @@
         <f aca="false">SUM(F399:O399)</f>
         <v>0</v>
       </c>
+      <c r="R399" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S399" s="1" t="n">
         <v>2</v>
       </c>
@@ -15923,6 +17198,9 @@
         <f aca="false">SUM(F400:O400)</f>
         <v>0</v>
       </c>
+      <c r="R400" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S400" s="1" t="n">
         <v>1</v>
       </c>
@@ -15947,6 +17225,9 @@
         <f aca="false">SUM(F401:O401)</f>
         <v>0</v>
       </c>
+      <c r="R401" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S401" s="1" t="n">
         <v>2</v>
       </c>
@@ -15965,6 +17246,9 @@
         <f aca="false">SUM(F402:O402)</f>
         <v>0</v>
       </c>
+      <c r="R402" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S402" s="1" t="n">
         <v>1</v>
       </c>
@@ -15989,6 +17273,9 @@
         <f aca="false">SUM(F403:O403)</f>
         <v>0</v>
       </c>
+      <c r="R403" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S403" s="1" t="n">
         <v>2</v>
       </c>
@@ -16007,6 +17294,9 @@
         <f aca="false">SUM(F404:O404)</f>
         <v>0</v>
       </c>
+      <c r="R404" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S404" s="1" t="n">
         <v>1</v>
       </c>
@@ -16031,6 +17321,9 @@
         <f aca="false">SUM(F405:O405)</f>
         <v>0</v>
       </c>
+      <c r="R405" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S405" s="1" t="n">
         <v>2</v>
       </c>
@@ -16049,6 +17342,9 @@
         <f aca="false">SUM(F406:O406)</f>
         <v>0</v>
       </c>
+      <c r="R406" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S406" s="1" t="n">
         <v>1</v>
       </c>
@@ -16073,6 +17369,9 @@
         <f aca="false">SUM(F407:O407)</f>
         <v>0</v>
       </c>
+      <c r="R407" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S407" s="1" t="n">
         <v>2</v>
       </c>
@@ -16091,6 +17390,9 @@
         <f aca="false">SUM(F408:O408)</f>
         <v>0</v>
       </c>
+      <c r="R408" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S408" s="1" t="n">
         <v>1</v>
       </c>
@@ -16115,6 +17417,9 @@
         <f aca="false">SUM(F409:O409)</f>
         <v>0</v>
       </c>
+      <c r="R409" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S409" s="1" t="n">
         <v>2</v>
       </c>
@@ -16133,6 +17438,9 @@
         <f aca="false">SUM(F410:O410)</f>
         <v>0</v>
       </c>
+      <c r="R410" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S410" s="1" t="n">
         <v>1</v>
       </c>
@@ -16157,6 +17465,9 @@
         <f aca="false">SUM(F411:O411)</f>
         <v>0</v>
       </c>
+      <c r="R411" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S411" s="1" t="n">
         <v>2</v>
       </c>
@@ -16175,6 +17486,9 @@
         <f aca="false">SUM(F412:O412)</f>
         <v>0</v>
       </c>
+      <c r="R412" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S412" s="1" t="n">
         <v>1</v>
       </c>
@@ -16199,6 +17513,9 @@
         <f aca="false">SUM(F413:O413)</f>
         <v>0</v>
       </c>
+      <c r="R413" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S413" s="1" t="n">
         <v>2</v>
       </c>
@@ -16214,6 +17531,9 @@
       <c r="Q414" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="R414" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S414" s="1" t="n">
         <v>1</v>
       </c>
@@ -16238,6 +17558,9 @@
         <f aca="false">SUM(F415:O415)</f>
         <v>0</v>
       </c>
+      <c r="R415" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S415" s="1" t="n">
         <v>2</v>
       </c>
@@ -16256,6 +17579,9 @@
         <f aca="false">SUM(F416:O416)</f>
         <v>0</v>
       </c>
+      <c r="R416" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S416" s="1" t="n">
         <v>1</v>
       </c>
@@ -16280,6 +17606,9 @@
         <f aca="false">SUM(F417:O417)</f>
         <v>0</v>
       </c>
+      <c r="R417" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S417" s="1" t="n">
         <v>2</v>
       </c>
@@ -16298,6 +17627,9 @@
         <f aca="false">SUM(F418:O418)</f>
         <v>0</v>
       </c>
+      <c r="R418" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S418" s="1" t="n">
         <v>1</v>
       </c>
@@ -16322,6 +17654,9 @@
         <f aca="false">SUM(F419:O419)</f>
         <v>0</v>
       </c>
+      <c r="R419" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="S419" s="1" t="n">
         <v>2</v>
       </c>
@@ -16336,6 +17671,9 @@
       </c>
       <c r="Q420" s="2" t="s">
         <v>28</v>
+      </c>
+      <c r="R420" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="S420" s="1" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
day 6 data committed on day 7 morning
</commit_message>
<xml_diff>
--- a/Data acquisition/wing_leakage_data_samples_filt.xlsx
+++ b/Data acquisition/wing_leakage_data_samples_filt.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="35">
   <si>
     <t xml:space="preserve">sample_number</t>
   </si>
@@ -113,6 +113,18 @@
   </si>
   <si>
     <t xml:space="preserve">needle change 2. value seems to be higher after needle change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changed 1 needle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum seemed high. Couldnt figure out the issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verified for zero leakage before this observation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">had a leakage. Solved with 2 step method</t>
   </si>
 </sst>
 </file>
@@ -298,10 +310,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S2001"/>
+  <dimension ref="A1:S2007"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A306" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F320" activeCellId="0" sqref="F320"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A419" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O426" activeCellId="0" sqref="O426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15276,7 +15288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="320" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="4" t="n">
         <v>318</v>
       </c>
@@ -15286,9 +15298,42 @@
       <c r="C320" s="1" t="n">
         <v>1850</v>
       </c>
+      <c r="F320" s="1" t="n">
+        <v>0.0508</v>
+      </c>
+      <c r="G320" s="1" t="n">
+        <v>0.0552</v>
+      </c>
+      <c r="H320" s="1" t="n">
+        <v>0.0293</v>
+      </c>
+      <c r="I320" s="1" t="n">
+        <v>0.0132</v>
+      </c>
+      <c r="J320" s="1" t="n">
+        <v>0.0234</v>
+      </c>
+      <c r="K320" s="1" t="n">
+        <v>0.0702</v>
+      </c>
+      <c r="L320" s="1" t="n">
+        <v>0.0806</v>
+      </c>
+      <c r="M320" s="1" t="n">
+        <v>0.0327</v>
+      </c>
+      <c r="N320" s="1" t="n">
+        <v>0.0135</v>
+      </c>
+      <c r="O320" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P320" s="1" t="n">
         <f aca="false">SUM(F320:O320)</f>
-        <v>0</v>
+        <v>0.3689</v>
+      </c>
+      <c r="Q320" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="R320" s="1" t="n">
         <v>6</v>
@@ -15313,9 +15358,42 @@
       <c r="E321" s="1" t="n">
         <v>2850</v>
       </c>
+      <c r="F321" s="1" t="n">
+        <v>0.1078</v>
+      </c>
+      <c r="G321" s="1" t="n">
+        <v>0.1261</v>
+      </c>
+      <c r="H321" s="1" t="n">
+        <v>0.0629</v>
+      </c>
+      <c r="I321" s="1" t="n">
+        <v>0.0268</v>
+      </c>
+      <c r="J321" s="1" t="n">
+        <v>0.0286</v>
+      </c>
+      <c r="K321" s="1" t="n">
+        <v>0.1246</v>
+      </c>
+      <c r="L321" s="1" t="n">
+        <v>0.1377</v>
+      </c>
+      <c r="M321" s="1" t="n">
+        <v>0.0635</v>
+      </c>
+      <c r="N321" s="1" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="O321" s="1" t="n">
+        <v>0.0118</v>
+      </c>
       <c r="P321" s="1" t="n">
         <f aca="false">SUM(F321:O321)</f>
-        <v>0</v>
+        <v>0.7158</v>
+      </c>
+      <c r="Q321" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="R321" s="1" t="n">
         <v>6</v>
@@ -15334,9 +15412,39 @@
       <c r="C322" s="1" t="n">
         <v>2850</v>
       </c>
+      <c r="F322" s="1" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G322" s="1" t="n">
+        <v>0.0789</v>
+      </c>
+      <c r="H322" s="1" t="n">
+        <v>0.0387</v>
+      </c>
+      <c r="I322" s="1" t="n">
+        <v>0.0181</v>
+      </c>
+      <c r="J322" s="1" t="n">
+        <v>0.0272</v>
+      </c>
+      <c r="K322" s="1" t="n">
+        <v>0.0585</v>
+      </c>
+      <c r="L322" s="1" t="n">
+        <v>0.0628</v>
+      </c>
+      <c r="M322" s="1" t="n">
+        <v>0.0346</v>
+      </c>
+      <c r="N322" s="1" t="n">
+        <v>0.0168</v>
+      </c>
+      <c r="O322" s="1" t="n">
+        <v>0.0093</v>
+      </c>
       <c r="P322" s="1" t="n">
         <f aca="false">SUM(F322:O322)</f>
-        <v>0</v>
+        <v>0.4074</v>
       </c>
       <c r="R322" s="1" t="n">
         <v>6</v>
@@ -15361,9 +15469,39 @@
       <c r="E323" s="1" t="n">
         <v>4350</v>
       </c>
+      <c r="F323" s="1" t="n">
+        <v>0.0673</v>
+      </c>
+      <c r="G323" s="1" t="n">
+        <v>0.0943</v>
+      </c>
+      <c r="H323" s="1" t="n">
+        <v>0.0945</v>
+      </c>
+      <c r="I323" s="1" t="n">
+        <v>0.1163</v>
+      </c>
+      <c r="J323" s="1" t="n">
+        <v>0.0484</v>
+      </c>
+      <c r="K323" s="1" t="n">
+        <v>0.0631</v>
+      </c>
+      <c r="L323" s="1" t="n">
+        <v>0.0728</v>
+      </c>
+      <c r="M323" s="1" t="n">
+        <v>0.0578</v>
+      </c>
+      <c r="N323" s="1" t="n">
+        <v>0.0459</v>
+      </c>
+      <c r="O323" s="1" t="n">
+        <v>0.0283</v>
+      </c>
       <c r="P323" s="1" t="n">
         <f aca="false">SUM(F323:O323)</f>
-        <v>0</v>
+        <v>0.6887</v>
       </c>
       <c r="R323" s="1" t="n">
         <v>6</v>
@@ -15382,9 +15520,39 @@
       <c r="C324" s="1" t="n">
         <v>4350</v>
       </c>
+      <c r="F324" s="1" t="n">
+        <v>0.0097</v>
+      </c>
+      <c r="G324" s="1" t="n">
+        <v>0.0234</v>
+      </c>
+      <c r="H324" s="1" t="n">
+        <v>0.0618</v>
+      </c>
+      <c r="I324" s="1" t="n">
+        <v>0.104</v>
+      </c>
+      <c r="J324" s="1" t="n">
+        <v>0.0454</v>
+      </c>
+      <c r="K324" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L324" s="1" t="n">
+        <v>0.0158</v>
+      </c>
+      <c r="M324" s="1" t="n">
+        <v>0.0274</v>
+      </c>
+      <c r="N324" s="1" t="n">
+        <v>0.0346</v>
+      </c>
+      <c r="O324" s="1" t="n">
+        <v>0.0239</v>
+      </c>
       <c r="P324" s="1" t="n">
         <f aca="false">SUM(F324:O324)</f>
-        <v>0</v>
+        <v>0.346</v>
       </c>
       <c r="R324" s="1" t="n">
         <v>6</v>
@@ -15409,9 +15577,39 @@
       <c r="E325" s="1" t="n">
         <v>3600</v>
       </c>
+      <c r="F325" s="1" t="n">
+        <v>0.0703</v>
+      </c>
+      <c r="G325" s="1" t="n">
+        <v>0.1332</v>
+      </c>
+      <c r="H325" s="1" t="n">
+        <v>0.106</v>
+      </c>
+      <c r="I325" s="1" t="n">
+        <v>0.118</v>
+      </c>
+      <c r="J325" s="1" t="n">
+        <v>0.0505</v>
+      </c>
+      <c r="K325" s="1" t="n">
+        <v>0.0531</v>
+      </c>
+      <c r="L325" s="1" t="n">
+        <v>0.0639</v>
+      </c>
+      <c r="M325" s="1" t="n">
+        <v>0.0591</v>
+      </c>
+      <c r="N325" s="1" t="n">
+        <v>0.0474</v>
+      </c>
+      <c r="O325" s="1" t="n">
+        <v>0.0295</v>
+      </c>
       <c r="P325" s="1" t="n">
         <f aca="false">SUM(F325:O325)</f>
-        <v>0</v>
+        <v>0.731</v>
       </c>
       <c r="R325" s="1" t="n">
         <v>6</v>
@@ -15430,9 +15628,39 @@
       <c r="C326" s="1" t="n">
         <v>3600</v>
       </c>
+      <c r="F326" s="1" t="n">
+        <v>0.0645</v>
+      </c>
+      <c r="G326" s="1" t="n">
+        <v>0.1168</v>
+      </c>
+      <c r="H326" s="1" t="n">
+        <v>0.0499</v>
+      </c>
+      <c r="I326" s="1" t="n">
+        <v>0.0198</v>
+      </c>
+      <c r="J326" s="1" t="n">
+        <v>0.0292</v>
+      </c>
+      <c r="K326" s="1" t="n">
+        <v>0.0475</v>
+      </c>
+      <c r="L326" s="1" t="n">
+        <v>0.0531</v>
+      </c>
+      <c r="M326" s="1" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="N326" s="1" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="O326" s="1" t="n">
+        <v>0.01</v>
+      </c>
       <c r="P326" s="1" t="n">
         <f aca="false">SUM(F326:O326)</f>
-        <v>0</v>
+        <v>0.4438</v>
       </c>
       <c r="R326" s="1" t="n">
         <v>6</v>
@@ -15457,9 +15685,39 @@
       <c r="E327" s="1" t="n">
         <v>2350</v>
       </c>
+      <c r="F327" s="1" t="n">
+        <v>0.0932</v>
+      </c>
+      <c r="G327" s="1" t="n">
+        <v>0.1677</v>
+      </c>
+      <c r="H327" s="1" t="n">
+        <v>0.0881</v>
+      </c>
+      <c r="I327" s="1" t="n">
+        <v>0.0348</v>
+      </c>
+      <c r="J327" s="1" t="n">
+        <v>0.0329</v>
+      </c>
+      <c r="K327" s="1" t="n">
+        <v>0.0784</v>
+      </c>
+      <c r="L327" s="1" t="n">
+        <v>0.1073</v>
+      </c>
+      <c r="M327" s="1" t="n">
+        <v>0.0785</v>
+      </c>
+      <c r="N327" s="1" t="n">
+        <v>0.0333</v>
+      </c>
+      <c r="O327" s="1" t="n">
+        <v>0.0149</v>
+      </c>
       <c r="P327" s="1" t="n">
         <f aca="false">SUM(F327:O327)</f>
-        <v>0</v>
+        <v>0.7291</v>
       </c>
       <c r="R327" s="1" t="n">
         <v>6</v>
@@ -15478,9 +15736,39 @@
       <c r="C328" s="1" t="n">
         <v>2350</v>
       </c>
+      <c r="F328" s="1" t="n">
+        <v>0.0354</v>
+      </c>
+      <c r="G328" s="1" t="n">
+        <v>0.0607</v>
+      </c>
+      <c r="H328" s="1" t="n">
+        <v>0.0451</v>
+      </c>
+      <c r="I328" s="1" t="n">
+        <v>0.0222</v>
+      </c>
+      <c r="J328" s="1" t="n">
+        <v>0.0301</v>
+      </c>
+      <c r="K328" s="1" t="n">
+        <v>0.0361</v>
+      </c>
+      <c r="L328" s="1" t="n">
+        <v>0.0608</v>
+      </c>
+      <c r="M328" s="1" t="n">
+        <v>0.0482</v>
+      </c>
+      <c r="N328" s="1" t="n">
+        <v>0.0216</v>
+      </c>
+      <c r="O328" s="1" t="n">
+        <v>0.0114</v>
+      </c>
       <c r="P328" s="1" t="n">
         <f aca="false">SUM(F328:O328)</f>
-        <v>0</v>
+        <v>0.3716</v>
       </c>
       <c r="R328" s="1" t="n">
         <v>6</v>
@@ -15489,7 +15777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="329" customFormat="false" ht="24.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="1" t="n">
         <v>327</v>
       </c>
@@ -15505,9 +15793,42 @@
       <c r="E329" s="1" t="n">
         <v>4600</v>
       </c>
+      <c r="F329" s="1" t="n">
+        <v>0.0462</v>
+      </c>
+      <c r="G329" s="1" t="n">
+        <v>0.0996</v>
+      </c>
+      <c r="H329" s="1" t="n">
+        <v>0.182</v>
+      </c>
+      <c r="I329" s="1" t="n">
+        <v>0.0455</v>
+      </c>
+      <c r="J329" s="1" t="n">
+        <v>0.0356</v>
+      </c>
+      <c r="K329" s="1" t="n">
+        <v>0.0446</v>
+      </c>
+      <c r="L329" s="1" t="n">
+        <v>0.0762</v>
+      </c>
+      <c r="M329" s="1" t="n">
+        <v>0.0699</v>
+      </c>
+      <c r="N329" s="1" t="n">
+        <v>0.0357</v>
+      </c>
+      <c r="O329" s="1" t="n">
+        <v>0.0175</v>
+      </c>
       <c r="P329" s="1" t="n">
         <f aca="false">SUM(F329:O329)</f>
-        <v>0</v>
+        <v>0.6528</v>
+      </c>
+      <c r="Q329" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="R329" s="1" t="n">
         <v>6</v>
@@ -15526,9 +15847,39 @@
       <c r="C330" s="1" t="n">
         <v>4600</v>
       </c>
+      <c r="F330" s="1" t="n">
+        <v>0.0207</v>
+      </c>
+      <c r="G330" s="1" t="n">
+        <v>0.0516</v>
+      </c>
+      <c r="H330" s="1" t="n">
+        <v>0.1474</v>
+      </c>
+      <c r="I330" s="1" t="n">
+        <v>0.0327</v>
+      </c>
+      <c r="J330" s="1" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="K330" s="1" t="n">
+        <v>0.0173</v>
+      </c>
+      <c r="L330" s="1" t="n">
+        <v>0.0248</v>
+      </c>
+      <c r="M330" s="1" t="n">
+        <v>0.0284</v>
+      </c>
+      <c r="N330" s="1" t="n">
+        <v>0.0218</v>
+      </c>
+      <c r="O330" s="1" t="n">
+        <v>0.0133</v>
+      </c>
       <c r="P330" s="1" t="n">
         <f aca="false">SUM(F330:O330)</f>
-        <v>0</v>
+        <v>0.39</v>
       </c>
       <c r="R330" s="1" t="n">
         <v>6</v>
@@ -15537,7 +15888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="331" customFormat="false" ht="24.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="1" t="n">
         <v>329</v>
       </c>
@@ -15553,9 +15904,42 @@
       <c r="E331" s="1" t="n">
         <v>2350</v>
       </c>
+      <c r="F331" s="1" t="n">
+        <v>0.0381</v>
+      </c>
+      <c r="G331" s="1" t="n">
+        <v>0.0926</v>
+      </c>
+      <c r="H331" s="1" t="n">
+        <v>0.1889</v>
+      </c>
+      <c r="I331" s="1" t="n">
+        <v>0.0503</v>
+      </c>
+      <c r="J331" s="1" t="n">
+        <v>0.0353</v>
+      </c>
+      <c r="K331" s="1" t="n">
+        <v>0.0347</v>
+      </c>
+      <c r="L331" s="1" t="n">
+        <v>0.0667</v>
+      </c>
+      <c r="M331" s="1" t="n">
+        <v>0.0788</v>
+      </c>
+      <c r="N331" s="1" t="n">
+        <v>0.0406</v>
+      </c>
+      <c r="O331" s="1" t="n">
+        <v>0.0189</v>
+      </c>
       <c r="P331" s="1" t="n">
         <f aca="false">SUM(F331:O331)</f>
-        <v>0</v>
+        <v>0.6449</v>
+      </c>
+      <c r="Q331" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="R331" s="1" t="n">
         <v>6</v>
@@ -15574,9 +15958,39 @@
       <c r="C332" s="1" t="n">
         <v>2350</v>
       </c>
+      <c r="F332" s="1" t="n">
+        <v>0.0277</v>
+      </c>
+      <c r="G332" s="1" t="n">
+        <v>0.0533</v>
+      </c>
+      <c r="H332" s="1" t="n">
+        <v>0.0492</v>
+      </c>
+      <c r="I332" s="1" t="n">
+        <v>0.0257</v>
+      </c>
+      <c r="J332" s="1" t="n">
+        <v>0.0303</v>
+      </c>
+      <c r="K332" s="1" t="n">
+        <v>0.0271</v>
+      </c>
+      <c r="L332" s="1" t="n">
+        <v>0.0519</v>
+      </c>
+      <c r="M332" s="1" t="n">
+        <v>0.0572</v>
+      </c>
+      <c r="N332" s="1" t="n">
+        <v>0.0261</v>
+      </c>
+      <c r="O332" s="1" t="n">
+        <v>0.0124</v>
+      </c>
       <c r="P332" s="1" t="n">
         <f aca="false">SUM(F332:O332)</f>
-        <v>0</v>
+        <v>0.3609</v>
       </c>
       <c r="R332" s="1" t="n">
         <v>6</v>
@@ -15601,9 +16015,39 @@
       <c r="E333" s="1" t="n">
         <v>2850</v>
       </c>
+      <c r="F333" s="1" t="n">
+        <v>0.0874</v>
+      </c>
+      <c r="G333" s="1" t="n">
+        <v>0.113</v>
+      </c>
+      <c r="H333" s="1" t="n">
+        <v>0.0736</v>
+      </c>
+      <c r="I333" s="1" t="n">
+        <v>0.0345</v>
+      </c>
+      <c r="J333" s="1" t="n">
+        <v>0.0339</v>
+      </c>
+      <c r="K333" s="1" t="n">
+        <v>0.0844</v>
+      </c>
+      <c r="L333" s="1" t="n">
+        <v>0.1014</v>
+      </c>
+      <c r="M333" s="1" t="n">
+        <v>0.0802</v>
+      </c>
+      <c r="N333" s="1" t="n">
+        <v>0.0344</v>
+      </c>
+      <c r="O333" s="1" t="n">
+        <v>0.0159</v>
+      </c>
       <c r="P333" s="1" t="n">
         <f aca="false">SUM(F333:O333)</f>
-        <v>0</v>
+        <v>0.6587</v>
       </c>
       <c r="R333" s="1" t="n">
         <v>6</v>
@@ -15622,9 +16066,39 @@
       <c r="C334" s="1" t="n">
         <v>2850</v>
       </c>
+      <c r="F334" s="1" t="n">
+        <v>0.0649</v>
+      </c>
+      <c r="G334" s="1" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="H334" s="1" t="n">
+        <v>0.0296</v>
+      </c>
+      <c r="I334" s="1" t="n">
+        <v>0.0142</v>
+      </c>
+      <c r="J334" s="1" t="n">
+        <v>0.0271</v>
+      </c>
+      <c r="K334" s="1" t="n">
+        <v>0.0607</v>
+      </c>
+      <c r="L334" s="1" t="n">
+        <v>0.0557</v>
+      </c>
+      <c r="M334" s="1" t="n">
+        <v>0.0278</v>
+      </c>
+      <c r="N334" s="1" t="n">
+        <v>0.0136</v>
+      </c>
+      <c r="O334" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P334" s="1" t="n">
         <f aca="false">SUM(F334:O334)</f>
-        <v>0</v>
+        <v>0.3616</v>
       </c>
       <c r="R334" s="1" t="n">
         <v>6</v>
@@ -15649,9 +16123,39 @@
       <c r="E335" s="1" t="n">
         <v>2350</v>
       </c>
+      <c r="F335" s="1" t="n">
+        <v>0.0653</v>
+      </c>
+      <c r="G335" s="1" t="n">
+        <v>0.0699</v>
+      </c>
+      <c r="H335" s="1" t="n">
+        <v>0.0358</v>
+      </c>
+      <c r="I335" s="1" t="n">
+        <v>0.0426</v>
+      </c>
+      <c r="J335" s="1" t="n">
+        <v>0.1133</v>
+      </c>
+      <c r="K335" s="1" t="n">
+        <v>0.0609</v>
+      </c>
+      <c r="L335" s="1" t="n">
+        <v>0.0573</v>
+      </c>
+      <c r="M335" s="1" t="n">
+        <v>0.0347</v>
+      </c>
+      <c r="N335" s="1" t="n">
+        <v>0.0437</v>
+      </c>
+      <c r="O335" s="1" t="n">
+        <v>0.1346</v>
+      </c>
       <c r="P335" s="1" t="n">
         <f aca="false">SUM(F335:O335)</f>
-        <v>0</v>
+        <v>0.6581</v>
       </c>
       <c r="R335" s="1" t="n">
         <v>6</v>
@@ -15670,9 +16174,39 @@
       <c r="C336" s="1" t="n">
         <v>2350</v>
       </c>
+      <c r="F336" s="1" t="n">
+        <v>0.0092</v>
+      </c>
+      <c r="G336" s="1" t="n">
+        <v>0.0139</v>
+      </c>
+      <c r="H336" s="1" t="n">
+        <v>0.0142</v>
+      </c>
+      <c r="I336" s="1" t="n">
+        <v>0.0358</v>
+      </c>
+      <c r="J336" s="1" t="n">
+        <v>0.1114</v>
+      </c>
+      <c r="K336" s="1" t="n">
+        <v>0.0097</v>
+      </c>
+      <c r="L336" s="1" t="n">
+        <v>0.0124</v>
+      </c>
+      <c r="M336" s="1" t="n">
+        <v>0.0146</v>
+      </c>
+      <c r="N336" s="1" t="n">
+        <v>0.0373</v>
+      </c>
+      <c r="O336" s="1" t="n">
+        <v>0.1323</v>
+      </c>
       <c r="P336" s="1" t="n">
         <f aca="false">SUM(F336:O336)</f>
-        <v>0</v>
+        <v>0.3908</v>
       </c>
       <c r="R336" s="1" t="n">
         <v>6</v>
@@ -15681,7 +16215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="337" customFormat="false" ht="24.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="1" t="n">
         <v>335</v>
       </c>
@@ -15697,9 +16231,42 @@
       <c r="E337" s="1" t="n">
         <v>100</v>
       </c>
+      <c r="F337" s="1" t="n">
+        <v>0.0129</v>
+      </c>
+      <c r="G337" s="1" t="n">
+        <v>0.0205</v>
+      </c>
+      <c r="H337" s="1" t="n">
+        <v>0.0186</v>
+      </c>
+      <c r="I337" s="1" t="n">
+        <v>0.0369</v>
+      </c>
+      <c r="J337" s="1" t="n">
+        <v>0.1116</v>
+      </c>
+      <c r="K337" s="1" t="n">
+        <v>0.0191</v>
+      </c>
+      <c r="L337" s="1" t="n">
+        <v>0.1931</v>
+      </c>
+      <c r="M337" s="1" t="n">
+        <v>0.0318</v>
+      </c>
+      <c r="N337" s="1" t="n">
+        <v>0.0394</v>
+      </c>
+      <c r="O337" s="1" t="n">
+        <v>0.1308</v>
+      </c>
       <c r="P337" s="1" t="n">
         <f aca="false">SUM(F337:O337)</f>
-        <v>0</v>
+        <v>0.6147</v>
+      </c>
+      <c r="Q337" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="R337" s="1" t="n">
         <v>6</v>
@@ -15718,9 +16285,39 @@
       <c r="C338" s="1" t="n">
         <v>100</v>
       </c>
+      <c r="F338" s="1" t="n">
+        <v>0.0166</v>
+      </c>
+      <c r="G338" s="1" t="n">
+        <v>0.0226</v>
+      </c>
+      <c r="H338" s="1" t="n">
+        <v>0.0156</v>
+      </c>
+      <c r="I338" s="1" t="n">
+        <v>0.0107</v>
+      </c>
+      <c r="J338" s="1" t="n">
+        <v>0.0273</v>
+      </c>
+      <c r="K338" s="1" t="n">
+        <v>0.0231</v>
+      </c>
+      <c r="L338" s="1" t="n">
+        <v>0.1934</v>
+      </c>
+      <c r="M338" s="1" t="n">
+        <v>0.0272</v>
+      </c>
+      <c r="N338" s="1" t="n">
+        <v>0.0115</v>
+      </c>
+      <c r="O338" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P338" s="1" t="n">
         <f aca="false">SUM(F338:O338)</f>
-        <v>0</v>
+        <v>0.348</v>
       </c>
       <c r="R338" s="1" t="n">
         <v>6</v>
@@ -15745,9 +16342,39 @@
       <c r="E339" s="1" t="n">
         <v>4100</v>
       </c>
+      <c r="F339" s="1" t="n">
+        <v>0.0212</v>
+      </c>
+      <c r="G339" s="1" t="n">
+        <v>0.0366</v>
+      </c>
+      <c r="H339" s="1" t="n">
+        <v>0.0624</v>
+      </c>
+      <c r="I339" s="1" t="n">
+        <v>0.1157</v>
+      </c>
+      <c r="J339" s="1" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="K339" s="1" t="n">
+        <v>0.0275</v>
+      </c>
+      <c r="L339" s="1" t="n">
+        <v>0.2019</v>
+      </c>
+      <c r="M339" s="1" t="n">
+        <v>0.0502</v>
+      </c>
+      <c r="N339" s="1" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="O339" s="1" t="n">
+        <v>0.0281</v>
+      </c>
       <c r="P339" s="1" t="n">
         <f aca="false">SUM(F339:O339)</f>
-        <v>0</v>
+        <v>0.6376</v>
       </c>
       <c r="R339" s="1" t="n">
         <v>6</v>
@@ -15766,9 +16393,39 @@
       <c r="C340" s="1" t="n">
         <v>4100</v>
       </c>
+      <c r="F340" s="1" t="n">
+        <v>0.0117</v>
+      </c>
+      <c r="G340" s="1" t="n">
+        <v>0.0236</v>
+      </c>
+      <c r="H340" s="1" t="n">
+        <v>0.0529</v>
+      </c>
+      <c r="I340" s="1" t="n">
+        <v>0.1116</v>
+      </c>
+      <c r="J340" s="1" t="n">
+        <v>0.0502</v>
+      </c>
+      <c r="K340" s="1" t="n">
+        <v>0.0099</v>
+      </c>
+      <c r="L340" s="1" t="n">
+        <v>0.0146</v>
+      </c>
+      <c r="M340" s="1" t="n">
+        <v>0.0282</v>
+      </c>
+      <c r="N340" s="1" t="n">
+        <v>0.0378</v>
+      </c>
+      <c r="O340" s="1" t="n">
+        <v>0.0267</v>
+      </c>
       <c r="P340" s="1" t="n">
         <f aca="false">SUM(F340:O340)</f>
-        <v>0</v>
+        <v>0.3672</v>
       </c>
       <c r="R340" s="1" t="n">
         <v>6</v>
@@ -15793,9 +16450,39 @@
       <c r="E341" s="1" t="n">
         <v>1100</v>
       </c>
+      <c r="F341" s="1" t="n">
+        <v>0.0236</v>
+      </c>
+      <c r="G341" s="1" t="n">
+        <v>0.0485</v>
+      </c>
+      <c r="H341" s="1" t="n">
+        <v>0.0816</v>
+      </c>
+      <c r="I341" s="1" t="n">
+        <v>0.1283</v>
+      </c>
+      <c r="J341" s="1" t="n">
+        <v>0.0568</v>
+      </c>
+      <c r="K341" s="1" t="n">
+        <v>0.0244</v>
+      </c>
+      <c r="L341" s="1" t="n">
+        <v>0.061</v>
+      </c>
+      <c r="M341" s="1" t="n">
+        <v>0.1199</v>
+      </c>
+      <c r="N341" s="1" t="n">
+        <v>0.0612</v>
+      </c>
+      <c r="O341" s="1" t="n">
+        <v>0.0349</v>
+      </c>
       <c r="P341" s="1" t="n">
         <f aca="false">SUM(F341:O341)</f>
-        <v>0</v>
+        <v>0.6402</v>
       </c>
       <c r="R341" s="1" t="n">
         <v>6</v>
@@ -15814,9 +16501,39 @@
       <c r="C342" s="1" t="n">
         <v>1100</v>
       </c>
+      <c r="F342" s="1" t="n">
+        <v>0.0215</v>
+      </c>
+      <c r="G342" s="1" t="n">
+        <v>0.0364</v>
+      </c>
+      <c r="H342" s="1" t="n">
+        <v>0.0352</v>
+      </c>
+      <c r="I342" s="1" t="n">
+        <v>0.0242</v>
+      </c>
+      <c r="J342" s="1" t="n">
+        <v>0.033</v>
+      </c>
+      <c r="K342" s="1" t="n">
+        <v>0.0233</v>
+      </c>
+      <c r="L342" s="1" t="n">
+        <v>0.0534</v>
+      </c>
+      <c r="M342" s="1" t="n">
+        <v>0.0976</v>
+      </c>
+      <c r="N342" s="1" t="n">
+        <v>0.0303</v>
+      </c>
+      <c r="O342" s="1" t="n">
+        <v>0.0142</v>
+      </c>
       <c r="P342" s="1" t="n">
         <f aca="false">SUM(F342:O342)</f>
-        <v>0</v>
+        <v>0.3691</v>
       </c>
       <c r="R342" s="1" t="n">
         <v>6</v>
@@ -15845,6 +16562,9 @@
         <f aca="false">SUM(F343:O343)</f>
         <v>0</v>
       </c>
+      <c r="Q343" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R343" s="1" t="n">
         <v>6</v>
       </c>
@@ -15866,6 +16586,9 @@
         <f aca="false">SUM(F344:O344)</f>
         <v>0</v>
       </c>
+      <c r="Q344" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R344" s="1" t="n">
         <v>6</v>
       </c>
@@ -15893,6 +16616,9 @@
         <f aca="false">SUM(F345:O345)</f>
         <v>0</v>
       </c>
+      <c r="Q345" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R345" s="1" t="n">
         <v>6</v>
       </c>
@@ -15910,9 +16636,39 @@
       <c r="C346" s="1" t="n">
         <v>850</v>
       </c>
+      <c r="F346" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G346" s="1" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="H346" s="1" t="n">
+        <v>0.0155</v>
+      </c>
+      <c r="I346" s="1" t="n">
+        <v>0.0341</v>
+      </c>
+      <c r="J346" s="1" t="n">
+        <v>0.0619</v>
+      </c>
+      <c r="K346" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L346" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M346" s="1" t="n">
+        <v>0.0189</v>
+      </c>
+      <c r="N346" s="1" t="n">
+        <v>0.0897</v>
+      </c>
+      <c r="O346" s="1" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P346" s="1" t="n">
         <f aca="false">SUM(F346:O346)</f>
-        <v>0</v>
+        <v>0.3321</v>
       </c>
       <c r="R346" s="1" t="n">
         <v>6</v>
@@ -15937,9 +16693,39 @@
       <c r="E347" s="1" t="n">
         <v>2100</v>
       </c>
+      <c r="F347" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G347" s="1" t="n">
+        <v>0.0125</v>
+      </c>
+      <c r="H347" s="1" t="n">
+        <v>0.0217</v>
+      </c>
+      <c r="I347" s="1" t="n">
+        <v>0.0639</v>
+      </c>
+      <c r="J347" s="1" t="n">
+        <v>0.1302</v>
+      </c>
+      <c r="K347" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L347" s="1" t="n">
+        <v>0.087</v>
+      </c>
+      <c r="M347" s="1" t="n">
+        <v>0.0268</v>
+      </c>
+      <c r="N347" s="1" t="n">
+        <v>0.1268</v>
+      </c>
+      <c r="O347" s="1" t="n">
+        <v>0.2319</v>
+      </c>
       <c r="P347" s="1" t="n">
         <f aca="false">SUM(F347:O347)</f>
-        <v>0</v>
+        <v>0.7008</v>
       </c>
       <c r="R347" s="1" t="n">
         <v>6</v>
@@ -15958,9 +16744,39 @@
       <c r="C348" s="1" t="n">
         <v>2100</v>
       </c>
+      <c r="F348" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G348" s="1" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="H348" s="1" t="n">
+        <v>0.0134</v>
+      </c>
+      <c r="I348" s="1" t="n">
+        <v>0.0364</v>
+      </c>
+      <c r="J348" s="1" t="n">
+        <v>0.0959</v>
+      </c>
+      <c r="K348" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L348" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M348" s="1" t="n">
+        <v>0.0132</v>
+      </c>
+      <c r="N348" s="1" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="O348" s="1" t="n">
+        <v>0.1388</v>
+      </c>
       <c r="P348" s="1" t="n">
         <f aca="false">SUM(F348:O348)</f>
-        <v>0</v>
+        <v>0.3517</v>
       </c>
       <c r="R348" s="1" t="n">
         <v>6</v>
@@ -15985,9 +16801,39 @@
       <c r="E349" s="1" t="n">
         <v>3600</v>
       </c>
+      <c r="F349" s="1" t="n">
+        <v>0.0438</v>
+      </c>
+      <c r="G349" s="1" t="n">
+        <v>0.0971</v>
+      </c>
+      <c r="H349" s="1" t="n">
+        <v>0.0537</v>
+      </c>
+      <c r="I349" s="1" t="n">
+        <v>0.0484</v>
+      </c>
+      <c r="J349" s="1" t="n">
+        <v>0.0991</v>
+      </c>
+      <c r="K349" s="1" t="n">
+        <v>0.0323</v>
+      </c>
+      <c r="L349" s="1" t="n">
+        <v>0.0413</v>
+      </c>
+      <c r="M349" s="1" t="n">
+        <v>0.0394</v>
+      </c>
+      <c r="N349" s="1" t="n">
+        <v>0.0535</v>
+      </c>
+      <c r="O349" s="1" t="n">
+        <v>0.1431</v>
+      </c>
       <c r="P349" s="1" t="n">
         <f aca="false">SUM(F349:O349)</f>
-        <v>0</v>
+        <v>0.6517</v>
       </c>
       <c r="R349" s="1" t="n">
         <v>6</v>
@@ -16006,9 +16852,39 @@
       <c r="C350" s="1" t="n">
         <v>3600</v>
       </c>
+      <c r="F350" s="1" t="n">
+        <v>0.0441</v>
+      </c>
+      <c r="G350" s="1" t="n">
+        <v>0.0952</v>
+      </c>
+      <c r="H350" s="1" t="n">
+        <v>0.0464</v>
+      </c>
+      <c r="I350" s="1" t="n">
+        <v>0.0179</v>
+      </c>
+      <c r="J350" s="1" t="n">
+        <v>0.0283</v>
+      </c>
+      <c r="K350" s="1" t="n">
+        <v>0.0333</v>
+      </c>
+      <c r="L350" s="1" t="n">
+        <v>0.0403</v>
+      </c>
+      <c r="M350" s="1" t="n">
+        <v>0.0309</v>
+      </c>
+      <c r="N350" s="1" t="n">
+        <v>0.0159</v>
+      </c>
+      <c r="O350" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P350" s="1" t="n">
         <f aca="false">SUM(F350:O350)</f>
-        <v>0</v>
+        <v>0.3523</v>
       </c>
       <c r="R350" s="1" t="n">
         <v>6</v>
@@ -16033,9 +16909,39 @@
       <c r="E351" s="1" t="n">
         <v>100</v>
       </c>
+      <c r="F351" s="1" t="n">
+        <v>0.0664</v>
+      </c>
+      <c r="G351" s="1" t="n">
+        <v>0.1185</v>
+      </c>
+      <c r="H351" s="1" t="n">
+        <v>0.0596</v>
+      </c>
+      <c r="I351" s="1" t="n">
+        <v>0.0226</v>
+      </c>
+      <c r="J351" s="1" t="n">
+        <v>0.0286</v>
+      </c>
+      <c r="K351" s="1" t="n">
+        <v>0.0851</v>
+      </c>
+      <c r="L351" s="1" t="n">
+        <v>0.186</v>
+      </c>
+      <c r="M351" s="1" t="n">
+        <v>0.0521</v>
+      </c>
+      <c r="N351" s="1" t="n">
+        <v>0.0214</v>
+      </c>
+      <c r="O351" s="1" t="n">
+        <v>0.0094</v>
+      </c>
       <c r="P351" s="1" t="n">
         <f aca="false">SUM(F351:O351)</f>
-        <v>0</v>
+        <v>0.6497</v>
       </c>
       <c r="R351" s="1" t="n">
         <v>6</v>
@@ -16054,9 +16960,39 @@
       <c r="C352" s="1" t="n">
         <v>100</v>
       </c>
+      <c r="F352" s="1" t="n">
+        <v>0.0305</v>
+      </c>
+      <c r="G352" s="1" t="n">
+        <v>0.0339</v>
+      </c>
+      <c r="H352" s="1" t="n">
+        <v>0.0203</v>
+      </c>
+      <c r="I352" s="1" t="n">
+        <v>0.0122</v>
+      </c>
+      <c r="J352" s="1" t="n">
+        <v>0.0271</v>
+      </c>
+      <c r="K352" s="1" t="n">
+        <v>0.0577</v>
+      </c>
+      <c r="L352" s="1" t="n">
+        <v>0.1513</v>
+      </c>
+      <c r="M352" s="1" t="n">
+        <v>0.0272</v>
+      </c>
+      <c r="N352" s="1" t="n">
+        <v>0.0125</v>
+      </c>
+      <c r="O352" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P352" s="1" t="n">
         <f aca="false">SUM(F352:O352)</f>
-        <v>0</v>
+        <v>0.3727</v>
       </c>
       <c r="R352" s="1" t="n">
         <v>6</v>
@@ -16081,9 +17017,39 @@
       <c r="E353" s="1" t="n">
         <v>2100</v>
       </c>
+      <c r="F353" s="1" t="n">
+        <v>0.0892</v>
+      </c>
+      <c r="G353" s="1" t="n">
+        <v>0.0673</v>
+      </c>
+      <c r="H353" s="1" t="n">
+        <v>0.0314</v>
+      </c>
+      <c r="I353" s="1" t="n">
+        <v>0.0142</v>
+      </c>
+      <c r="J353" s="1" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="K353" s="1" t="n">
+        <v>0.1668</v>
+      </c>
+      <c r="L353" s="1" t="n">
+        <v>0.1889</v>
+      </c>
+      <c r="M353" s="1" t="n">
+        <v>0.0395</v>
+      </c>
+      <c r="N353" s="1" t="n">
+        <v>0.0148</v>
+      </c>
+      <c r="O353" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P353" s="1" t="n">
         <f aca="false">SUM(F353:O353)</f>
-        <v>0</v>
+        <v>0.6381</v>
       </c>
       <c r="R353" s="1" t="n">
         <v>6</v>
@@ -16102,9 +17068,39 @@
       <c r="C354" s="1" t="n">
         <v>2100</v>
       </c>
+      <c r="F354" s="1" t="n">
+        <v>0.0669</v>
+      </c>
+      <c r="G354" s="1" t="n">
+        <v>0.0447</v>
+      </c>
+      <c r="H354" s="1" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="I354" s="1" t="n">
+        <v>0.0105</v>
+      </c>
+      <c r="J354" s="1" t="n">
+        <v>0.0258</v>
+      </c>
+      <c r="K354" s="1" t="n">
+        <v>0.1169</v>
+      </c>
+      <c r="L354" s="1" t="n">
+        <v>0.0455</v>
+      </c>
+      <c r="M354" s="1" t="n">
+        <v>0.0194</v>
+      </c>
+      <c r="N354" s="1" t="n">
+        <v>0.0108</v>
+      </c>
+      <c r="O354" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P354" s="1" t="n">
         <f aca="false">SUM(F354:O354)</f>
-        <v>0</v>
+        <v>0.3605</v>
       </c>
       <c r="R354" s="1" t="n">
         <v>6</v>
@@ -16129,9 +17125,39 @@
       <c r="E355" s="1" t="n">
         <v>3350</v>
       </c>
+      <c r="F355" s="1" t="n">
+        <v>0.066</v>
+      </c>
+      <c r="G355" s="1" t="n">
+        <v>0.0445</v>
+      </c>
+      <c r="H355" s="1" t="n">
+        <v>0.0236</v>
+      </c>
+      <c r="I355" s="1" t="n">
+        <v>0.0406</v>
+      </c>
+      <c r="J355" s="1" t="n">
+        <v>0.1471</v>
+      </c>
+      <c r="K355" s="1" t="n">
+        <v>0.1161</v>
+      </c>
+      <c r="L355" s="1" t="n">
+        <v>0.0453</v>
+      </c>
+      <c r="M355" s="1" t="n">
+        <v>0.0237</v>
+      </c>
+      <c r="N355" s="1" t="n">
+        <v>0.0354</v>
+      </c>
+      <c r="O355" s="1" t="n">
+        <v>0.0964</v>
+      </c>
       <c r="P355" s="1" t="n">
         <f aca="false">SUM(F355:O355)</f>
-        <v>0</v>
+        <v>0.6387</v>
       </c>
       <c r="R355" s="1" t="n">
         <v>6</v>
@@ -16174,9 +17200,39 @@
       <c r="E357" s="1" t="n">
         <v>4350</v>
       </c>
+      <c r="F357" s="1" t="n">
+        <v>0.0094</v>
+      </c>
+      <c r="G357" s="1" t="n">
+        <v>0.0155</v>
+      </c>
+      <c r="H357" s="1" t="n">
+        <v>0.0204</v>
+      </c>
+      <c r="I357" s="1" t="n">
+        <v>0.0732</v>
+      </c>
+      <c r="J357" s="1" t="n">
+        <v>0.3409</v>
+      </c>
+      <c r="K357" s="1" t="n">
+        <v>0.0023</v>
+      </c>
+      <c r="L357" s="1" t="n">
+        <v>0.0109</v>
+      </c>
+      <c r="M357" s="1" t="n">
+        <v>0.0186</v>
+      </c>
+      <c r="N357" s="1" t="n">
+        <v>0.0491</v>
+      </c>
+      <c r="O357" s="1" t="n">
+        <v>0.1247</v>
+      </c>
       <c r="P357" s="1" t="n">
         <f aca="false">SUM(F357:O357)</f>
-        <v>0</v>
+        <v>0.665</v>
       </c>
       <c r="R357" s="1" t="n">
         <v>6</v>
@@ -16195,9 +17251,39 @@
       <c r="C358" s="1" t="n">
         <v>4350</v>
       </c>
+      <c r="F358" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G358" s="1" t="n">
+        <v>0.0112</v>
+      </c>
+      <c r="H358" s="1" t="n">
+        <v>0.0129</v>
+      </c>
+      <c r="I358" s="1" t="n">
+        <v>0.0403</v>
+      </c>
+      <c r="J358" s="1" t="n">
+        <v>0.2042</v>
+      </c>
+      <c r="K358" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L358" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M358" s="1" t="n">
+        <v>0.0109</v>
+      </c>
+      <c r="N358" s="1" t="n">
+        <v>0.0235</v>
+      </c>
+      <c r="O358" s="1" t="n">
+        <v>0.0436</v>
+      </c>
       <c r="P358" s="1" t="n">
         <f aca="false">SUM(F358:O358)</f>
-        <v>0</v>
+        <v>0.3466</v>
       </c>
       <c r="R358" s="1" t="n">
         <v>6</v>
@@ -16226,6 +17312,9 @@
         <f aca="false">SUM(F359:O359)</f>
         <v>0</v>
       </c>
+      <c r="Q359" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R359" s="1" t="n">
         <v>6</v>
       </c>
@@ -16247,6 +17336,9 @@
         <f aca="false">SUM(F360:O360)</f>
         <v>0</v>
       </c>
+      <c r="Q360" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R360" s="1" t="n">
         <v>6</v>
       </c>
@@ -16274,6 +17366,9 @@
         <f aca="false">SUM(F361:O361)</f>
         <v>0</v>
       </c>
+      <c r="Q361" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R361" s="1" t="n">
         <v>6</v>
       </c>
@@ -16291,9 +17386,39 @@
       <c r="C362" s="1" t="n">
         <v>100</v>
       </c>
+      <c r="F362" s="1" t="n">
+        <v>0.0329</v>
+      </c>
+      <c r="G362" s="1" t="n">
+        <v>0.0278</v>
+      </c>
+      <c r="H362" s="1" t="n">
+        <v>0.0134</v>
+      </c>
+      <c r="I362" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J362" s="1" t="n">
+        <v>0.0254</v>
+      </c>
+      <c r="K362" s="1" t="n">
+        <v>0.1836</v>
+      </c>
+      <c r="L362" s="1" t="n">
+        <v>0.0453</v>
+      </c>
+      <c r="M362" s="1" t="n">
+        <v>0.0147</v>
+      </c>
+      <c r="N362" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O362" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P362" s="1" t="n">
         <f aca="false">SUM(F362:O362)</f>
-        <v>0</v>
+        <v>0.3431</v>
       </c>
       <c r="R362" s="1" t="n">
         <v>6</v>
@@ -16318,9 +17443,39 @@
       <c r="E363" s="1" t="n">
         <v>1100</v>
       </c>
+      <c r="F363" s="1" t="n">
+        <v>0.0545</v>
+      </c>
+      <c r="G363" s="1" t="n">
+        <v>0.0608</v>
+      </c>
+      <c r="H363" s="1" t="n">
+        <v>0.0381</v>
+      </c>
+      <c r="I363" s="1" t="n">
+        <v>0.0177</v>
+      </c>
+      <c r="J363" s="1" t="n">
+        <v>0.0255</v>
+      </c>
+      <c r="K363" s="1" t="n">
+        <v>0.2116</v>
+      </c>
+      <c r="L363" s="1" t="n">
+        <v>0.1292</v>
+      </c>
+      <c r="M363" s="1" t="n">
+        <v>0.0696</v>
+      </c>
+      <c r="N363" s="1" t="n">
+        <v>0.0209</v>
+      </c>
+      <c r="O363" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P363" s="1" t="n">
         <f aca="false">SUM(F363:O363)</f>
-        <v>0</v>
+        <v>0.6279</v>
       </c>
       <c r="R363" s="1" t="n">
         <v>6</v>
@@ -16339,9 +17494,39 @@
       <c r="C364" s="1" t="n">
         <v>1100</v>
       </c>
+      <c r="F364" s="1" t="n">
+        <v>0.0291</v>
+      </c>
+      <c r="G364" s="1" t="n">
+        <v>0.0427</v>
+      </c>
+      <c r="H364" s="1" t="n">
+        <v>0.0323</v>
+      </c>
+      <c r="I364" s="1" t="n">
+        <v>0.0184</v>
+      </c>
+      <c r="J364" s="1" t="n">
+        <v>0.0279</v>
+      </c>
+      <c r="K364" s="1" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="L364" s="1" t="n">
+        <v>0.0896</v>
+      </c>
+      <c r="M364" s="1" t="n">
+        <v>0.0605</v>
+      </c>
+      <c r="N364" s="1" t="n">
+        <v>0.0207</v>
+      </c>
+      <c r="O364" s="1" t="n">
+        <v>0.0096</v>
+      </c>
       <c r="P364" s="1" t="n">
         <f aca="false">SUM(F364:O364)</f>
-        <v>0</v>
+        <v>0.3658</v>
       </c>
       <c r="R364" s="1" t="n">
         <v>6</v>
@@ -16370,6 +17555,9 @@
         <f aca="false">SUM(F365:O365)</f>
         <v>0</v>
       </c>
+      <c r="Q365" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R365" s="1" t="n">
         <v>6</v>
       </c>
@@ -16391,6 +17579,9 @@
         <f aca="false">SUM(F366:O366)</f>
         <v>0</v>
       </c>
+      <c r="Q366" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R366" s="1" t="n">
         <v>6</v>
       </c>
@@ -16418,6 +17609,9 @@
         <f aca="false">SUM(F367:O367)</f>
         <v>0</v>
       </c>
+      <c r="Q367" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R367" s="1" t="n">
         <v>6</v>
       </c>
@@ -16435,9 +17629,39 @@
       <c r="C368" s="1" t="n">
         <v>3600</v>
       </c>
+      <c r="F368" s="1" t="n">
+        <v>0.0476</v>
+      </c>
+      <c r="G368" s="1" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="H368" s="1" t="n">
+        <v>0.0424</v>
+      </c>
+      <c r="I368" s="1" t="n">
+        <v>0.0166</v>
+      </c>
+      <c r="J368" s="1" t="n">
+        <v>0.0269</v>
+      </c>
+      <c r="K368" s="1" t="n">
+        <v>0.0339</v>
+      </c>
+      <c r="L368" s="1" t="n">
+        <v>0.0402</v>
+      </c>
+      <c r="M368" s="1" t="n">
+        <v>0.0292</v>
+      </c>
+      <c r="N368" s="1" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="O368" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P368" s="1" t="n">
         <f aca="false">SUM(F368:O368)</f>
-        <v>0</v>
+        <v>0.3568</v>
       </c>
       <c r="R368" s="1" t="n">
         <v>6</v>
@@ -16462,9 +17686,39 @@
       <c r="E369" s="1" t="n">
         <v>5100</v>
       </c>
+      <c r="F369" s="1" t="n">
+        <v>0.1204</v>
+      </c>
+      <c r="G369" s="1" t="n">
+        <v>0.2062</v>
+      </c>
+      <c r="H369" s="1" t="n">
+        <v>0.0653</v>
+      </c>
+      <c r="I369" s="1" t="n">
+        <v>0.0224</v>
+      </c>
+      <c r="J369" s="1" t="n">
+        <v>0.0278</v>
+      </c>
+      <c r="K369" s="1" t="n">
+        <v>0.0643</v>
+      </c>
+      <c r="L369" s="1" t="n">
+        <v>0.0655</v>
+      </c>
+      <c r="M369" s="1" t="n">
+        <v>0.0437</v>
+      </c>
+      <c r="N369" s="1" t="n">
+        <v>0.0204</v>
+      </c>
+      <c r="O369" s="1" t="n">
+        <v>0.0092</v>
+      </c>
       <c r="P369" s="1" t="n">
         <f aca="false">SUM(F369:O369)</f>
-        <v>0</v>
+        <v>0.6452</v>
       </c>
       <c r="R369" s="1" t="n">
         <v>6</v>
@@ -16483,9 +17737,39 @@
       <c r="C370" s="1" t="n">
         <v>5100</v>
       </c>
+      <c r="F370" s="1" t="n">
+        <v>0.0803</v>
+      </c>
+      <c r="G370" s="1" t="n">
+        <v>0.1216</v>
+      </c>
+      <c r="H370" s="1" t="n">
+        <v>0.0303</v>
+      </c>
+      <c r="I370" s="1" t="n">
+        <v>0.0136</v>
+      </c>
+      <c r="J370" s="1" t="n">
+        <v>0.0268</v>
+      </c>
+      <c r="K370" s="1" t="n">
+        <v>0.0358</v>
+      </c>
+      <c r="L370" s="1" t="n">
+        <v>0.0321</v>
+      </c>
+      <c r="M370" s="1" t="n">
+        <v>0.0208</v>
+      </c>
+      <c r="N370" s="1" t="n">
+        <v>0.0124</v>
+      </c>
+      <c r="O370" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P370" s="1" t="n">
         <f aca="false">SUM(F370:O370)</f>
-        <v>0</v>
+        <v>0.3737</v>
       </c>
       <c r="R370" s="1" t="n">
         <v>6</v>
@@ -16510,9 +17794,39 @@
       <c r="E371" s="1" t="n">
         <v>1100</v>
       </c>
+      <c r="F371" s="1" t="n">
+        <v>0.1046</v>
+      </c>
+      <c r="G371" s="1" t="n">
+        <v>0.1531</v>
+      </c>
+      <c r="H371" s="1" t="n">
+        <v>0.0501</v>
+      </c>
+      <c r="I371" s="1" t="n">
+        <v>0.0205</v>
+      </c>
+      <c r="J371" s="1" t="n">
+        <v>0.0273</v>
+      </c>
+      <c r="K371" s="1" t="n">
+        <v>0.0743</v>
+      </c>
+      <c r="L371" s="1" t="n">
+        <v>0.1306</v>
+      </c>
+      <c r="M371" s="1" t="n">
+        <v>0.058</v>
+      </c>
+      <c r="N371" s="1" t="n">
+        <v>0.0211</v>
+      </c>
+      <c r="O371" s="1" t="n">
+        <v>0.009</v>
+      </c>
       <c r="P371" s="1" t="n">
         <f aca="false">SUM(F371:O371)</f>
-        <v>0</v>
+        <v>0.6486</v>
       </c>
       <c r="R371" s="1" t="n">
         <v>6</v>
@@ -16531,9 +17845,39 @@
       <c r="C372" s="1" t="n">
         <v>1100</v>
       </c>
+      <c r="F372" s="1" t="n">
+        <v>0.0323</v>
+      </c>
+      <c r="G372" s="1" t="n">
+        <v>0.0422</v>
+      </c>
+      <c r="H372" s="1" t="n">
+        <v>0.0278</v>
+      </c>
+      <c r="I372" s="1" t="n">
+        <v>0.0151</v>
+      </c>
+      <c r="J372" s="1" t="n">
+        <v>0.0269</v>
+      </c>
+      <c r="K372" s="1" t="n">
+        <v>0.0444</v>
+      </c>
+      <c r="L372" s="1" t="n">
+        <v>0.1055</v>
+      </c>
+      <c r="M372" s="1" t="n">
+        <v>0.0434</v>
+      </c>
+      <c r="N372" s="1" t="n">
+        <v>0.0164</v>
+      </c>
+      <c r="O372" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P372" s="1" t="n">
         <f aca="false">SUM(F372:O372)</f>
-        <v>0</v>
+        <v>0.354</v>
       </c>
       <c r="R372" s="1" t="n">
         <v>6</v>
@@ -16562,6 +17906,9 @@
         <f aca="false">SUM(F373:O373)</f>
         <v>0</v>
       </c>
+      <c r="Q373" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R373" s="1" t="n">
         <v>6</v>
       </c>
@@ -16583,6 +17930,9 @@
         <f aca="false">SUM(F374:O374)</f>
         <v>0</v>
       </c>
+      <c r="Q374" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R374" s="1" t="n">
         <v>6</v>
       </c>
@@ -16610,6 +17960,9 @@
         <f aca="false">SUM(F375:O375)</f>
         <v>0</v>
       </c>
+      <c r="Q375" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R375" s="1" t="n">
         <v>6</v>
       </c>
@@ -16631,6 +17984,9 @@
         <f aca="false">SUM(F376:O376)</f>
         <v>0</v>
       </c>
+      <c r="Q376" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R376" s="1" t="n">
         <v>6</v>
       </c>
@@ -16658,6 +18014,9 @@
         <f aca="false">SUM(F377:O377)</f>
         <v>0</v>
       </c>
+      <c r="Q377" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R377" s="1" t="n">
         <v>6</v>
       </c>
@@ -16703,6 +18062,9 @@
         <f aca="false">SUM(F379:O379)</f>
         <v>0</v>
       </c>
+      <c r="Q379" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R379" s="1" t="n">
         <v>6</v>
       </c>
@@ -16724,6 +18086,9 @@
         <f aca="false">SUM(F380:O380)</f>
         <v>0</v>
       </c>
+      <c r="Q380" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R380" s="1" t="n">
         <v>6</v>
       </c>
@@ -16751,6 +18116,9 @@
         <f aca="false">SUM(F381:O381)</f>
         <v>0</v>
       </c>
+      <c r="Q381" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R381" s="1" t="n">
         <v>6</v>
       </c>
@@ -16768,9 +18136,39 @@
       <c r="C382" s="1" t="n">
         <v>100</v>
       </c>
+      <c r="F382" s="1" t="n">
+        <v>0.0307</v>
+      </c>
+      <c r="G382" s="1" t="n">
+        <v>0.0259</v>
+      </c>
+      <c r="H382" s="1" t="n">
+        <v>0.0143</v>
+      </c>
+      <c r="I382" s="1" t="n">
+        <v>0.009</v>
+      </c>
+      <c r="J382" s="1" t="n">
+        <v>0.0254</v>
+      </c>
+      <c r="K382" s="1" t="n">
+        <v>0.2111</v>
+      </c>
+      <c r="L382" s="1" t="n">
+        <v>0.0306</v>
+      </c>
+      <c r="M382" s="1" t="n">
+        <v>0.0135</v>
+      </c>
+      <c r="N382" s="1" t="n">
+        <v>0.0089</v>
+      </c>
+      <c r="O382" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P382" s="1" t="n">
         <f aca="false">SUM(F382:O382)</f>
-        <v>0</v>
+        <v>0.3694</v>
       </c>
       <c r="R382" s="1" t="n">
         <v>6</v>
@@ -16795,9 +18193,39 @@
       <c r="E383" s="1" t="n">
         <v>3850</v>
       </c>
+      <c r="F383" s="1" t="n">
+        <v>0.1195</v>
+      </c>
+      <c r="G383" s="1" t="n">
+        <v>0.0923</v>
+      </c>
+      <c r="H383" s="1" t="n">
+        <v>0.0332</v>
+      </c>
+      <c r="I383" s="1" t="n">
+        <v>0.0136</v>
+      </c>
+      <c r="J383" s="1" t="n">
+        <v>0.0257</v>
+      </c>
+      <c r="K383" s="1" t="n">
+        <v>0.253</v>
+      </c>
+      <c r="L383" s="1" t="n">
+        <v>0.063</v>
+      </c>
+      <c r="M383" s="1" t="n">
+        <v>0.0287</v>
+      </c>
+      <c r="N383" s="1" t="n">
+        <v>0.0132</v>
+      </c>
+      <c r="O383" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P383" s="1" t="n">
         <f aca="false">SUM(F383:O383)</f>
-        <v>0</v>
+        <v>0.6422</v>
       </c>
       <c r="R383" s="1" t="n">
         <v>6</v>
@@ -16816,9 +18244,39 @@
       <c r="C384" s="1" t="n">
         <v>3850</v>
       </c>
+      <c r="F384" s="1" t="n">
+        <v>0.0966</v>
+      </c>
+      <c r="G384" s="1" t="n">
+        <v>0.0773</v>
+      </c>
+      <c r="H384" s="1" t="n">
+        <v>0.0275</v>
+      </c>
+      <c r="I384" s="1" t="n">
+        <v>0.0121</v>
+      </c>
+      <c r="J384" s="1" t="n">
+        <v>0.0255</v>
+      </c>
+      <c r="K384" s="1" t="n">
+        <v>0.0492</v>
+      </c>
+      <c r="L384" s="1" t="n">
+        <v>0.0401</v>
+      </c>
+      <c r="M384" s="1" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="N384" s="1" t="n">
+        <v>0.0117</v>
+      </c>
+      <c r="O384" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P384" s="1" t="n">
         <f aca="false">SUM(F384:O384)</f>
-        <v>0</v>
+        <v>0.362</v>
       </c>
       <c r="R384" s="1" t="n">
         <v>6</v>
@@ -16847,6 +18305,9 @@
         <f aca="false">SUM(F385:O385)</f>
         <v>0</v>
       </c>
+      <c r="Q385" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R385" s="1" t="n">
         <v>6</v>
       </c>
@@ -16892,6 +18353,9 @@
         <f aca="false">SUM(F387:O387)</f>
         <v>0</v>
       </c>
+      <c r="Q387" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R387" s="1" t="n">
         <v>6</v>
       </c>
@@ -16909,9 +18373,39 @@
       <c r="C388" s="1" t="n">
         <v>1850</v>
       </c>
+      <c r="F388" s="1" t="n">
+        <v>0.0265</v>
+      </c>
+      <c r="G388" s="1" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="H388" s="1" t="n">
+        <v>0.0416</v>
+      </c>
+      <c r="I388" s="1" t="n">
+        <v>0.0229</v>
+      </c>
+      <c r="J388" s="1" t="n">
+        <v>0.0287</v>
+      </c>
+      <c r="K388" s="1" t="n">
+        <v>0.0259</v>
+      </c>
+      <c r="L388" s="1" t="n">
+        <v>0.0575</v>
+      </c>
+      <c r="M388" s="1" t="n">
+        <v>0.0658</v>
+      </c>
+      <c r="N388" s="1" t="n">
+        <v>0.0253</v>
+      </c>
+      <c r="O388" s="1" t="n">
+        <v>0.0112</v>
+      </c>
       <c r="P388" s="1" t="n">
         <f aca="false">SUM(F388:O388)</f>
-        <v>0</v>
+        <v>0.3514</v>
       </c>
       <c r="R388" s="1" t="n">
         <v>6</v>
@@ -16936,9 +18430,39 @@
       <c r="E389" s="1" t="n">
         <v>3350</v>
       </c>
+      <c r="F389" s="1" t="n">
+        <v>0.0546</v>
+      </c>
+      <c r="G389" s="1" t="n">
+        <v>0.1168</v>
+      </c>
+      <c r="H389" s="1" t="n">
+        <v>0.0953</v>
+      </c>
+      <c r="I389" s="1" t="n">
+        <v>0.0411</v>
+      </c>
+      <c r="J389" s="1" t="n">
+        <v>0.0357</v>
+      </c>
+      <c r="K389" s="1" t="n">
+        <v>0.0497</v>
+      </c>
+      <c r="L389" s="1" t="n">
+        <v>0.0947</v>
+      </c>
+      <c r="M389" s="1" t="n">
+        <v>0.1012</v>
+      </c>
+      <c r="N389" s="1" t="n">
+        <v>0.0412</v>
+      </c>
+      <c r="O389" s="1" t="n">
+        <v>0.0185</v>
+      </c>
       <c r="P389" s="1" t="n">
         <f aca="false">SUM(F389:O389)</f>
-        <v>0</v>
+        <v>0.6488</v>
       </c>
       <c r="R389" s="1" t="n">
         <v>6</v>
@@ -16957,9 +18481,39 @@
       <c r="C390" s="1" t="n">
         <v>3350</v>
       </c>
+      <c r="F390" s="1" t="n">
+        <v>0.0343</v>
+      </c>
+      <c r="G390" s="1" t="n">
+        <v>0.0786</v>
+      </c>
+      <c r="H390" s="1" t="n">
+        <v>0.0586</v>
+      </c>
+      <c r="I390" s="1" t="n">
+        <v>0.0229</v>
+      </c>
+      <c r="J390" s="1" t="n">
+        <v>0.0297</v>
+      </c>
+      <c r="K390" s="1" t="n">
+        <v>0.0267</v>
+      </c>
+      <c r="L390" s="1" t="n">
+        <v>0.042</v>
+      </c>
+      <c r="M390" s="1" t="n">
+        <v>0.0388</v>
+      </c>
+      <c r="N390" s="1" t="n">
+        <v>0.0204</v>
+      </c>
+      <c r="O390" s="1" t="n">
+        <v>0.017</v>
+      </c>
       <c r="P390" s="1" t="n">
         <f aca="false">SUM(F390:O390)</f>
-        <v>0</v>
+        <v>0.369</v>
       </c>
       <c r="R390" s="1" t="n">
         <v>6</v>
@@ -16984,9 +18538,39 @@
       <c r="E391" s="1" t="n">
         <v>2600</v>
       </c>
+      <c r="F391" s="1" t="n">
+        <v>0.0357</v>
+      </c>
+      <c r="G391" s="1" t="n">
+        <v>0.0835</v>
+      </c>
+      <c r="H391" s="1" t="n">
+        <v>0.0723</v>
+      </c>
+      <c r="I391" s="1" t="n">
+        <v>0.0731</v>
+      </c>
+      <c r="J391" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="K391" s="1" t="n">
+        <v>0.0279</v>
+      </c>
+      <c r="L391" s="1" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="M391" s="1" t="n">
+        <v>0.0533</v>
+      </c>
+      <c r="N391" s="1" t="n">
+        <v>0.0717</v>
+      </c>
+      <c r="O391" s="1" t="n">
+        <v>0.094</v>
+      </c>
       <c r="P391" s="1" t="n">
         <f aca="false">SUM(F391:O391)</f>
-        <v>0</v>
+        <v>0.6575</v>
       </c>
       <c r="R391" s="1" t="n">
         <v>6</v>
@@ -17029,9 +18613,39 @@
       <c r="E393" s="1" t="n">
         <v>3600</v>
       </c>
+      <c r="F393" s="1" t="n">
+        <v>0.0114</v>
+      </c>
+      <c r="G393" s="1" t="n">
+        <v>0.0214</v>
+      </c>
+      <c r="H393" s="1" t="n">
+        <v>0.0397</v>
+      </c>
+      <c r="I393" s="1" t="n">
+        <v>0.1487</v>
+      </c>
+      <c r="J393" s="1" t="n">
+        <v>0.1572</v>
+      </c>
+      <c r="K393" s="1" t="n">
+        <v>0.0089</v>
+      </c>
+      <c r="L393" s="1" t="n">
+        <v>0.0165</v>
+      </c>
+      <c r="M393" s="1" t="n">
+        <v>0.0358</v>
+      </c>
+      <c r="N393" s="1" t="n">
+        <v>0.0963</v>
+      </c>
+      <c r="O393" s="1" t="n">
+        <v>0.1344</v>
+      </c>
       <c r="P393" s="1" t="n">
         <f aca="false">SUM(F393:O393)</f>
-        <v>0</v>
+        <v>0.6703</v>
       </c>
       <c r="R393" s="1" t="n">
         <v>6</v>
@@ -17050,9 +18664,39 @@
       <c r="C394" s="1" t="n">
         <v>3600</v>
       </c>
+      <c r="F394" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G394" s="1" t="n">
+        <v>0.0146</v>
+      </c>
+      <c r="H394" s="1" t="n">
+        <v>0.0249</v>
+      </c>
+      <c r="I394" s="1" t="n">
+        <v>0.0988</v>
+      </c>
+      <c r="J394" s="1" t="n">
+        <v>0.0905</v>
+      </c>
+      <c r="K394" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L394" s="1" t="n">
+        <v>0.0107</v>
+      </c>
+      <c r="M394" s="1" t="n">
+        <v>0.0201</v>
+      </c>
+      <c r="N394" s="1" t="n">
+        <v>0.0452</v>
+      </c>
+      <c r="O394" s="1" t="n">
+        <v>0.0523</v>
+      </c>
       <c r="P394" s="1" t="n">
         <f aca="false">SUM(F394:O394)</f>
-        <v>0</v>
+        <v>0.3571</v>
       </c>
       <c r="R394" s="1" t="n">
         <v>6</v>
@@ -17077,9 +18721,39 @@
       <c r="E395" s="1" t="n">
         <v>4850</v>
       </c>
+      <c r="F395" s="1" t="n">
+        <v>0.0121</v>
+      </c>
+      <c r="G395" s="1" t="n">
+        <v>0.0358</v>
+      </c>
+      <c r="H395" s="1" t="n">
+        <v>0.1703</v>
+      </c>
+      <c r="I395" s="1" t="n">
+        <v>0.1319</v>
+      </c>
+      <c r="J395" s="1" t="n">
+        <v>0.0968</v>
+      </c>
+      <c r="K395" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L395" s="1" t="n">
+        <v>0.0197</v>
+      </c>
+      <c r="M395" s="1" t="n">
+        <v>0.0383</v>
+      </c>
+      <c r="N395" s="1" t="n">
+        <v>0.0603</v>
+      </c>
+      <c r="O395" s="1" t="n">
+        <v>0.0595</v>
+      </c>
       <c r="P395" s="1" t="n">
         <f aca="false">SUM(F395:O395)</f>
-        <v>0</v>
+        <v>0.6247</v>
       </c>
       <c r="R395" s="1" t="n">
         <v>6</v>
@@ -17098,9 +18772,39 @@
       <c r="C396" s="1" t="n">
         <v>4850</v>
       </c>
+      <c r="F396" s="1" t="n">
+        <v>0.0125</v>
+      </c>
+      <c r="G396" s="1" t="n">
+        <v>0.0316</v>
+      </c>
+      <c r="H396" s="1" t="n">
+        <v>0.1525</v>
+      </c>
+      <c r="I396" s="1" t="n">
+        <v>0.0435</v>
+      </c>
+      <c r="J396" s="1" t="n">
+        <v>0.0355</v>
+      </c>
+      <c r="K396" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L396" s="1" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="M396" s="1" t="n">
+        <v>0.0242</v>
+      </c>
+      <c r="N396" s="1" t="n">
+        <v>0.0152</v>
+      </c>
+      <c r="O396" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P396" s="1" t="n">
         <f aca="false">SUM(F396:O396)</f>
-        <v>0</v>
+        <v>0.332</v>
       </c>
       <c r="R396" s="1" t="n">
         <v>6</v>
@@ -17125,9 +18829,39 @@
       <c r="E397" s="1" t="n">
         <v>2350</v>
       </c>
+      <c r="F397" s="1" t="n">
+        <v>0.0612</v>
+      </c>
+      <c r="G397" s="1" t="n">
+        <v>0.0841</v>
+      </c>
+      <c r="H397" s="1" t="n">
+        <v>0.1756</v>
+      </c>
+      <c r="I397" s="1" t="n">
+        <v>0.0511</v>
+      </c>
+      <c r="J397" s="1" t="n">
+        <v>0.0368</v>
+      </c>
+      <c r="K397" s="1" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="L397" s="1" t="n">
+        <v>0.0742</v>
+      </c>
+      <c r="M397" s="1" t="n">
+        <v>0.0499</v>
+      </c>
+      <c r="N397" s="1" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="O397" s="1" t="n">
+        <v>0.0171</v>
+      </c>
       <c r="P397" s="1" t="n">
         <f aca="false">SUM(F397:O397)</f>
-        <v>0</v>
+        <v>0.646</v>
       </c>
       <c r="R397" s="1" t="n">
         <v>6</v>
@@ -17146,9 +18880,39 @@
       <c r="C398" s="1" t="n">
         <v>2350</v>
       </c>
+      <c r="F398" s="1" t="n">
+        <v>0.0542</v>
+      </c>
+      <c r="G398" s="1" t="n">
+        <v>0.0604</v>
+      </c>
+      <c r="H398" s="1" t="n">
+        <v>0.0292</v>
+      </c>
+      <c r="I398" s="1" t="n">
+        <v>0.0142</v>
+      </c>
+      <c r="J398" s="1" t="n">
+        <v>0.0279</v>
+      </c>
+      <c r="K398" s="1" t="n">
+        <v>0.059</v>
+      </c>
+      <c r="L398" s="1" t="n">
+        <v>0.0628</v>
+      </c>
+      <c r="M398" s="1" t="n">
+        <v>0.0302</v>
+      </c>
+      <c r="N398" s="1" t="n">
+        <v>0.0143</v>
+      </c>
+      <c r="O398" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P398" s="1" t="n">
         <f aca="false">SUM(F398:O398)</f>
-        <v>0</v>
+        <v>0.3522</v>
       </c>
       <c r="R398" s="1" t="n">
         <v>6</v>
@@ -17177,6 +18941,9 @@
         <f aca="false">SUM(F399:O399)</f>
         <v>0</v>
       </c>
+      <c r="Q399" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R399" s="1" t="n">
         <v>6</v>
       </c>
@@ -17198,6 +18965,9 @@
         <f aca="false">SUM(F400:O400)</f>
         <v>0</v>
       </c>
+      <c r="Q400" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R400" s="1" t="n">
         <v>6</v>
       </c>
@@ -17225,6 +18995,9 @@
         <f aca="false">SUM(F401:O401)</f>
         <v>0</v>
       </c>
+      <c r="Q401" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R401" s="1" t="n">
         <v>6</v>
       </c>
@@ -17242,9 +19015,39 @@
       <c r="C402" s="1" t="n">
         <v>2850</v>
       </c>
+      <c r="F402" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G402" s="1" t="n">
+        <v>0.0107</v>
+      </c>
+      <c r="H402" s="1" t="n">
+        <v>0.0143</v>
+      </c>
+      <c r="I402" s="1" t="n">
+        <v>0.0462</v>
+      </c>
+      <c r="J402" s="1" t="n">
+        <v>0.1187</v>
+      </c>
+      <c r="K402" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L402" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M402" s="1" t="n">
+        <v>0.0136</v>
+      </c>
+      <c r="N402" s="1" t="n">
+        <v>0.0412</v>
+      </c>
+      <c r="O402" s="1" t="n">
+        <v>0.0949</v>
+      </c>
       <c r="P402" s="1" t="n">
         <f aca="false">SUM(F402:O402)</f>
-        <v>0</v>
+        <v>0.3396</v>
       </c>
       <c r="R402" s="1" t="n">
         <v>6</v>
@@ -17269,9 +19072,39 @@
       <c r="E403" s="1" t="n">
         <v>4600</v>
       </c>
+      <c r="F403" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G403" s="1" t="n">
+        <v>0.0143</v>
+      </c>
+      <c r="H403" s="1" t="n">
+        <v>0.0336</v>
+      </c>
+      <c r="I403" s="1" t="n">
+        <v>0.2312</v>
+      </c>
+      <c r="J403" s="1" t="n">
+        <v>0.1374</v>
+      </c>
+      <c r="K403" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L403" s="1" t="n">
+        <v>0.0099</v>
+      </c>
+      <c r="M403" s="1" t="n">
+        <v>0.0232</v>
+      </c>
+      <c r="N403" s="1" t="n">
+        <v>0.0583</v>
+      </c>
+      <c r="O403" s="1" t="n">
+        <v>0.1097</v>
+      </c>
       <c r="P403" s="1" t="n">
         <f aca="false">SUM(F403:O403)</f>
-        <v>0</v>
+        <v>0.6176</v>
       </c>
       <c r="R403" s="1" t="n">
         <v>6</v>
@@ -17290,9 +19123,39 @@
       <c r="C404" s="1" t="n">
         <v>4600</v>
       </c>
+      <c r="F404" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G404" s="1" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="H404" s="1" t="n">
+        <v>0.0261</v>
+      </c>
+      <c r="I404" s="1" t="n">
+        <v>0.1913</v>
+      </c>
+      <c r="J404" s="1" t="n">
+        <v>0.047</v>
+      </c>
+      <c r="K404" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L404" s="1" t="n">
+        <v>0.0096</v>
+      </c>
+      <c r="M404" s="1" t="n">
+        <v>0.0154</v>
+      </c>
+      <c r="N404" s="1" t="n">
+        <v>0.0243</v>
+      </c>
+      <c r="O404" s="1" t="n">
+        <v>0.0215</v>
+      </c>
       <c r="P404" s="1" t="n">
         <f aca="false">SUM(F404:O404)</f>
-        <v>0</v>
+        <v>0.3492</v>
       </c>
       <c r="R404" s="1" t="n">
         <v>6</v>
@@ -17317,9 +19180,39 @@
       <c r="E405" s="1" t="n">
         <v>350</v>
       </c>
+      <c r="F405" s="1" t="n">
+        <v>0.0429</v>
+      </c>
+      <c r="G405" s="1" t="n">
+        <v>0.0364</v>
+      </c>
+      <c r="H405" s="1" t="n">
+        <v>0.0345</v>
+      </c>
+      <c r="I405" s="1" t="n">
+        <v>0.1915</v>
+      </c>
+      <c r="J405" s="1" t="n">
+        <v>0.0463</v>
+      </c>
+      <c r="K405" s="1" t="n">
+        <v>0.1707</v>
+      </c>
+      <c r="L405" s="1" t="n">
+        <v>0.0414</v>
+      </c>
+      <c r="M405" s="1" t="n">
+        <v>0.0252</v>
+      </c>
+      <c r="N405" s="1" t="n">
+        <v>0.0264</v>
+      </c>
+      <c r="O405" s="1" t="n">
+        <v>0.0211</v>
+      </c>
       <c r="P405" s="1" t="n">
         <f aca="false">SUM(F405:O405)</f>
-        <v>0</v>
+        <v>0.6364</v>
       </c>
       <c r="R405" s="1" t="n">
         <v>6</v>
@@ -17338,9 +19231,39 @@
       <c r="C406" s="1" t="n">
         <v>350</v>
       </c>
+      <c r="F406" s="1" t="n">
+        <v>0.042</v>
+      </c>
+      <c r="G406" s="1" t="n">
+        <v>0.0324</v>
+      </c>
+      <c r="H406" s="1" t="n">
+        <v>0.0167</v>
+      </c>
+      <c r="I406" s="1" t="n">
+        <v>0.0102</v>
+      </c>
+      <c r="J406" s="1" t="n">
+        <v>0.0297</v>
+      </c>
+      <c r="K406" s="1" t="n">
+        <v>0.1696</v>
+      </c>
+      <c r="L406" s="1" t="n">
+        <v>0.0388</v>
+      </c>
+      <c r="M406" s="1" t="n">
+        <v>0.0168</v>
+      </c>
+      <c r="N406" s="1" t="n">
+        <v>0.0115</v>
+      </c>
+      <c r="O406" s="1" t="n">
+        <v>0.0091</v>
+      </c>
       <c r="P406" s="1" t="n">
         <f aca="false">SUM(F406:O406)</f>
-        <v>0</v>
+        <v>0.3768</v>
       </c>
       <c r="R406" s="1" t="n">
         <v>6</v>
@@ -17365,9 +19288,39 @@
       <c r="E407" s="1" t="n">
         <v>2600</v>
       </c>
+      <c r="F407" s="1" t="n">
+        <v>0.0424</v>
+      </c>
+      <c r="G407" s="1" t="n">
+        <v>0.0348</v>
+      </c>
+      <c r="H407" s="1" t="n">
+        <v>0.0257</v>
+      </c>
+      <c r="I407" s="1" t="n">
+        <v>0.0523</v>
+      </c>
+      <c r="J407" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="K407" s="1" t="n">
+        <v>0.1698</v>
+      </c>
+      <c r="L407" s="1" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="M407" s="1" t="n">
+        <v>0.0273</v>
+      </c>
+      <c r="N407" s="1" t="n">
+        <v>0.055</v>
+      </c>
+      <c r="O407" s="1" t="n">
+        <v>0.0942</v>
+      </c>
       <c r="P407" s="1" t="n">
         <f aca="false">SUM(F407:O407)</f>
-        <v>0</v>
+        <v>0.6415</v>
       </c>
       <c r="R407" s="1" t="n">
         <v>6</v>
@@ -17386,9 +19339,39 @@
       <c r="C408" s="1" t="n">
         <v>2600</v>
       </c>
+      <c r="F408" s="1" t="n">
+        <v>0.0094</v>
+      </c>
+      <c r="G408" s="1" t="n">
+        <v>0.0146</v>
+      </c>
+      <c r="H408" s="1" t="n">
+        <v>0.0182</v>
+      </c>
+      <c r="I408" s="1" t="n">
+        <v>0.0499</v>
+      </c>
+      <c r="J408" s="1" t="n">
+        <v>0.0993</v>
+      </c>
+      <c r="K408" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L408" s="1" t="n">
+        <v>0.0117</v>
+      </c>
+      <c r="M408" s="1" t="n">
+        <v>0.0181</v>
+      </c>
+      <c r="N408" s="1" t="n">
+        <v>0.0522</v>
+      </c>
+      <c r="O408" s="1" t="n">
+        <v>0.093</v>
+      </c>
       <c r="P408" s="1" t="n">
         <f aca="false">SUM(F408:O408)</f>
-        <v>0</v>
+        <v>0.3664</v>
       </c>
       <c r="R408" s="1" t="n">
         <v>6</v>
@@ -17413,9 +19396,39 @@
       <c r="E409" s="1" t="n">
         <v>4100</v>
       </c>
+      <c r="F409" s="1" t="n">
+        <v>0.0223</v>
+      </c>
+      <c r="G409" s="1" t="n">
+        <v>0.0666</v>
+      </c>
+      <c r="H409" s="1" t="n">
+        <v>0.1049</v>
+      </c>
+      <c r="I409" s="1" t="n">
+        <v>0.072</v>
+      </c>
+      <c r="J409" s="1" t="n">
+        <v>0.1056</v>
+      </c>
+      <c r="K409" s="1" t="n">
+        <v>0.0154</v>
+      </c>
+      <c r="L409" s="1" t="n">
+        <v>0.0302</v>
+      </c>
+      <c r="M409" s="1" t="n">
+        <v>0.0446</v>
+      </c>
+      <c r="N409" s="1" t="n">
+        <v>0.0675</v>
+      </c>
+      <c r="O409" s="1" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P409" s="1" t="n">
         <f aca="false">SUM(F409:O409)</f>
-        <v>0</v>
+        <v>0.6291</v>
       </c>
       <c r="R409" s="1" t="n">
         <v>6</v>
@@ -17434,9 +19447,39 @@
       <c r="C410" s="1" t="n">
         <v>4100</v>
       </c>
+      <c r="F410" s="1" t="n">
+        <v>0.0229</v>
+      </c>
+      <c r="G410" s="1" t="n">
+        <v>0.0639</v>
+      </c>
+      <c r="H410" s="1" t="n">
+        <v>0.0942</v>
+      </c>
+      <c r="I410" s="1" t="n">
+        <v>0.0281</v>
+      </c>
+      <c r="J410" s="1" t="n">
+        <v>0.0331</v>
+      </c>
+      <c r="K410" s="1" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="L410" s="1" t="n">
+        <v>0.0282</v>
+      </c>
+      <c r="M410" s="1" t="n">
+        <v>0.0329</v>
+      </c>
+      <c r="N410" s="1" t="n">
+        <v>0.0224</v>
+      </c>
+      <c r="O410" s="1" t="n">
+        <v>0.0132</v>
+      </c>
       <c r="P410" s="1" t="n">
         <f aca="false">SUM(F410:O410)</f>
-        <v>0</v>
+        <v>0.3559</v>
       </c>
       <c r="R410" s="1" t="n">
         <v>6</v>
@@ -17461,9 +19504,39 @@
       <c r="E411" s="1" t="n">
         <v>4100</v>
       </c>
+      <c r="F411" s="1" t="n">
+        <v>0.0491</v>
+      </c>
+      <c r="G411" s="1" t="n">
+        <v>0.1503</v>
+      </c>
+      <c r="H411" s="1" t="n">
+        <v>0.1526</v>
+      </c>
+      <c r="I411" s="1" t="n">
+        <v>0.0425</v>
+      </c>
+      <c r="J411" s="1" t="n">
+        <v>0.0362</v>
+      </c>
+      <c r="K411" s="1" t="n">
+        <v>0.0373</v>
+      </c>
+      <c r="L411" s="1" t="n">
+        <v>0.0556</v>
+      </c>
+      <c r="M411" s="1" t="n">
+        <v>0.059</v>
+      </c>
+      <c r="N411" s="1" t="n">
+        <v>0.0344</v>
+      </c>
+      <c r="O411" s="1" t="n">
+        <v>0.0173</v>
+      </c>
       <c r="P411" s="1" t="n">
         <f aca="false">SUM(F411:O411)</f>
-        <v>0</v>
+        <v>0.6343</v>
       </c>
       <c r="R411" s="1" t="n">
         <v>6</v>
@@ -17482,9 +19555,39 @@
       <c r="C412" s="1" t="n">
         <v>4100</v>
       </c>
+      <c r="F412" s="1" t="n">
+        <v>0.0342</v>
+      </c>
+      <c r="G412" s="1" t="n">
+        <v>0.0966</v>
+      </c>
+      <c r="H412" s="1" t="n">
+        <v>0.0659</v>
+      </c>
+      <c r="I412" s="1" t="n">
+        <v>0.0213</v>
+      </c>
+      <c r="J412" s="1" t="n">
+        <v>0.0311</v>
+      </c>
+      <c r="K412" s="1" t="n">
+        <v>0.0253</v>
+      </c>
+      <c r="L412" s="1" t="n">
+        <v>0.0347</v>
+      </c>
+      <c r="M412" s="1" t="n">
+        <v>0.0316</v>
+      </c>
+      <c r="N412" s="1" t="n">
+        <v>0.0192</v>
+      </c>
+      <c r="O412" s="1" t="n">
+        <v>0.0115</v>
+      </c>
       <c r="P412" s="1" t="n">
         <f aca="false">SUM(F412:O412)</f>
-        <v>0</v>
+        <v>0.3714</v>
       </c>
       <c r="R412" s="1" t="n">
         <v>6</v>
@@ -17513,6 +19616,9 @@
         <f aca="false">SUM(F413:O413)</f>
         <v>0</v>
       </c>
+      <c r="Q413" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R413" s="1" t="n">
         <v>6</v>
       </c>
@@ -17558,6 +19664,9 @@
         <f aca="false">SUM(F415:O415)</f>
         <v>0</v>
       </c>
+      <c r="Q415" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R415" s="1" t="n">
         <v>6</v>
       </c>
@@ -17575,9 +19684,39 @@
       <c r="C416" s="1" t="n">
         <v>4350</v>
       </c>
+      <c r="F416" s="1" t="n">
+        <v>0.0128</v>
+      </c>
+      <c r="G416" s="1" t="n">
+        <v>0.0238</v>
+      </c>
+      <c r="H416" s="1" t="n">
+        <v>0.0534</v>
+      </c>
+      <c r="I416" s="1" t="n">
+        <v>0.1142</v>
+      </c>
+      <c r="J416" s="1" t="n">
+        <v>0.0479</v>
+      </c>
+      <c r="K416" s="1" t="n">
+        <v>0.0105</v>
+      </c>
+      <c r="L416" s="1" t="n">
+        <v>0.0168</v>
+      </c>
+      <c r="M416" s="1" t="n">
+        <v>0.0266</v>
+      </c>
+      <c r="N416" s="1" t="n">
+        <v>0.0343</v>
+      </c>
+      <c r="O416" s="1" t="n">
+        <v>0.0233</v>
+      </c>
       <c r="P416" s="1" t="n">
         <f aca="false">SUM(F416:O416)</f>
-        <v>0</v>
+        <v>0.3636</v>
       </c>
       <c r="R416" s="1" t="n">
         <v>6</v>
@@ -17602,9 +19741,39 @@
       <c r="E417" s="1" t="n">
         <v>2350</v>
       </c>
+      <c r="F417" s="1" t="n">
+        <v>0.0116</v>
+      </c>
+      <c r="G417" s="1" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H417" s="1" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="I417" s="1" t="n">
+        <v>0.1676</v>
+      </c>
+      <c r="J417" s="1" t="n">
+        <v>0.0776</v>
+      </c>
+      <c r="K417" s="1" t="n">
+        <v>0.0053</v>
+      </c>
+      <c r="L417" s="1" t="n">
+        <v>0.0222</v>
+      </c>
+      <c r="M417" s="1" t="n">
+        <v>0.0569</v>
+      </c>
+      <c r="N417" s="1" t="n">
+        <v>0.1039</v>
+      </c>
+      <c r="O417" s="1" t="n">
+        <v>0.0611</v>
+      </c>
       <c r="P417" s="1" t="n">
         <f aca="false">SUM(F417:O417)</f>
-        <v>0</v>
+        <v>0.6142</v>
       </c>
       <c r="R417" s="1" t="n">
         <v>6</v>
@@ -17623,9 +19792,39 @@
       <c r="C418" s="1" t="n">
         <v>2350</v>
       </c>
+      <c r="F418" s="1" t="n">
+        <v>0.0098</v>
+      </c>
+      <c r="G418" s="1" t="n">
+        <v>0.0194</v>
+      </c>
+      <c r="H418" s="1" t="n">
+        <v>0.0327</v>
+      </c>
+      <c r="I418" s="1" t="n">
+        <v>0.0602</v>
+      </c>
+      <c r="J418" s="1" t="n">
+        <v>0.0568</v>
+      </c>
+      <c r="K418" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L418" s="1" t="n">
+        <v>0.0163</v>
+      </c>
+      <c r="M418" s="1" t="n">
+        <v>0.0374</v>
+      </c>
+      <c r="N418" s="1" t="n">
+        <v>0.0764</v>
+      </c>
+      <c r="O418" s="1" t="n">
+        <v>0.0425</v>
+      </c>
       <c r="P418" s="1" t="n">
         <f aca="false">SUM(F418:O418)</f>
-        <v>0</v>
+        <v>0.3515</v>
       </c>
       <c r="R418" s="1" t="n">
         <v>6</v>
@@ -17650,9 +19849,39 @@
       <c r="E419" s="1" t="n">
         <v>3350</v>
       </c>
+      <c r="F419" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G419" s="1" t="n">
+        <v>0.0201</v>
+      </c>
+      <c r="H419" s="1" t="n">
+        <v>0.0392</v>
+      </c>
+      <c r="I419" s="1" t="n">
+        <v>0.0942</v>
+      </c>
+      <c r="J419" s="1" t="n">
+        <v>0.183</v>
+      </c>
+      <c r="K419" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L419" s="1" t="n">
+        <v>0.0166</v>
+      </c>
+      <c r="M419" s="1" t="n">
+        <v>0.0437</v>
+      </c>
+      <c r="N419" s="1" t="n">
+        <v>0.1022</v>
+      </c>
+      <c r="O419" s="1" t="n">
+        <v>0.1165</v>
+      </c>
       <c r="P419" s="1" t="n">
         <f aca="false">SUM(F419:O419)</f>
-        <v>0</v>
+        <v>0.6155</v>
       </c>
       <c r="R419" s="1" t="n">
         <v>6</v>
@@ -17695,9 +19924,42 @@
       <c r="E421" s="1" t="n">
         <v>1600</v>
       </c>
+      <c r="F421" s="1" t="n">
+        <v>0.0127</v>
+      </c>
+      <c r="G421" s="1" t="n">
+        <v>0.0281</v>
+      </c>
+      <c r="H421" s="1" t="n">
+        <v>0.0451</v>
+      </c>
+      <c r="I421" s="1" t="n">
+        <v>0.0735</v>
+      </c>
+      <c r="J421" s="1" t="n">
+        <v>0.169</v>
+      </c>
+      <c r="K421" s="1" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L421" s="1" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="M421" s="1" t="n">
+        <v>0.0856</v>
+      </c>
+      <c r="N421" s="1" t="n">
+        <v>0.0922</v>
+      </c>
+      <c r="O421" s="1" t="n">
+        <v>0.0997</v>
+      </c>
       <c r="P421" s="1" t="n">
         <f aca="false">SUM(F421:O421)</f>
-        <v>0</v>
+        <v>0.6429</v>
+      </c>
+      <c r="R421" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="S421" s="1" t="n">
         <v>2</v>
@@ -17713,9 +19975,42 @@
       <c r="C422" s="1" t="n">
         <v>1600</v>
       </c>
+      <c r="F422" s="1" t="n">
+        <v>0.0128</v>
+      </c>
+      <c r="G422" s="1" t="n">
+        <v>0.0257</v>
+      </c>
+      <c r="H422" s="1" t="n">
+        <v>0.0373</v>
+      </c>
+      <c r="I422" s="1" t="n">
+        <v>0.0387</v>
+      </c>
+      <c r="J422" s="1" t="n">
+        <v>0.0419</v>
+      </c>
+      <c r="K422" s="1" t="n">
+        <v>0.0108</v>
+      </c>
+      <c r="L422" s="1" t="n">
+        <v>0.0254</v>
+      </c>
+      <c r="M422" s="1" t="n">
+        <v>0.0777</v>
+      </c>
+      <c r="N422" s="1" t="n">
+        <v>0.0656</v>
+      </c>
+      <c r="O422" s="1" t="n">
+        <v>0.0257</v>
+      </c>
       <c r="P422" s="1" t="n">
         <f aca="false">SUM(F422:O422)</f>
-        <v>0</v>
+        <v>0.3616</v>
+      </c>
+      <c r="R422" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="S422" s="1" t="n">
         <v>1</v>
@@ -17737,9 +20032,42 @@
       <c r="E423" s="1" t="n">
         <v>1850</v>
       </c>
+      <c r="F423" s="1" t="n">
+        <v>0.0707</v>
+      </c>
+      <c r="G423" s="1" t="n">
+        <v>0.0612</v>
+      </c>
+      <c r="H423" s="1" t="n">
+        <v>0.0508</v>
+      </c>
+      <c r="I423" s="1" t="n">
+        <v>0.0426</v>
+      </c>
+      <c r="J423" s="1" t="n">
+        <v>0.0421</v>
+      </c>
+      <c r="K423" s="1" t="n">
+        <v>0.1319</v>
+      </c>
+      <c r="L423" s="1" t="n">
+        <v>0.0679</v>
+      </c>
+      <c r="M423" s="1" t="n">
+        <v>0.0924</v>
+      </c>
+      <c r="N423" s="1" t="n">
+        <v>0.0702</v>
+      </c>
+      <c r="O423" s="1" t="n">
+        <v>0.0265</v>
+      </c>
       <c r="P423" s="1" t="n">
         <f aca="false">SUM(F423:O423)</f>
-        <v>0</v>
+        <v>0.6563</v>
+      </c>
+      <c r="R423" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="S423" s="1" t="n">
         <v>2</v>
@@ -17755,9 +20083,42 @@
       <c r="C424" s="1" t="n">
         <v>1850</v>
       </c>
+      <c r="F424" s="1" t="n">
+        <v>0.0637</v>
+      </c>
+      <c r="G424" s="1" t="n">
+        <v>0.0445</v>
+      </c>
+      <c r="H424" s="1" t="n">
+        <v>0.0208</v>
+      </c>
+      <c r="I424" s="1" t="n">
+        <v>0.0113</v>
+      </c>
+      <c r="J424" s="1" t="n">
+        <v>0.0285</v>
+      </c>
+      <c r="K424" s="1" t="n">
+        <v>0.1244</v>
+      </c>
+      <c r="L424" s="1" t="n">
+        <v>0.0495</v>
+      </c>
+      <c r="M424" s="1" t="n">
+        <v>0.0204</v>
+      </c>
+      <c r="N424" s="1" t="n">
+        <v>0.0118</v>
+      </c>
+      <c r="O424" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P424" s="1" t="n">
         <f aca="false">SUM(F424:O424)</f>
-        <v>0</v>
+        <v>0.3749</v>
+      </c>
+      <c r="R424" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="S424" s="1" t="n">
         <v>1</v>
@@ -17779,9 +20140,39 @@
       <c r="E425" s="1" t="n">
         <v>3350</v>
       </c>
+      <c r="F425" s="1" t="n">
+        <v>0.061</v>
+      </c>
+      <c r="G425" s="1" t="n">
+        <v>0.0441</v>
+      </c>
+      <c r="H425" s="1" t="n">
+        <v>0.0275</v>
+      </c>
+      <c r="I425" s="1" t="n">
+        <v>0.0566</v>
+      </c>
+      <c r="J425" s="1" t="n">
+        <v>0.1757</v>
+      </c>
+      <c r="K425" s="1" t="n">
+        <v>0.1197</v>
+      </c>
+      <c r="L425" s="1" t="n">
+        <v>0.0487</v>
+      </c>
+      <c r="M425" s="1" t="n">
+        <v>0.0274</v>
+      </c>
+      <c r="N425" s="1" t="n">
+        <v>0.0436</v>
+      </c>
+      <c r="O425" s="1" t="n">
+        <v>0.0942</v>
+      </c>
       <c r="P425" s="1" t="n">
         <f aca="false">SUM(F425:O425)</f>
-        <v>0</v>
+        <v>0.6985</v>
       </c>
       <c r="S425" s="1" t="n">
         <v>2</v>
@@ -50035,6 +52426,54 @@
       </c>
       <c r="S2001" s="1" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2007" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2007" s="1" t="n">
+        <v>1930</v>
+      </c>
+      <c r="C2007" s="1" t="n">
+        <v>2100</v>
+      </c>
+      <c r="D2007" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="E2007" s="1" t="n">
+        <v>-2</v>
+      </c>
+      <c r="F2007" s="1" t="n">
+        <v>0.066</v>
+      </c>
+      <c r="G2007" s="1" t="n">
+        <v>0.0445</v>
+      </c>
+      <c r="H2007" s="1" t="n">
+        <v>0.0236</v>
+      </c>
+      <c r="I2007" s="1" t="n">
+        <v>0.0406</v>
+      </c>
+      <c r="J2007" s="1" t="n">
+        <v>0.1471</v>
+      </c>
+      <c r="K2007" s="1" t="n">
+        <v>0.1161</v>
+      </c>
+      <c r="L2007" s="1" t="n">
+        <v>0.0453</v>
+      </c>
+      <c r="M2007" s="1" t="n">
+        <v>0.0237</v>
+      </c>
+      <c r="N2007" s="1" t="n">
+        <v>0.0354</v>
+      </c>
+      <c r="O2007" s="1" t="n">
+        <v>0.0964</v>
+      </c>
+      <c r="P2007" s="1" t="n">
+        <f aca="false">SUM(F2007:O2007)</f>
+        <v>0.6387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
till day 11 morning
</commit_message>
<xml_diff>
--- a/Data acquisition/wing_leakage_data_samples_filt.xlsx
+++ b/Data acquisition/wing_leakage_data_samples_filt.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="42">
   <si>
     <t xml:space="preserve">sample_number</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t xml:space="preserve">residual flow of 0.010 in mfc7 and 0.0173 in mfc10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">observed residual leakage of 0.0167 in mfc10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">residual flow of 0.0161 in mfc10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">residual flow of 0.0152 in mfc10</t>
   </si>
 </sst>
 </file>
@@ -332,8 +341,8 @@
   </sheetPr>
   <dimension ref="A1:S2008"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A665" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F699" activeCellId="0" sqref="F699"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C719" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q748" activeCellId="0" sqref="Q748"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -349,9 +358,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="4.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="19" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="16.05"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="20" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15797,7 +15807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" customFormat="false" ht="24.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="329" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="1" t="n">
         <v>327</v>
       </c>
@@ -15908,7 +15918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" customFormat="false" ht="24.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="331" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="1" t="n">
         <v>329</v>
       </c>
@@ -16235,7 +16245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" customFormat="false" ht="24.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="337" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="1" t="n">
         <v>335</v>
       </c>
@@ -20201,7 +20211,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="426" customFormat="false" ht="24.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="426" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="1" t="n">
         <v>424</v>
       </c>
@@ -23690,7 +23700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="507" customFormat="false" ht="24.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="507" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="1" t="n">
         <v>505</v>
       </c>
@@ -24806,7 +24816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="534" customFormat="false" ht="24.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="1" t="n">
         <v>532</v>
       </c>
@@ -24850,6 +24860,9 @@
         <f aca="false">SUM(F534:O534)</f>
         <v>0.38</v>
       </c>
+      <c r="Q534" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="R534" s="1" t="n">
         <v>9</v>
       </c>
@@ -30034,6 +30047,9 @@
         <f aca="false">SUM(F655:O655)</f>
         <v>0.6714</v>
       </c>
+      <c r="Q655" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="R655" s="1" t="n">
         <v>10</v>
       </c>
@@ -31758,9 +31774,39 @@
       <c r="E691" s="1" t="n">
         <v>2100</v>
       </c>
+      <c r="F691" s="1" t="n">
+        <v>0.0637</v>
+      </c>
+      <c r="G691" s="1" t="n">
+        <v>0.042</v>
+      </c>
+      <c r="H691" s="1" t="n">
+        <v>0.0237</v>
+      </c>
+      <c r="I691" s="1" t="n">
+        <v>0.0351</v>
+      </c>
+      <c r="J691" s="1" t="n">
+        <v>0.168</v>
+      </c>
+      <c r="K691" s="1" t="n">
+        <v>0.1169</v>
+      </c>
+      <c r="L691" s="1" t="n">
+        <v>0.0473</v>
+      </c>
+      <c r="M691" s="1" t="n">
+        <v>0.0217</v>
+      </c>
+      <c r="N691" s="1" t="n">
+        <v>0.0294</v>
+      </c>
+      <c r="O691" s="1" t="n">
+        <v>0.0851</v>
+      </c>
       <c r="P691" s="1" t="n">
         <f aca="false">SUM(F691:O691)</f>
-        <v>0</v>
+        <v>0.6329</v>
       </c>
       <c r="R691" s="1" t="n">
         <v>10</v>
@@ -31807,6 +31853,9 @@
         <f aca="false">SUM(F693:O693)</f>
         <v>0</v>
       </c>
+      <c r="Q693" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R693" s="1" t="n">
         <v>10</v>
       </c>
@@ -31852,6 +31901,9 @@
         <f aca="false">SUM(F695:O695)</f>
         <v>0</v>
       </c>
+      <c r="Q695" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R695" s="1" t="n">
         <v>10</v>
       </c>
@@ -31869,9 +31921,39 @@
       <c r="C696" s="1" t="n">
         <v>3850</v>
       </c>
+      <c r="F696" s="1" t="n">
+        <v>0.0112</v>
+      </c>
+      <c r="G696" s="1" t="n">
+        <v>0.0153</v>
+      </c>
+      <c r="H696" s="1" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="I696" s="1" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="J696" s="1" t="n">
+        <v>0.2046</v>
+      </c>
+      <c r="K696" s="1" t="n">
+        <v>0.0111</v>
+      </c>
+      <c r="L696" s="1" t="n">
+        <v>0.0132</v>
+      </c>
+      <c r="M696" s="1" t="n">
+        <v>0.0128</v>
+      </c>
+      <c r="N696" s="1" t="n">
+        <v>0.0238</v>
+      </c>
+      <c r="O696" s="1" t="n">
+        <v>0.0569</v>
+      </c>
       <c r="P696" s="1" t="n">
         <f aca="false">SUM(F696:O696)</f>
-        <v>0</v>
+        <v>0.3969</v>
       </c>
       <c r="R696" s="1" t="n">
         <v>10</v>
@@ -31900,6 +31982,9 @@
         <f aca="false">SUM(F697:O697)</f>
         <v>0</v>
       </c>
+      <c r="Q697" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R697" s="1" t="n">
         <v>10</v>
       </c>
@@ -31921,6 +32006,9 @@
         <f aca="false">SUM(F698:O698)</f>
         <v>0</v>
       </c>
+      <c r="Q698" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R698" s="1" t="n">
         <v>10</v>
       </c>
@@ -31948,6 +32036,9 @@
         <f aca="false">SUM(F699:O699)</f>
         <v>0</v>
       </c>
+      <c r="Q699" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R699" s="1" t="n">
         <v>10</v>
       </c>
@@ -31965,9 +32056,39 @@
       <c r="C700" s="1" t="n">
         <v>2600</v>
       </c>
+      <c r="F700" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G700" s="1" t="n">
+        <v>0.0128</v>
+      </c>
+      <c r="H700" s="1" t="n">
+        <v>0.0228</v>
+      </c>
+      <c r="I700" s="1" t="n">
+        <v>0.0637</v>
+      </c>
+      <c r="J700" s="1" t="n">
+        <v>0.0777</v>
+      </c>
+      <c r="K700" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L700" s="1" t="n">
+        <v>0.0109</v>
+      </c>
+      <c r="M700" s="1" t="n">
+        <v>0.0216</v>
+      </c>
+      <c r="N700" s="1" t="n">
+        <v>0.0651</v>
+      </c>
+      <c r="O700" s="1" t="n">
+        <v>0.0764</v>
+      </c>
       <c r="P700" s="1" t="n">
         <f aca="false">SUM(F700:O700)</f>
-        <v>0</v>
+        <v>0.351</v>
       </c>
       <c r="R700" s="1" t="n">
         <v>10</v>
@@ -31996,6 +32117,9 @@
         <f aca="false">SUM(F701:O701)</f>
         <v>0</v>
       </c>
+      <c r="Q701" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R701" s="1" t="n">
         <v>10</v>
       </c>
@@ -32017,6 +32141,9 @@
         <f aca="false">SUM(F702:O702)</f>
         <v>0</v>
       </c>
+      <c r="Q702" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R702" s="1" t="n">
         <v>10</v>
       </c>
@@ -32044,6 +32171,9 @@
         <f aca="false">SUM(F703:O703)</f>
         <v>0</v>
       </c>
+      <c r="Q703" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R703" s="1" t="n">
         <v>10</v>
       </c>
@@ -32061,9 +32191,39 @@
       <c r="C704" s="1" t="n">
         <v>3600</v>
       </c>
+      <c r="F704" s="1" t="n">
+        <v>0.067</v>
+      </c>
+      <c r="G704" s="1" t="n">
+        <v>0.083</v>
+      </c>
+      <c r="H704" s="1" t="n">
+        <v>0.033</v>
+      </c>
+      <c r="I704" s="1" t="n">
+        <v>0.0128</v>
+      </c>
+      <c r="J704" s="1" t="n">
+        <v>0.0197</v>
+      </c>
+      <c r="K704" s="1" t="n">
+        <v>0.0456</v>
+      </c>
+      <c r="L704" s="1" t="n">
+        <v>0.0438</v>
+      </c>
+      <c r="M704" s="1" t="n">
+        <v>0.0239</v>
+      </c>
+      <c r="N704" s="1" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="O704" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P704" s="1" t="n">
         <f aca="false">SUM(F704:O704)</f>
-        <v>0</v>
+        <v>0.3408</v>
       </c>
       <c r="R704" s="1" t="n">
         <v>10</v>
@@ -32088,9 +32248,39 @@
       <c r="E705" s="1" t="n">
         <v>1350</v>
       </c>
+      <c r="F705" s="1" t="n">
+        <v>0.0678</v>
+      </c>
+      <c r="G705" s="1" t="n">
+        <v>0.0842</v>
+      </c>
+      <c r="H705" s="1" t="n">
+        <v>0.0359</v>
+      </c>
+      <c r="I705" s="1" t="n">
+        <v>0.0269</v>
+      </c>
+      <c r="J705" s="1" t="n">
+        <v>0.0584</v>
+      </c>
+      <c r="K705" s="1" t="n">
+        <v>0.0467</v>
+      </c>
+      <c r="L705" s="1" t="n">
+        <v>0.0451</v>
+      </c>
+      <c r="M705" s="1" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="N705" s="1" t="n">
+        <v>0.033</v>
+      </c>
+      <c r="O705" s="1" t="n">
+        <v>0.2036</v>
+      </c>
       <c r="P705" s="1" t="n">
         <f aca="false">SUM(F705:O705)</f>
-        <v>0</v>
+        <v>0.6296</v>
       </c>
       <c r="R705" s="1" t="n">
         <v>10</v>
@@ -32109,9 +32299,39 @@
       <c r="C706" s="1" t="n">
         <v>1350</v>
       </c>
+      <c r="F706" s="1" t="n">
+        <v>0.0113</v>
+      </c>
+      <c r="G706" s="1" t="n">
+        <v>0.0153</v>
+      </c>
+      <c r="H706" s="1" t="n">
+        <v>0.0153</v>
+      </c>
+      <c r="I706" s="1" t="n">
+        <v>0.0235</v>
+      </c>
+      <c r="J706" s="1" t="n">
+        <v>0.0587</v>
+      </c>
+      <c r="K706" s="1" t="n">
+        <v>0.0113</v>
+      </c>
+      <c r="L706" s="1" t="n">
+        <v>0.0132</v>
+      </c>
+      <c r="M706" s="1" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="N706" s="1" t="n">
+        <v>0.0294</v>
+      </c>
+      <c r="O706" s="1" t="n">
+        <v>0.2006</v>
+      </c>
       <c r="P706" s="1" t="n">
         <f aca="false">SUM(F706:O706)</f>
-        <v>0</v>
+        <v>0.3916</v>
       </c>
       <c r="R706" s="1" t="n">
         <v>10</v>
@@ -32136,9 +32356,39 @@
       <c r="E707" s="1" t="n">
         <v>1100</v>
       </c>
+      <c r="F707" s="1" t="n">
+        <v>0.0413</v>
+      </c>
+      <c r="G707" s="1" t="n">
+        <v>0.0432</v>
+      </c>
+      <c r="H707" s="1" t="n">
+        <v>0.0288</v>
+      </c>
+      <c r="I707" s="1" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="J707" s="1" t="n">
+        <v>0.0597</v>
+      </c>
+      <c r="K707" s="1" t="n">
+        <v>0.0797</v>
+      </c>
+      <c r="L707" s="1" t="n">
+        <v>0.0928</v>
+      </c>
+      <c r="M707" s="1" t="n">
+        <v>0.033</v>
+      </c>
+      <c r="N707" s="1" t="n">
+        <v>0.0343</v>
+      </c>
+      <c r="O707" s="1" t="n">
+        <v>0.1971</v>
+      </c>
       <c r="P707" s="1" t="n">
         <f aca="false">SUM(F707:O707)</f>
-        <v>0</v>
+        <v>0.6379</v>
       </c>
       <c r="R707" s="1" t="n">
         <v>10</v>
@@ -32238,7 +32488,7 @@
       </c>
     </row>
     <row r="712" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A712" s="1" t="n">
+      <c r="A712" s="4" t="n">
         <v>710</v>
       </c>
       <c r="B712" s="1" t="n">
@@ -32247,9 +32497,39 @@
       <c r="C712" s="1" t="n">
         <v>850</v>
       </c>
+      <c r="F712" s="1" t="n">
+        <v>0.0518</v>
+      </c>
+      <c r="G712" s="1" t="n">
+        <v>0.0386</v>
+      </c>
+      <c r="H712" s="1" t="n">
+        <v>0.0212</v>
+      </c>
+      <c r="I712" s="1" t="n">
+        <v>0.0111</v>
+      </c>
+      <c r="J712" s="1" t="n">
+        <v>0.0195</v>
+      </c>
+      <c r="K712" s="1" t="n">
+        <v>0.165</v>
+      </c>
+      <c r="L712" s="1" t="n">
+        <v>0.0479</v>
+      </c>
+      <c r="M712" s="1" t="n">
+        <v>0.0191</v>
+      </c>
+      <c r="N712" s="1" t="n">
+        <v>0.0106</v>
+      </c>
+      <c r="O712" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P712" s="1" t="n">
         <f aca="false">SUM(F712:O712)</f>
-        <v>0</v>
+        <v>0.3848</v>
       </c>
       <c r="R712" s="1" t="n">
         <v>10</v>
@@ -32274,9 +32554,39 @@
       <c r="E713" s="1" t="n">
         <v>2100</v>
       </c>
+      <c r="F713" s="1" t="n">
+        <v>0.0581</v>
+      </c>
+      <c r="G713" s="1" t="n">
+        <v>0.0577</v>
+      </c>
+      <c r="H713" s="1" t="n">
+        <v>0.0592</v>
+      </c>
+      <c r="I713" s="1" t="n">
+        <v>0.0425</v>
+      </c>
+      <c r="J713" s="1" t="n">
+        <v>0.0288</v>
+      </c>
+      <c r="K713" s="1" t="n">
+        <v>0.1728</v>
+      </c>
+      <c r="L713" s="1" t="n">
+        <v>0.0688</v>
+      </c>
+      <c r="M713" s="1" t="n">
+        <v>0.0809</v>
+      </c>
+      <c r="N713" s="1" t="n">
+        <v>0.0516</v>
+      </c>
+      <c r="O713" s="1" t="n">
+        <v>0.0166</v>
+      </c>
       <c r="P713" s="1" t="n">
         <f aca="false">SUM(F713:O713)</f>
-        <v>0</v>
+        <v>0.637</v>
       </c>
       <c r="R713" s="1" t="n">
         <v>10</v>
@@ -32295,9 +32605,39 @@
       <c r="C714" s="1" t="n">
         <v>2100</v>
       </c>
+      <c r="F714" s="1" t="n">
+        <v>0.0175</v>
+      </c>
+      <c r="G714" s="1" t="n">
+        <v>0.0333</v>
+      </c>
+      <c r="H714" s="1" t="n">
+        <v>0.0501</v>
+      </c>
+      <c r="I714" s="1" t="n">
+        <v>0.0411</v>
+      </c>
+      <c r="J714" s="1" t="n">
+        <v>0.0311</v>
+      </c>
+      <c r="K714" s="1" t="n">
+        <v>0.0173</v>
+      </c>
+      <c r="L714" s="1" t="n">
+        <v>0.0323</v>
+      </c>
+      <c r="M714" s="1" t="n">
+        <v>0.0705</v>
+      </c>
+      <c r="N714" s="1" t="n">
+        <v>0.0495</v>
+      </c>
+      <c r="O714" s="1" t="n">
+        <v>0.0179</v>
+      </c>
       <c r="P714" s="1" t="n">
         <f aca="false">SUM(F714:O714)</f>
-        <v>0</v>
+        <v>0.3606</v>
       </c>
       <c r="R714" s="1" t="n">
         <v>10</v>
@@ -32322,9 +32662,39 @@
       <c r="E715" s="1" t="n">
         <v>4350</v>
       </c>
+      <c r="F715" s="1" t="n">
+        <v>0.0155</v>
+      </c>
+      <c r="G715" s="1" t="n">
+        <v>0.0333</v>
+      </c>
+      <c r="H715" s="1" t="n">
+        <v>0.0568</v>
+      </c>
+      <c r="I715" s="1" t="n">
+        <v>0.0862</v>
+      </c>
+      <c r="J715" s="1" t="n">
+        <v>0.1849</v>
+      </c>
+      <c r="K715" s="1" t="n">
+        <v>0.0146</v>
+      </c>
+      <c r="L715" s="1" t="n">
+        <v>0.0321</v>
+      </c>
+      <c r="M715" s="1" t="n">
+        <v>0.0763</v>
+      </c>
+      <c r="N715" s="1" t="n">
+        <v>0.0702</v>
+      </c>
+      <c r="O715" s="1" t="n">
+        <v>0.0607</v>
+      </c>
       <c r="P715" s="1" t="n">
         <f aca="false">SUM(F715:O715)</f>
-        <v>0</v>
+        <v>0.6306</v>
       </c>
       <c r="R715" s="1" t="n">
         <v>10</v>
@@ -32343,9 +32713,39 @@
       <c r="C716" s="1" t="n">
         <v>4350</v>
       </c>
+      <c r="F716" s="1" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G716" s="1" t="n">
+        <v>0.0156</v>
+      </c>
+      <c r="H716" s="1" t="n">
+        <v>0.0195</v>
+      </c>
+      <c r="I716" s="1" t="n">
+        <v>0.0551</v>
+      </c>
+      <c r="J716" s="1" t="n">
+        <v>0.1728</v>
+      </c>
+      <c r="K716" s="1" t="n">
+        <v>0.009</v>
+      </c>
+      <c r="L716" s="1" t="n">
+        <v>0.0129</v>
+      </c>
+      <c r="M716" s="1" t="n">
+        <v>0.0151</v>
+      </c>
+      <c r="N716" s="1" t="n">
+        <v>0.0291</v>
+      </c>
+      <c r="O716" s="1" t="n">
+        <v>0.0463</v>
+      </c>
       <c r="P716" s="1" t="n">
         <f aca="false">SUM(F716:O716)</f>
-        <v>0</v>
+        <v>0.3854</v>
       </c>
       <c r="R716" s="1" t="n">
         <v>10</v>
@@ -32370,9 +32770,39 @@
       <c r="E717" s="1" t="n">
         <v>350</v>
       </c>
+      <c r="F717" s="1" t="n">
+        <v>0.0298</v>
+      </c>
+      <c r="G717" s="1" t="n">
+        <v>0.0333</v>
+      </c>
+      <c r="H717" s="1" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="I717" s="1" t="n">
+        <v>0.0563</v>
+      </c>
+      <c r="J717" s="1" t="n">
+        <v>0.1721</v>
+      </c>
+      <c r="K717" s="1" t="n">
+        <v>0.0661</v>
+      </c>
+      <c r="L717" s="1" t="n">
+        <v>0.1246</v>
+      </c>
+      <c r="M717" s="1" t="n">
+        <v>0.0311</v>
+      </c>
+      <c r="N717" s="1" t="n">
+        <v>0.0317</v>
+      </c>
+      <c r="O717" s="1" t="n">
+        <v>0.0464</v>
+      </c>
       <c r="P717" s="1" t="n">
         <f aca="false">SUM(F717:O717)</f>
-        <v>0</v>
+        <v>0.6184</v>
       </c>
       <c r="R717" s="1" t="n">
         <v>10</v>
@@ -32391,9 +32821,39 @@
       <c r="C718" s="1" t="n">
         <v>350</v>
       </c>
+      <c r="F718" s="1" t="n">
+        <v>0.0327</v>
+      </c>
+      <c r="G718" s="1" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="H718" s="1" t="n">
+        <v>0.0228</v>
+      </c>
+      <c r="I718" s="1" t="n">
+        <v>0.0133</v>
+      </c>
+      <c r="J718" s="1" t="n">
+        <v>0.0221</v>
+      </c>
+      <c r="K718" s="1" t="n">
+        <v>0.0693</v>
+      </c>
+      <c r="L718" s="1" t="n">
+        <v>0.1256</v>
+      </c>
+      <c r="M718" s="1" t="n">
+        <v>0.0276</v>
+      </c>
+      <c r="N718" s="1" t="n">
+        <v>0.0133</v>
+      </c>
+      <c r="O718" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P718" s="1" t="n">
         <f aca="false">SUM(F718:O718)</f>
-        <v>0</v>
+        <v>0.3617</v>
       </c>
       <c r="R718" s="1" t="n">
         <v>10</v>
@@ -32418,9 +32878,39 @@
       <c r="E719" s="1" t="n">
         <v>350</v>
       </c>
+      <c r="F719" s="1" t="n">
+        <v>0.0649</v>
+      </c>
+      <c r="G719" s="1" t="n">
+        <v>0.0613</v>
+      </c>
+      <c r="H719" s="1" t="n">
+        <v>0.0335</v>
+      </c>
+      <c r="I719" s="1" t="n">
+        <v>0.0139</v>
+      </c>
+      <c r="J719" s="1" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="K719" s="1" t="n">
+        <v>0.1842</v>
+      </c>
+      <c r="L719" s="1" t="n">
+        <v>0.1965</v>
+      </c>
+      <c r="M719" s="1" t="n">
+        <v>0.0426</v>
+      </c>
+      <c r="N719" s="1" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="O719" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P719" s="1" t="n">
         <f aca="false">SUM(F719:O719)</f>
-        <v>0</v>
+        <v>0.6309</v>
       </c>
       <c r="R719" s="1" t="n">
         <v>10</v>
@@ -32439,9 +32929,39 @@
       <c r="C720" s="1" t="n">
         <v>350</v>
       </c>
+      <c r="F720" s="1" t="n">
+        <v>0.0426</v>
+      </c>
+      <c r="G720" s="1" t="n">
+        <v>0.0397</v>
+      </c>
+      <c r="H720" s="1" t="n">
+        <v>0.0237</v>
+      </c>
+      <c r="I720" s="1" t="n">
+        <v>0.0122</v>
+      </c>
+      <c r="J720" s="1" t="n">
+        <v>0.0193</v>
+      </c>
+      <c r="K720" s="1" t="n">
+        <v>0.1251</v>
+      </c>
+      <c r="L720" s="1" t="n">
+        <v>0.0825</v>
+      </c>
+      <c r="M720" s="1" t="n">
+        <v>0.0248</v>
+      </c>
+      <c r="N720" s="1" t="n">
+        <v>0.0122</v>
+      </c>
+      <c r="O720" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P720" s="1" t="n">
         <f aca="false">SUM(F720:O720)</f>
-        <v>0</v>
+        <v>0.3821</v>
       </c>
       <c r="R720" s="1" t="n">
         <v>10</v>
@@ -32470,6 +32990,9 @@
         <f aca="false">SUM(F721:O721)</f>
         <v>0</v>
       </c>
+      <c r="Q721" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R721" s="1" t="n">
         <v>10</v>
       </c>
@@ -32491,6 +33014,9 @@
         <f aca="false">SUM(F722:O722)</f>
         <v>0</v>
       </c>
+      <c r="Q722" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R722" s="1" t="n">
         <v>10</v>
       </c>
@@ -32518,6 +33044,9 @@
         <f aca="false">SUM(F723:O723)</f>
         <v>0</v>
       </c>
+      <c r="Q723" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R723" s="1" t="n">
         <v>10</v>
       </c>
@@ -32559,9 +33088,39 @@
       <c r="E725" s="1" t="n">
         <v>4100</v>
       </c>
+      <c r="F725" s="1" t="n">
+        <v>0.0132</v>
+      </c>
+      <c r="G725" s="1" t="n">
+        <v>0.0243</v>
+      </c>
+      <c r="H725" s="1" t="n">
+        <v>0.0473</v>
+      </c>
+      <c r="I725" s="1" t="n">
+        <v>0.1499</v>
+      </c>
+      <c r="J725" s="1" t="n">
+        <v>0.1513</v>
+      </c>
+      <c r="K725" s="1" t="n">
+        <v>0.0124</v>
+      </c>
+      <c r="L725" s="1" t="n">
+        <v>0.0202</v>
+      </c>
+      <c r="M725" s="1" t="n">
+        <v>0.0415</v>
+      </c>
+      <c r="N725" s="1" t="n">
+        <v>0.0935</v>
+      </c>
+      <c r="O725" s="1" t="n">
+        <v>0.0906</v>
+      </c>
       <c r="P725" s="1" t="n">
         <f aca="false">SUM(F725:O725)</f>
-        <v>0</v>
+        <v>0.6442</v>
       </c>
       <c r="R725" s="1" t="n">
         <v>10</v>
@@ -32580,9 +33139,39 @@
       <c r="C726" s="1" t="n">
         <v>4100</v>
       </c>
+      <c r="F726" s="1" t="n">
+        <v>0.009</v>
+      </c>
+      <c r="G726" s="1" t="n">
+        <v>0.0152</v>
+      </c>
+      <c r="H726" s="1" t="n">
+        <v>0.0225</v>
+      </c>
+      <c r="I726" s="1" t="n">
+        <v>0.0807</v>
+      </c>
+      <c r="J726" s="1" t="n">
+        <v>0.113</v>
+      </c>
+      <c r="K726" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L726" s="1" t="n">
+        <v>0.0123</v>
+      </c>
+      <c r="M726" s="1" t="n">
+        <v>0.0172</v>
+      </c>
+      <c r="N726" s="1" t="n">
+        <v>0.0356</v>
+      </c>
+      <c r="O726" s="1" t="n">
+        <v>0.0483</v>
+      </c>
       <c r="P726" s="1" t="n">
         <f aca="false">SUM(F726:O726)</f>
-        <v>0</v>
+        <v>0.3538</v>
       </c>
       <c r="R726" s="1" t="n">
         <v>10</v>
@@ -32607,9 +33196,39 @@
       <c r="E727" s="1" t="n">
         <v>350</v>
       </c>
+      <c r="F727" s="1" t="n">
+        <v>0.0356</v>
+      </c>
+      <c r="G727" s="1" t="n">
+        <v>0.0388</v>
+      </c>
+      <c r="H727" s="1" t="n">
+        <v>0.0335</v>
+      </c>
+      <c r="I727" s="1" t="n">
+        <v>0.0837</v>
+      </c>
+      <c r="J727" s="1" t="n">
+        <v>0.1134</v>
+      </c>
+      <c r="K727" s="1" t="n">
+        <v>0.0825</v>
+      </c>
+      <c r="L727" s="1" t="n">
+        <v>0.1148</v>
+      </c>
+      <c r="M727" s="1" t="n">
+        <v>0.0353</v>
+      </c>
+      <c r="N727" s="1" t="n">
+        <v>0.0395</v>
+      </c>
+      <c r="O727" s="1" t="n">
+        <v>0.0492</v>
+      </c>
       <c r="P727" s="1" t="n">
         <f aca="false">SUM(F727:O727)</f>
-        <v>0</v>
+        <v>0.6263</v>
       </c>
       <c r="R727" s="1" t="n">
         <v>10</v>
@@ -32652,9 +33271,39 @@
       <c r="E729" s="1" t="n">
         <v>3100</v>
       </c>
+      <c r="F729" s="1" t="n">
+        <v>0.0371</v>
+      </c>
+      <c r="G729" s="1" t="n">
+        <v>0.0401</v>
+      </c>
+      <c r="H729" s="1" t="n">
+        <v>0.0329</v>
+      </c>
+      <c r="I729" s="1" t="n">
+        <v>0.0578</v>
+      </c>
+      <c r="J729" s="1" t="n">
+        <v>0.1113</v>
+      </c>
+      <c r="K729" s="1" t="n">
+        <v>0.0841</v>
+      </c>
+      <c r="L729" s="1" t="n">
+        <v>0.1158</v>
+      </c>
+      <c r="M729" s="1" t="n">
+        <v>0.0365</v>
+      </c>
+      <c r="N729" s="1" t="n">
+        <v>0.0463</v>
+      </c>
+      <c r="O729" s="1" t="n">
+        <v>0.0768</v>
+      </c>
       <c r="P729" s="1" t="n">
         <f aca="false">SUM(F729:O729)</f>
-        <v>0</v>
+        <v>0.6387</v>
       </c>
       <c r="R729" s="1" t="n">
         <v>10</v>
@@ -32673,9 +33322,39 @@
       <c r="C730" s="1" t="n">
         <v>3100</v>
       </c>
+      <c r="F730" s="1" t="n">
+        <v>0.0101</v>
+      </c>
+      <c r="G730" s="1" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="H730" s="1" t="n">
+        <v>0.0197</v>
+      </c>
+      <c r="I730" s="1" t="n">
+        <v>0.0529</v>
+      </c>
+      <c r="J730" s="1" t="n">
+        <v>0.1094</v>
+      </c>
+      <c r="K730" s="1" t="n">
+        <v>0.0092</v>
+      </c>
+      <c r="L730" s="1" t="n">
+        <v>0.0123</v>
+      </c>
+      <c r="M730" s="1" t="n">
+        <v>0.0164</v>
+      </c>
+      <c r="N730" s="1" t="n">
+        <v>0.0407</v>
+      </c>
+      <c r="O730" s="1" t="n">
+        <v>0.0747</v>
+      </c>
       <c r="P730" s="1" t="n">
         <f aca="false">SUM(F730:O730)</f>
-        <v>0</v>
+        <v>0.3604</v>
       </c>
       <c r="R730" s="1" t="n">
         <v>10</v>
@@ -32700,9 +33379,39 @@
       <c r="E731" s="1" t="n">
         <v>3600</v>
       </c>
+      <c r="F731" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G731" s="1" t="n">
+        <v>0.0137</v>
+      </c>
+      <c r="H731" s="1" t="n">
+        <v>0.0271</v>
+      </c>
+      <c r="I731" s="1" t="n">
+        <v>0.1042</v>
+      </c>
+      <c r="J731" s="1" t="n">
+        <v>0.2219</v>
+      </c>
+      <c r="K731" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L731" s="1" t="n">
+        <v>0.0107</v>
+      </c>
+      <c r="M731" s="1" t="n">
+        <v>0.0235</v>
+      </c>
+      <c r="N731" s="1" t="n">
+        <v>0.0699</v>
+      </c>
+      <c r="O731" s="1" t="n">
+        <v>0.1346</v>
+      </c>
       <c r="P731" s="1" t="n">
         <f aca="false">SUM(F731:O731)</f>
-        <v>0</v>
+        <v>0.6056</v>
       </c>
       <c r="R731" s="1" t="n">
         <v>10</v>
@@ -32721,9 +33430,39 @@
       <c r="C732" s="1" t="n">
         <v>3600</v>
       </c>
+      <c r="F732" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G732" s="1" t="n">
+        <v>0.0121</v>
+      </c>
+      <c r="H732" s="1" t="n">
+        <v>0.0187</v>
+      </c>
+      <c r="I732" s="1" t="n">
+        <v>0.0596</v>
+      </c>
+      <c r="J732" s="1" t="n">
+        <v>0.1322</v>
+      </c>
+      <c r="K732" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L732" s="1" t="n">
+        <v>0.0096</v>
+      </c>
+      <c r="M732" s="1" t="n">
+        <v>0.0147</v>
+      </c>
+      <c r="N732" s="1" t="n">
+        <v>0.0361</v>
+      </c>
+      <c r="O732" s="1" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="P732" s="1" t="n">
         <f aca="false">SUM(F732:O732)</f>
-        <v>0</v>
+        <v>0.3455</v>
       </c>
       <c r="R732" s="1" t="n">
         <v>10</v>
@@ -32752,6 +33491,9 @@
         <f aca="false">SUM(F733:O733)</f>
         <v>0</v>
       </c>
+      <c r="Q733" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R733" s="1" t="n">
         <v>10</v>
       </c>
@@ -32773,6 +33515,9 @@
         <f aca="false">SUM(F734:O734)</f>
         <v>0</v>
       </c>
+      <c r="Q734" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R734" s="1" t="n">
         <v>10</v>
       </c>
@@ -32800,6 +33545,9 @@
         <f aca="false">SUM(F735:O735)</f>
         <v>0</v>
       </c>
+      <c r="Q735" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R735" s="1" t="n">
         <v>10</v>
       </c>
@@ -32817,9 +33565,39 @@
       <c r="C736" s="1" t="n">
         <v>4850</v>
       </c>
+      <c r="F736" s="1" t="n">
+        <v>0.0265</v>
+      </c>
+      <c r="G736" s="1" t="n">
+        <v>0.1649</v>
+      </c>
+      <c r="H736" s="1" t="n">
+        <v>0.0369</v>
+      </c>
+      <c r="I736" s="1" t="n">
+        <v>0.0128</v>
+      </c>
+      <c r="J736" s="1" t="n">
+        <v>0.0209</v>
+      </c>
+      <c r="K736" s="1" t="n">
+        <v>0.0129</v>
+      </c>
+      <c r="L736" s="1" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="M736" s="1" t="n">
+        <v>0.0157</v>
+      </c>
+      <c r="N736" s="1" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="O736" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P736" s="1" t="n">
         <f aca="false">SUM(F736:O736)</f>
-        <v>0</v>
+        <v>0.3216</v>
       </c>
       <c r="R736" s="1" t="n">
         <v>10</v>
@@ -32844,9 +33622,39 @@
       <c r="E737" s="1" t="n">
         <v>3600</v>
       </c>
+      <c r="F737" s="1" t="n">
+        <v>0.0305</v>
+      </c>
+      <c r="G737" s="1" t="n">
+        <v>0.1702</v>
+      </c>
+      <c r="H737" s="1" t="n">
+        <v>0.0532</v>
+      </c>
+      <c r="I737" s="1" t="n">
+        <v>0.0957</v>
+      </c>
+      <c r="J737" s="1" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="K737" s="1" t="n">
+        <v>0.0185</v>
+      </c>
+      <c r="L737" s="1" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="M737" s="1" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N737" s="1" t="n">
+        <v>0.0475</v>
+      </c>
+      <c r="O737" s="1" t="n">
+        <v>0.0521</v>
+      </c>
       <c r="P737" s="1" t="n">
         <f aca="false">SUM(F737:O737)</f>
-        <v>0</v>
+        <v>0.6137</v>
       </c>
       <c r="R737" s="1" t="n">
         <v>10</v>
@@ -32865,9 +33673,39 @@
       <c r="C738" s="1" t="n">
         <v>3600</v>
       </c>
+      <c r="F738" s="1" t="n">
+        <v>0.0093</v>
+      </c>
+      <c r="G738" s="1" t="n">
+        <v>0.0145</v>
+      </c>
+      <c r="H738" s="1" t="n">
+        <v>0.0251</v>
+      </c>
+      <c r="I738" s="1" t="n">
+        <v>0.0904</v>
+      </c>
+      <c r="J738" s="1" t="n">
+        <v>0.089</v>
+      </c>
+      <c r="K738" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L738" s="1" t="n">
+        <v>0.0126</v>
+      </c>
+      <c r="M738" s="1" t="n">
+        <v>0.0197</v>
+      </c>
+      <c r="N738" s="1" t="n">
+        <v>0.0433</v>
+      </c>
+      <c r="O738" s="1" t="n">
+        <v>0.051</v>
+      </c>
       <c r="P738" s="1" t="n">
         <f aca="false">SUM(F738:O738)</f>
-        <v>0</v>
+        <v>0.3549</v>
       </c>
       <c r="R738" s="1" t="n">
         <v>10</v>
@@ -32892,9 +33730,39 @@
       <c r="E739" s="1" t="n">
         <v>2850</v>
       </c>
+      <c r="F739" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G739" s="1" t="n">
+        <v>0.0152</v>
+      </c>
+      <c r="H739" s="1" t="n">
+        <v>0.0359</v>
+      </c>
+      <c r="I739" s="1" t="n">
+        <v>0.1407</v>
+      </c>
+      <c r="J739" s="1" t="n">
+        <v>0.157</v>
+      </c>
+      <c r="K739" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L739" s="1" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="M739" s="1" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="N739" s="1" t="n">
+        <v>0.087</v>
+      </c>
+      <c r="O739" s="1" t="n">
+        <v>0.1222</v>
+      </c>
       <c r="P739" s="1" t="n">
         <f aca="false">SUM(F739:O739)</f>
-        <v>0</v>
+        <v>0.602</v>
       </c>
       <c r="R739" s="1" t="n">
         <v>10</v>
@@ -32913,9 +33781,39 @@
       <c r="C740" s="1" t="n">
         <v>2850</v>
       </c>
+      <c r="F740" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G740" s="1" t="n">
+        <v>0.0133</v>
+      </c>
+      <c r="H740" s="1" t="n">
+        <v>0.0222</v>
+      </c>
+      <c r="I740" s="1" t="n">
+        <v>0.0594</v>
+      </c>
+      <c r="J740" s="1" t="n">
+        <v>0.0888</v>
+      </c>
+      <c r="K740" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L740" s="1" t="n">
+        <v>0.0116</v>
+      </c>
+      <c r="M740" s="1" t="n">
+        <v>0.0195</v>
+      </c>
+      <c r="N740" s="1" t="n">
+        <v>0.0513</v>
+      </c>
+      <c r="O740" s="1" t="n">
+        <v>0.0746</v>
+      </c>
       <c r="P740" s="1" t="n">
         <f aca="false">SUM(F740:O740)</f>
-        <v>0</v>
+        <v>0.3407</v>
       </c>
       <c r="R740" s="1" t="n">
         <v>10</v>
@@ -32940,9 +33838,39 @@
       <c r="E741" s="1" t="n">
         <v>2350</v>
       </c>
+      <c r="F741" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G741" s="1" t="n">
+        <v>0.0192</v>
+      </c>
+      <c r="H741" s="1" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="I741" s="1" t="n">
+        <v>0.1133</v>
+      </c>
+      <c r="J741" s="1" t="n">
+        <v>0.1228</v>
+      </c>
+      <c r="K741" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L741" s="1" t="n">
+        <v>0.0172</v>
+      </c>
+      <c r="M741" s="1" t="n">
+        <v>0.0445</v>
+      </c>
+      <c r="N741" s="1" t="n">
+        <v>0.1229</v>
+      </c>
+      <c r="O741" s="1" t="n">
+        <v>0.1198</v>
+      </c>
       <c r="P741" s="1" t="n">
         <f aca="false">SUM(F741:O741)</f>
-        <v>0</v>
+        <v>0.6027</v>
       </c>
       <c r="R741" s="1" t="n">
         <v>10</v>
@@ -32961,9 +33889,39 @@
       <c r="C742" s="1" t="n">
         <v>2350</v>
       </c>
+      <c r="F742" s="1" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="G742" s="1" t="n">
+        <v>0.0165</v>
+      </c>
+      <c r="H742" s="1" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="I742" s="1" t="n">
+        <v>0.0624</v>
+      </c>
+      <c r="J742" s="1" t="n">
+        <v>0.0542</v>
+      </c>
+      <c r="K742" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L742" s="1" t="n">
+        <v>0.0149</v>
+      </c>
+      <c r="M742" s="1" t="n">
+        <v>0.0322</v>
+      </c>
+      <c r="N742" s="1" t="n">
+        <v>0.0787</v>
+      </c>
+      <c r="O742" s="1" t="n">
+        <v>0.0487</v>
+      </c>
       <c r="P742" s="1" t="n">
         <f aca="false">SUM(F742:O742)</f>
-        <v>0</v>
+        <v>0.3436</v>
       </c>
       <c r="R742" s="1" t="n">
         <v>10</v>
@@ -32988,9 +33946,39 @@
       <c r="E743" s="1" t="n">
         <v>100</v>
       </c>
+      <c r="F743" s="1" t="n">
+        <v>0.0367</v>
+      </c>
+      <c r="G743" s="1" t="n">
+        <v>0.0364</v>
+      </c>
+      <c r="H743" s="1" t="n">
+        <v>0.0393</v>
+      </c>
+      <c r="I743" s="1" t="n">
+        <v>0.0646</v>
+      </c>
+      <c r="J743" s="1" t="n">
+        <v>0.0543</v>
+      </c>
+      <c r="K743" s="1" t="n">
+        <v>0.1533</v>
+      </c>
+      <c r="L743" s="1" t="n">
+        <v>0.0639</v>
+      </c>
+      <c r="M743" s="1" t="n">
+        <v>0.0433</v>
+      </c>
+      <c r="N743" s="1" t="n">
+        <v>0.0814</v>
+      </c>
+      <c r="O743" s="1" t="n">
+        <v>0.0494</v>
+      </c>
       <c r="P743" s="1" t="n">
         <f aca="false">SUM(F743:O743)</f>
-        <v>0</v>
+        <v>0.6226</v>
       </c>
       <c r="R743" s="1" t="n">
         <v>10</v>
@@ -33009,9 +33997,39 @@
       <c r="C744" s="1" t="n">
         <v>100</v>
       </c>
+      <c r="F744" s="1" t="n">
+        <v>0.0366</v>
+      </c>
+      <c r="G744" s="1" t="n">
+        <v>0.0314</v>
+      </c>
+      <c r="H744" s="1" t="n">
+        <v>0.0199</v>
+      </c>
+      <c r="I744" s="1" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="J744" s="1" t="n">
+        <v>0.0215</v>
+      </c>
+      <c r="K744" s="1" t="n">
+        <v>0.1522</v>
+      </c>
+      <c r="L744" s="1" t="n">
+        <v>0.0584</v>
+      </c>
+      <c r="M744" s="1" t="n">
+        <v>0.0195</v>
+      </c>
+      <c r="N744" s="1" t="n">
+        <v>0.0115</v>
+      </c>
+      <c r="O744" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P744" s="1" t="n">
         <f aca="false">SUM(F744:O744)</f>
-        <v>0</v>
+        <v>0.363</v>
       </c>
       <c r="R744" s="1" t="n">
         <v>10</v>
@@ -33036,9 +34054,39 @@
       <c r="E745" s="1" t="n">
         <v>2350</v>
       </c>
+      <c r="F745" s="1" t="n">
+        <v>0.0828</v>
+      </c>
+      <c r="G745" s="1" t="n">
+        <v>0.0808</v>
+      </c>
+      <c r="H745" s="1" t="n">
+        <v>0.0413</v>
+      </c>
+      <c r="I745" s="1" t="n">
+        <v>0.0164</v>
+      </c>
+      <c r="J745" s="1" t="n">
+        <v>0.0196</v>
+      </c>
+      <c r="K745" s="1" t="n">
+        <v>0.2065</v>
+      </c>
+      <c r="L745" s="1" t="n">
+        <v>0.1161</v>
+      </c>
+      <c r="M745" s="1" t="n">
+        <v>0.0423</v>
+      </c>
+      <c r="N745" s="1" t="n">
+        <v>0.0167</v>
+      </c>
+      <c r="O745" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P745" s="1" t="n">
         <f aca="false">SUM(F745:O745)</f>
-        <v>0</v>
+        <v>0.6225</v>
       </c>
       <c r="R745" s="1" t="n">
         <v>10</v>
@@ -33081,10 +34129,41 @@
       <c r="E747" s="1" t="n">
         <v>1100</v>
       </c>
+      <c r="F747" s="1" t="n">
+        <v>0.0984</v>
+      </c>
+      <c r="G747" s="1" t="n">
+        <v>0.087</v>
+      </c>
+      <c r="H747" s="1" t="n">
+        <v>0.0426</v>
+      </c>
+      <c r="I747" s="1" t="n">
+        <v>0.0173</v>
+      </c>
+      <c r="J747" s="1" t="n">
+        <v>0.0203</v>
+      </c>
+      <c r="K747" s="1" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="L747" s="1" t="n">
+        <v>0.1069</v>
+      </c>
+      <c r="M747" s="1" t="n">
+        <v>0.0423</v>
+      </c>
+      <c r="N747" s="1" t="n">
+        <v>0.0173</v>
+      </c>
+      <c r="O747" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P747" s="1" t="n">
         <f aca="false">SUM(F747:O747)</f>
-        <v>0</v>
-      </c>
+        <v>0.6431</v>
+      </c>
+      <c r="Q747" s="0"/>
       <c r="R747" s="1" t="n">
         <v>10</v>
       </c>
@@ -33106,8 +34185,11 @@
         <f aca="false">SUM(F748:O748)</f>
         <v>0</v>
       </c>
+      <c r="Q748" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="R748" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S748" s="1" t="n">
         <v>1</v>
@@ -33134,7 +34216,7 @@
         <v>0</v>
       </c>
       <c r="R749" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S749" s="1" t="n">
         <v>2</v>
@@ -33155,7 +34237,7 @@
         <v>0</v>
       </c>
       <c r="R750" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S750" s="1" t="n">
         <v>1</v>
@@ -33182,7 +34264,7 @@
         <v>0</v>
       </c>
       <c r="R751" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S751" s="1" t="n">
         <v>2</v>
@@ -33203,7 +34285,7 @@
         <v>0</v>
       </c>
       <c r="R752" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S752" s="1" t="n">
         <v>1</v>
@@ -33230,7 +34312,7 @@
         <v>0</v>
       </c>
       <c r="R753" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S753" s="1" t="n">
         <v>2</v>
@@ -33251,7 +34333,7 @@
         <v>0</v>
       </c>
       <c r="R754" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S754" s="1" t="n">
         <v>1</v>
@@ -33278,7 +34360,7 @@
         <v>0</v>
       </c>
       <c r="R755" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S755" s="1" t="n">
         <v>2</v>
@@ -33299,7 +34381,7 @@
         <v>0</v>
       </c>
       <c r="R756" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S756" s="1" t="n">
         <v>1</v>
@@ -33326,7 +34408,7 @@
         <v>0</v>
       </c>
       <c r="R757" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S757" s="1" t="n">
         <v>2</v>
@@ -33347,7 +34429,7 @@
         <v>0</v>
       </c>
       <c r="R758" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S758" s="1" t="n">
         <v>1</v>
@@ -33374,7 +34456,7 @@
         <v>0</v>
       </c>
       <c r="R759" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S759" s="1" t="n">
         <v>2</v>
@@ -33392,7 +34474,7 @@
         <v>28</v>
       </c>
       <c r="R760" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S760" s="1" t="n">
         <v>1</v>
@@ -33419,7 +34501,7 @@
         <v>0</v>
       </c>
       <c r="R761" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S761" s="1" t="n">
         <v>2</v>
@@ -33440,7 +34522,7 @@
         <v>0</v>
       </c>
       <c r="R762" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S762" s="1" t="n">
         <v>1</v>
@@ -33466,6 +34548,9 @@
         <f aca="false">SUM(F763:O763)</f>
         <v>0</v>
       </c>
+      <c r="R763" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S763" s="1" t="n">
         <v>2</v>
       </c>
@@ -33484,6 +34569,9 @@
         <f aca="false">SUM(F764:O764)</f>
         <v>0</v>
       </c>
+      <c r="R764" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S764" s="1" t="n">
         <v>1</v>
       </c>
@@ -33508,6 +34596,9 @@
         <f aca="false">SUM(F765:O765)</f>
         <v>0</v>
       </c>
+      <c r="R765" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S765" s="1" t="n">
         <v>2</v>
       </c>
@@ -33526,6 +34617,9 @@
         <f aca="false">SUM(F766:O766)</f>
         <v>0</v>
       </c>
+      <c r="R766" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S766" s="1" t="n">
         <v>1</v>
       </c>
@@ -33550,6 +34644,9 @@
         <f aca="false">SUM(F767:O767)</f>
         <v>0</v>
       </c>
+      <c r="R767" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S767" s="1" t="n">
         <v>2</v>
       </c>
@@ -33568,6 +34665,9 @@
         <f aca="false">SUM(F768:O768)</f>
         <v>0</v>
       </c>
+      <c r="R768" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S768" s="1" t="n">
         <v>1</v>
       </c>
@@ -33592,6 +34692,9 @@
         <f aca="false">SUM(F769:O769)</f>
         <v>0</v>
       </c>
+      <c r="R769" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S769" s="1" t="n">
         <v>2</v>
       </c>
@@ -33610,6 +34713,9 @@
         <f aca="false">SUM(F770:O770)</f>
         <v>0</v>
       </c>
+      <c r="R770" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S770" s="1" t="n">
         <v>1</v>
       </c>
@@ -33634,6 +34740,9 @@
         <f aca="false">SUM(F771:O771)</f>
         <v>0</v>
       </c>
+      <c r="R771" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S771" s="1" t="n">
         <v>2</v>
       </c>
@@ -33649,6 +34758,9 @@
       <c r="Q772" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="R772" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S772" s="1" t="n">
         <v>1</v>
       </c>
@@ -33673,6 +34785,9 @@
         <f aca="false">SUM(F773:O773)</f>
         <v>0</v>
       </c>
+      <c r="R773" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S773" s="1" t="n">
         <v>2</v>
       </c>
@@ -33691,6 +34806,9 @@
         <f aca="false">SUM(F774:O774)</f>
         <v>0</v>
       </c>
+      <c r="R774" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S774" s="1" t="n">
         <v>1</v>
       </c>
@@ -33715,6 +34833,9 @@
         <f aca="false">SUM(F775:O775)</f>
         <v>0</v>
       </c>
+      <c r="R775" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S775" s="1" t="n">
         <v>2</v>
       </c>
@@ -33733,6 +34854,9 @@
         <f aca="false">SUM(F776:O776)</f>
         <v>0</v>
       </c>
+      <c r="R776" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S776" s="1" t="n">
         <v>1</v>
       </c>
@@ -33757,6 +34881,9 @@
         <f aca="false">SUM(F777:O777)</f>
         <v>0</v>
       </c>
+      <c r="R777" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S777" s="1" t="n">
         <v>2</v>
       </c>
@@ -33775,6 +34902,9 @@
         <f aca="false">SUM(F778:O778)</f>
         <v>0</v>
       </c>
+      <c r="R778" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S778" s="1" t="n">
         <v>1</v>
       </c>
@@ -33799,6 +34929,9 @@
         <f aca="false">SUM(F779:O779)</f>
         <v>0</v>
       </c>
+      <c r="R779" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S779" s="1" t="n">
         <v>2</v>
       </c>
@@ -33817,6 +34950,9 @@
         <f aca="false">SUM(F780:O780)</f>
         <v>0</v>
       </c>
+      <c r="R780" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S780" s="1" t="n">
         <v>1</v>
       </c>
@@ -33841,6 +34977,9 @@
         <f aca="false">SUM(F781:O781)</f>
         <v>0</v>
       </c>
+      <c r="R781" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S781" s="1" t="n">
         <v>2</v>
       </c>
@@ -33856,6 +34995,9 @@
       <c r="Q782" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="R782" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S782" s="1" t="n">
         <v>1</v>
       </c>
@@ -33880,6 +35022,9 @@
         <f aca="false">SUM(F783:O783)</f>
         <v>0</v>
       </c>
+      <c r="R783" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S783" s="1" t="n">
         <v>2</v>
       </c>
@@ -33895,6 +35040,9 @@
       <c r="Q784" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="R784" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S784" s="1" t="n">
         <v>1</v>
       </c>
@@ -33919,6 +35067,9 @@
         <f aca="false">SUM(F785:O785)</f>
         <v>0</v>
       </c>
+      <c r="R785" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S785" s="1" t="n">
         <v>2</v>
       </c>
@@ -33934,6 +35085,9 @@
       <c r="Q786" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="R786" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S786" s="1" t="n">
         <v>1</v>
       </c>
@@ -33958,6 +35112,9 @@
         <f aca="false">SUM(F787:O787)</f>
         <v>0</v>
       </c>
+      <c r="R787" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S787" s="1" t="n">
         <v>2</v>
       </c>
@@ -33973,6 +35130,9 @@
       <c r="Q788" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="R788" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S788" s="1" t="n">
         <v>1</v>
       </c>
@@ -33997,6 +35157,9 @@
         <f aca="false">SUM(F789:O789)</f>
         <v>0</v>
       </c>
+      <c r="R789" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S789" s="1" t="n">
         <v>2</v>
       </c>
@@ -34015,6 +35178,9 @@
         <f aca="false">SUM(F790:O790)</f>
         <v>0</v>
       </c>
+      <c r="R790" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S790" s="1" t="n">
         <v>1</v>
       </c>
@@ -34039,6 +35205,9 @@
         <f aca="false">SUM(F791:O791)</f>
         <v>0</v>
       </c>
+      <c r="R791" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S791" s="1" t="n">
         <v>2</v>
       </c>
@@ -34057,6 +35226,9 @@
         <f aca="false">SUM(F792:O792)</f>
         <v>0</v>
       </c>
+      <c r="R792" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S792" s="1" t="n">
         <v>1</v>
       </c>
@@ -34081,6 +35253,9 @@
         <f aca="false">SUM(F793:O793)</f>
         <v>0</v>
       </c>
+      <c r="R793" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S793" s="1" t="n">
         <v>2</v>
       </c>
@@ -34099,6 +35274,9 @@
         <f aca="false">SUM(F794:O794)</f>
         <v>0</v>
       </c>
+      <c r="R794" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S794" s="1" t="n">
         <v>1</v>
       </c>
@@ -34123,6 +35301,9 @@
         <f aca="false">SUM(F795:O795)</f>
         <v>0</v>
       </c>
+      <c r="R795" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S795" s="1" t="n">
         <v>2</v>
       </c>
@@ -34141,6 +35322,9 @@
         <f aca="false">SUM(F796:O796)</f>
         <v>0</v>
       </c>
+      <c r="R796" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S796" s="1" t="n">
         <v>1</v>
       </c>
@@ -34165,6 +35349,9 @@
         <f aca="false">SUM(F797:O797)</f>
         <v>0</v>
       </c>
+      <c r="R797" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S797" s="1" t="n">
         <v>2</v>
       </c>
@@ -34183,6 +35370,9 @@
         <f aca="false">SUM(F798:O798)</f>
         <v>0</v>
       </c>
+      <c r="R798" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S798" s="1" t="n">
         <v>1</v>
       </c>
@@ -34207,6 +35397,9 @@
         <f aca="false">SUM(F799:O799)</f>
         <v>0</v>
       </c>
+      <c r="R799" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S799" s="1" t="n">
         <v>2</v>
       </c>
@@ -34225,6 +35418,9 @@
         <f aca="false">SUM(F800:O800)</f>
         <v>0</v>
       </c>
+      <c r="R800" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S800" s="1" t="n">
         <v>1</v>
       </c>
@@ -34249,6 +35445,9 @@
         <f aca="false">SUM(F801:O801)</f>
         <v>0</v>
       </c>
+      <c r="R801" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S801" s="1" t="n">
         <v>2</v>
       </c>
@@ -34267,6 +35466,9 @@
         <f aca="false">SUM(F802:O802)</f>
         <v>0</v>
       </c>
+      <c r="R802" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S802" s="1" t="n">
         <v>1</v>
       </c>
@@ -34291,6 +35493,9 @@
         <f aca="false">SUM(F803:O803)</f>
         <v>0</v>
       </c>
+      <c r="R803" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S803" s="1" t="n">
         <v>2</v>
       </c>
@@ -34309,6 +35514,9 @@
         <f aca="false">SUM(F804:O804)</f>
         <v>0</v>
       </c>
+      <c r="R804" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S804" s="1" t="n">
         <v>1</v>
       </c>
@@ -34333,6 +35541,9 @@
         <f aca="false">SUM(F805:O805)</f>
         <v>0</v>
       </c>
+      <c r="R805" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S805" s="1" t="n">
         <v>2</v>
       </c>
@@ -34351,6 +35562,9 @@
         <f aca="false">SUM(F806:O806)</f>
         <v>0</v>
       </c>
+      <c r="R806" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S806" s="1" t="n">
         <v>1</v>
       </c>
@@ -34375,6 +35589,9 @@
         <f aca="false">SUM(F807:O807)</f>
         <v>0</v>
       </c>
+      <c r="R807" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S807" s="1" t="n">
         <v>2</v>
       </c>
@@ -34393,6 +35610,9 @@
         <f aca="false">SUM(F808:O808)</f>
         <v>0</v>
       </c>
+      <c r="R808" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S808" s="1" t="n">
         <v>1</v>
       </c>
@@ -34417,6 +35637,9 @@
         <f aca="false">SUM(F809:O809)</f>
         <v>0</v>
       </c>
+      <c r="R809" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S809" s="1" t="n">
         <v>2</v>
       </c>
@@ -34435,6 +35658,9 @@
         <f aca="false">SUM(F810:O810)</f>
         <v>0</v>
       </c>
+      <c r="R810" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S810" s="1" t="n">
         <v>1</v>
       </c>
@@ -34459,6 +35685,9 @@
         <f aca="false">SUM(F811:O811)</f>
         <v>0</v>
       </c>
+      <c r="R811" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S811" s="1" t="n">
         <v>2</v>
       </c>
@@ -34477,6 +35706,9 @@
         <f aca="false">SUM(F812:O812)</f>
         <v>0</v>
       </c>
+      <c r="R812" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S812" s="1" t="n">
         <v>1</v>
       </c>
@@ -34501,6 +35733,9 @@
         <f aca="false">SUM(F813:O813)</f>
         <v>0</v>
       </c>
+      <c r="R813" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S813" s="1" t="n">
         <v>2</v>
       </c>
@@ -34516,6 +35751,9 @@
       <c r="Q814" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="R814" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S814" s="1" t="n">
         <v>1</v>
       </c>
@@ -34540,6 +35778,9 @@
         <f aca="false">SUM(F815:O815)</f>
         <v>0</v>
       </c>
+      <c r="R815" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S815" s="1" t="n">
         <v>2</v>
       </c>
@@ -34558,6 +35799,9 @@
         <f aca="false">SUM(F816:O816)</f>
         <v>0</v>
       </c>
+      <c r="R816" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S816" s="1" t="n">
         <v>1</v>
       </c>
@@ -34582,6 +35826,9 @@
         <f aca="false">SUM(F817:O817)</f>
         <v>0</v>
       </c>
+      <c r="R817" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S817" s="1" t="n">
         <v>2</v>
       </c>
@@ -34600,6 +35847,9 @@
         <f aca="false">SUM(F818:O818)</f>
         <v>0</v>
       </c>
+      <c r="R818" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S818" s="1" t="n">
         <v>1</v>
       </c>
@@ -34624,6 +35874,9 @@
         <f aca="false">SUM(F819:O819)</f>
         <v>0</v>
       </c>
+      <c r="R819" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S819" s="1" t="n">
         <v>2</v>
       </c>
@@ -34642,6 +35895,9 @@
         <f aca="false">SUM(F820:O820)</f>
         <v>0</v>
       </c>
+      <c r="R820" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S820" s="1" t="n">
         <v>1</v>
       </c>
@@ -34666,6 +35922,9 @@
         <f aca="false">SUM(F821:O821)</f>
         <v>0</v>
       </c>
+      <c r="R821" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S821" s="1" t="n">
         <v>2</v>
       </c>
@@ -34681,6 +35940,9 @@
       <c r="Q822" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="R822" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S822" s="1" t="n">
         <v>1</v>
       </c>
@@ -34705,6 +35967,9 @@
         <f aca="false">SUM(F823:O823)</f>
         <v>0</v>
       </c>
+      <c r="R823" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S823" s="1" t="n">
         <v>2</v>
       </c>
@@ -34723,6 +35988,9 @@
         <f aca="false">SUM(F824:O824)</f>
         <v>0</v>
       </c>
+      <c r="R824" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S824" s="1" t="n">
         <v>1</v>
       </c>
@@ -34747,6 +36015,9 @@
         <f aca="false">SUM(F825:O825)</f>
         <v>0</v>
       </c>
+      <c r="R825" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S825" s="1" t="n">
         <v>2</v>
       </c>
@@ -34765,6 +36036,9 @@
         <f aca="false">SUM(F826:O826)</f>
         <v>0</v>
       </c>
+      <c r="R826" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S826" s="1" t="n">
         <v>1</v>
       </c>
@@ -34789,6 +36063,9 @@
         <f aca="false">SUM(F827:O827)</f>
         <v>0</v>
       </c>
+      <c r="R827" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S827" s="1" t="n">
         <v>2</v>
       </c>
@@ -34804,6 +36081,9 @@
       <c r="Q828" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="R828" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S828" s="1" t="n">
         <v>1</v>
       </c>
@@ -34828,6 +36108,9 @@
         <f aca="false">SUM(F829:O829)</f>
         <v>0</v>
       </c>
+      <c r="R829" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S829" s="1" t="n">
         <v>2</v>
       </c>
@@ -34846,6 +36129,9 @@
         <f aca="false">SUM(F830:O830)</f>
         <v>0</v>
       </c>
+      <c r="R830" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S830" s="1" t="n">
         <v>1</v>
       </c>
@@ -34870,6 +36156,9 @@
         <f aca="false">SUM(F831:O831)</f>
         <v>0</v>
       </c>
+      <c r="R831" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S831" s="1" t="n">
         <v>2</v>
       </c>
@@ -34888,6 +36177,9 @@
         <f aca="false">SUM(F832:O832)</f>
         <v>0</v>
       </c>
+      <c r="R832" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S832" s="1" t="n">
         <v>1</v>
       </c>
@@ -34912,6 +36204,9 @@
         <f aca="false">SUM(F833:O833)</f>
         <v>0</v>
       </c>
+      <c r="R833" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S833" s="1" t="n">
         <v>2</v>
       </c>
@@ -34927,6 +36222,9 @@
       <c r="Q834" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="R834" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S834" s="1" t="n">
         <v>1</v>
       </c>
@@ -34951,6 +36249,9 @@
         <f aca="false">SUM(F835:O835)</f>
         <v>0</v>
       </c>
+      <c r="R835" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S835" s="1" t="n">
         <v>2</v>
       </c>
@@ -34969,6 +36270,9 @@
         <f aca="false">SUM(F836:O836)</f>
         <v>0</v>
       </c>
+      <c r="R836" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S836" s="1" t="n">
         <v>1</v>
       </c>
@@ -34993,6 +36297,9 @@
         <f aca="false">SUM(F837:O837)</f>
         <v>0</v>
       </c>
+      <c r="R837" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S837" s="1" t="n">
         <v>2</v>
       </c>
@@ -35011,6 +36318,9 @@
         <f aca="false">SUM(F838:O838)</f>
         <v>0</v>
       </c>
+      <c r="R838" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S838" s="1" t="n">
         <v>1</v>
       </c>
@@ -35035,6 +36345,9 @@
         <f aca="false">SUM(F839:O839)</f>
         <v>0</v>
       </c>
+      <c r="R839" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="S839" s="1" t="n">
         <v>2</v>
       </c>
@@ -35052,6 +36365,9 @@
       <c r="P840" s="1" t="n">
         <f aca="false">SUM(F840:O840)</f>
         <v>0</v>
+      </c>
+      <c r="R840" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="S840" s="1" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
data preprocess - contour plot
</commit_message>
<xml_diff>
--- a/Data acquisition/wing_leakage_data_samples_filt.xlsx
+++ b/Data acquisition/wing_leakage_data_samples_filt.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="42">
   <si>
     <t xml:space="preserve">sample_number</t>
   </si>
@@ -233,7 +233,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -255,10 +255,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -341,8 +337,8 @@
   </sheetPr>
   <dimension ref="A1:S2008"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C719" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q748" activeCellId="0" sqref="Q748"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A847" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F865" activeCellId="0" sqref="F865:O865"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -358,7 +354,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="27.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="4.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="16.05"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="20" style="1" width="11.53"/>
@@ -31492,7 +31488,7 @@
       </c>
     </row>
     <row r="686" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A686" s="6" t="n">
+      <c r="A686" s="1" t="n">
         <v>684</v>
       </c>
       <c r="B686" s="1" t="n">
@@ -34113,7 +34109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="747" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="747" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A747" s="1" t="n">
         <v>745</v>
       </c>
@@ -34163,7 +34159,6 @@
         <f aca="false">SUM(F747:O747)</f>
         <v>0.6431</v>
       </c>
-      <c r="Q747" s="0"/>
       <c r="R747" s="1" t="n">
         <v>10</v>
       </c>
@@ -34181,9 +34176,39 @@
       <c r="C748" s="1" t="n">
         <v>1100</v>
       </c>
+      <c r="F748" s="1" t="n">
+        <v>0.0496</v>
+      </c>
+      <c r="G748" s="1" t="n">
+        <v>0.0348</v>
+      </c>
+      <c r="H748" s="1" t="n">
+        <v>0.0161</v>
+      </c>
+      <c r="I748" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J748" s="1" t="n">
+        <v>0.0163</v>
+      </c>
+      <c r="K748" s="1" t="n">
+        <v>0.1527</v>
+      </c>
+      <c r="L748" s="1" t="n">
+        <v>0.0456</v>
+      </c>
+      <c r="M748" s="1" t="n">
+        <v>0.0147</v>
+      </c>
+      <c r="N748" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O748" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P748" s="1" t="n">
         <f aca="false">SUM(F748:O748)</f>
-        <v>0</v>
+        <v>0.3298</v>
       </c>
       <c r="Q748" s="2" t="s">
         <v>41</v>
@@ -34211,9 +34236,39 @@
       <c r="E749" s="1" t="n">
         <v>850</v>
       </c>
+      <c r="F749" s="1" t="n">
+        <v>0.0524</v>
+      </c>
+      <c r="G749" s="1" t="n">
+        <v>0.0415</v>
+      </c>
+      <c r="H749" s="1" t="n">
+        <v>0.0303</v>
+      </c>
+      <c r="I749" s="1" t="n">
+        <v>0.0364</v>
+      </c>
+      <c r="J749" s="1" t="n">
+        <v>0.0425</v>
+      </c>
+      <c r="K749" s="1" t="n">
+        <v>0.1557</v>
+      </c>
+      <c r="L749" s="1" t="n">
+        <v>0.0522</v>
+      </c>
+      <c r="M749" s="1" t="n">
+        <v>0.0359</v>
+      </c>
+      <c r="N749" s="1" t="n">
+        <v>0.1397</v>
+      </c>
+      <c r="O749" s="1" t="n">
+        <v>0.0613</v>
+      </c>
       <c r="P749" s="1" t="n">
         <f aca="false">SUM(F749:O749)</f>
-        <v>0</v>
+        <v>0.6479</v>
       </c>
       <c r="R749" s="1" t="n">
         <v>11</v>
@@ -34232,9 +34287,39 @@
       <c r="C750" s="1" t="n">
         <v>850</v>
       </c>
+      <c r="F750" s="1" t="n">
+        <v>0.0103</v>
+      </c>
+      <c r="G750" s="1" t="n">
+        <v>0.0162</v>
+      </c>
+      <c r="H750" s="1" t="n">
+        <v>0.0209</v>
+      </c>
+      <c r="I750" s="1" t="n">
+        <v>0.0336</v>
+      </c>
+      <c r="J750" s="1" t="n">
+        <v>0.0428</v>
+      </c>
+      <c r="K750" s="1" t="n">
+        <v>0.0094</v>
+      </c>
+      <c r="L750" s="1" t="n">
+        <v>0.0144</v>
+      </c>
+      <c r="M750" s="1" t="n">
+        <v>0.0248</v>
+      </c>
+      <c r="N750" s="1" t="n">
+        <v>0.1353</v>
+      </c>
+      <c r="O750" s="1" t="n">
+        <v>0.0599</v>
+      </c>
       <c r="P750" s="1" t="n">
         <f aca="false">SUM(F750:O750)</f>
-        <v>0</v>
+        <v>0.3676</v>
       </c>
       <c r="R750" s="1" t="n">
         <v>11</v>
@@ -34259,9 +34344,39 @@
       <c r="E751" s="1" t="n">
         <v>3100</v>
       </c>
+      <c r="F751" s="1" t="n">
+        <v>0.0137</v>
+      </c>
+      <c r="G751" s="1" t="n">
+        <v>0.0369</v>
+      </c>
+      <c r="H751" s="1" t="n">
+        <v>0.081</v>
+      </c>
+      <c r="I751" s="1" t="n">
+        <v>0.0829</v>
+      </c>
+      <c r="J751" s="1" t="n">
+        <v>0.0585</v>
+      </c>
+      <c r="K751" s="1" t="n">
+        <v>0.0107</v>
+      </c>
+      <c r="L751" s="1" t="n">
+        <v>0.0294</v>
+      </c>
+      <c r="M751" s="1" t="n">
+        <v>0.0668</v>
+      </c>
+      <c r="N751" s="1" t="n">
+        <v>0.1723</v>
+      </c>
+      <c r="O751" s="1" t="n">
+        <v>0.0772</v>
+      </c>
       <c r="P751" s="1" t="n">
         <f aca="false">SUM(F751:O751)</f>
-        <v>0</v>
+        <v>0.6294</v>
       </c>
       <c r="R751" s="1" t="n">
         <v>11</v>
@@ -34280,9 +34395,39 @@
       <c r="C752" s="1" t="n">
         <v>3100</v>
       </c>
+      <c r="F752" s="1" t="n">
+        <v>0.0157</v>
+      </c>
+      <c r="G752" s="1" t="n">
+        <v>0.0348</v>
+      </c>
+      <c r="H752" s="1" t="n">
+        <v>0.0708</v>
+      </c>
+      <c r="I752" s="1" t="n">
+        <v>0.0577</v>
+      </c>
+      <c r="J752" s="1" t="n">
+        <v>0.0343</v>
+      </c>
+      <c r="K752" s="1" t="n">
+        <v>0.0136</v>
+      </c>
+      <c r="L752" s="1" t="n">
+        <v>0.0273</v>
+      </c>
+      <c r="M752" s="1" t="n">
+        <v>0.0498</v>
+      </c>
+      <c r="N752" s="1" t="n">
+        <v>0.0443</v>
+      </c>
+      <c r="O752" s="1" t="n">
+        <v>0.0227</v>
+      </c>
       <c r="P752" s="1" t="n">
         <f aca="false">SUM(F752:O752)</f>
-        <v>0</v>
+        <v>0.371</v>
       </c>
       <c r="R752" s="1" t="n">
         <v>11</v>
@@ -34311,6 +34456,9 @@
         <f aca="false">SUM(F753:O753)</f>
         <v>0</v>
       </c>
+      <c r="Q753" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R753" s="1" t="n">
         <v>11</v>
       </c>
@@ -34332,6 +34480,9 @@
         <f aca="false">SUM(F754:O754)</f>
         <v>0</v>
       </c>
+      <c r="Q754" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R754" s="1" t="n">
         <v>11</v>
       </c>
@@ -34359,6 +34510,9 @@
         <f aca="false">SUM(F755:O755)</f>
         <v>0</v>
       </c>
+      <c r="Q755" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R755" s="1" t="n">
         <v>11</v>
       </c>
@@ -34376,9 +34530,39 @@
       <c r="C756" s="1" t="n">
         <v>4100</v>
       </c>
+      <c r="F756" s="1" t="n">
+        <v>0.0116</v>
+      </c>
+      <c r="G756" s="1" t="n">
+        <v>0.0214</v>
+      </c>
+      <c r="H756" s="1" t="n">
+        <v>0.0418</v>
+      </c>
+      <c r="I756" s="1" t="n">
+        <v>0.1556</v>
+      </c>
+      <c r="J756" s="1" t="n">
+        <v>0.0531</v>
+      </c>
+      <c r="K756" s="1" t="n">
+        <v>0.0101</v>
+      </c>
+      <c r="L756" s="1" t="n">
+        <v>0.0167</v>
+      </c>
+      <c r="M756" s="1" t="n">
+        <v>0.0255</v>
+      </c>
+      <c r="N756" s="1" t="n">
+        <v>0.0386</v>
+      </c>
+      <c r="O756" s="1" t="n">
+        <v>0.0323</v>
+      </c>
       <c r="P756" s="1" t="n">
         <f aca="false">SUM(F756:O756)</f>
-        <v>0</v>
+        <v>0.4067</v>
       </c>
       <c r="R756" s="1" t="n">
         <v>11</v>
@@ -34403,9 +34587,39 @@
       <c r="E757" s="1" t="n">
         <v>4600</v>
       </c>
+      <c r="F757" s="1" t="n">
+        <v>0.0091</v>
+      </c>
+      <c r="G757" s="1" t="n">
+        <v>0.0219</v>
+      </c>
+      <c r="H757" s="1" t="n">
+        <v>0.0549</v>
+      </c>
+      <c r="I757" s="1" t="n">
+        <v>0.2591</v>
+      </c>
+      <c r="J757" s="1" t="n">
+        <v>0.1496</v>
+      </c>
+      <c r="K757" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L757" s="1" t="n">
+        <v>0.0166</v>
+      </c>
+      <c r="M757" s="1" t="n">
+        <v>0.0349</v>
+      </c>
+      <c r="N757" s="1" t="n">
+        <v>0.0691</v>
+      </c>
+      <c r="O757" s="1" t="n">
+        <v>0.079</v>
+      </c>
       <c r="P757" s="1" t="n">
         <f aca="false">SUM(F757:O757)</f>
-        <v>0</v>
+        <v>0.6942</v>
       </c>
       <c r="R757" s="1" t="n">
         <v>11</v>
@@ -34424,9 +34638,39 @@
       <c r="C758" s="1" t="n">
         <v>4600</v>
       </c>
+      <c r="F758" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G758" s="1" t="n">
+        <v>0.0148</v>
+      </c>
+      <c r="H758" s="1" t="n">
+        <v>0.0249</v>
+      </c>
+      <c r="I758" s="1" t="n">
+        <v>0.1136</v>
+      </c>
+      <c r="J758" s="1" t="n">
+        <v>0.1165</v>
+      </c>
+      <c r="K758" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L758" s="1" t="n">
+        <v>0.0119</v>
+      </c>
+      <c r="M758" s="1" t="n">
+        <v>0.0182</v>
+      </c>
+      <c r="N758" s="1" t="n">
+        <v>0.0379</v>
+      </c>
+      <c r="O758" s="1" t="n">
+        <v>0.0522</v>
+      </c>
       <c r="P758" s="1" t="n">
         <f aca="false">SUM(F758:O758)</f>
-        <v>0</v>
+        <v>0.39</v>
       </c>
       <c r="R758" s="1" t="n">
         <v>11</v>
@@ -34455,6 +34699,9 @@
         <f aca="false">SUM(F759:O759)</f>
         <v>0</v>
       </c>
+      <c r="Q759" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R759" s="1" t="n">
         <v>11</v>
       </c>
@@ -34500,6 +34747,9 @@
         <f aca="false">SUM(F761:O761)</f>
         <v>0</v>
       </c>
+      <c r="Q761" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R761" s="1" t="n">
         <v>11</v>
       </c>
@@ -34517,9 +34767,39 @@
       <c r="C762" s="1" t="n">
         <v>4350</v>
       </c>
+      <c r="F762" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G762" s="1" t="n">
+        <v>0.0133</v>
+      </c>
+      <c r="H762" s="1" t="n">
+        <v>0.0261</v>
+      </c>
+      <c r="I762" s="1" t="n">
+        <v>0.1492</v>
+      </c>
+      <c r="J762" s="1" t="n">
+        <v>0.0468</v>
+      </c>
+      <c r="K762" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L762" s="1" t="n">
+        <v>0.0101</v>
+      </c>
+      <c r="M762" s="1" t="n">
+        <v>0.0153</v>
+      </c>
+      <c r="N762" s="1" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="O762" s="1" t="n">
+        <v>0.0244</v>
+      </c>
       <c r="P762" s="1" t="n">
         <f aca="false">SUM(F762:O762)</f>
-        <v>0</v>
+        <v>0.3112</v>
       </c>
       <c r="R762" s="1" t="n">
         <v>11</v>
@@ -34544,9 +34824,39 @@
       <c r="E763" s="1" t="n">
         <v>850</v>
       </c>
+      <c r="F763" s="1" t="n">
+        <v>0.0444</v>
+      </c>
+      <c r="G763" s="1" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="H763" s="1" t="n">
+        <v>0.0371</v>
+      </c>
+      <c r="I763" s="1" t="n">
+        <v>0.1521</v>
+      </c>
+      <c r="J763" s="1" t="n">
+        <v>0.0478</v>
+      </c>
+      <c r="K763" s="1" t="n">
+        <v>0.1537</v>
+      </c>
+      <c r="L763" s="1" t="n">
+        <v>0.054</v>
+      </c>
+      <c r="M763" s="1" t="n">
+        <v>0.0282</v>
+      </c>
+      <c r="N763" s="1" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="O763" s="1" t="n">
+        <v>0.0258</v>
+      </c>
       <c r="P763" s="1" t="n">
         <f aca="false">SUM(F763:O763)</f>
-        <v>0</v>
+        <v>0.6121</v>
       </c>
       <c r="R763" s="1" t="n">
         <v>11</v>
@@ -34565,9 +34875,39 @@
       <c r="C764" s="1" t="n">
         <v>850</v>
       </c>
+      <c r="F764" s="1" t="n">
+        <v>0.0435</v>
+      </c>
+      <c r="G764" s="1" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="H764" s="1" t="n">
+        <v>0.0194</v>
+      </c>
+      <c r="I764" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J764" s="1" t="n">
+        <v>0.0202</v>
+      </c>
+      <c r="K764" s="1" t="n">
+        <v>0.1531</v>
+      </c>
+      <c r="L764" s="1" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="M764" s="1" t="n">
+        <v>0.0182</v>
+      </c>
+      <c r="N764" s="1" t="n">
+        <v>0.0099</v>
+      </c>
+      <c r="O764" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P764" s="1" t="n">
         <f aca="false">SUM(F764:O764)</f>
-        <v>0</v>
+        <v>0.3503</v>
       </c>
       <c r="R764" s="1" t="n">
         <v>11</v>
@@ -34596,6 +34936,9 @@
         <f aca="false">SUM(F765:O765)</f>
         <v>0</v>
       </c>
+      <c r="Q765" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R765" s="1" t="n">
         <v>11</v>
       </c>
@@ -34617,6 +34960,9 @@
         <f aca="false">SUM(F766:O766)</f>
         <v>0</v>
       </c>
+      <c r="Q766" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R766" s="1" t="n">
         <v>11</v>
       </c>
@@ -34644,6 +34990,9 @@
         <f aca="false">SUM(F767:O767)</f>
         <v>0</v>
       </c>
+      <c r="Q767" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R767" s="1" t="n">
         <v>11</v>
       </c>
@@ -34665,6 +35014,9 @@
         <f aca="false">SUM(F768:O768)</f>
         <v>0</v>
       </c>
+      <c r="Q768" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R768" s="1" t="n">
         <v>11</v>
       </c>
@@ -34692,6 +35044,9 @@
         <f aca="false">SUM(F769:O769)</f>
         <v>0</v>
       </c>
+      <c r="Q769" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R769" s="1" t="n">
         <v>11</v>
       </c>
@@ -34709,9 +35064,39 @@
       <c r="C770" s="1" t="n">
         <v>5100</v>
       </c>
+      <c r="F770" s="1" t="n">
+        <v>0.0954</v>
+      </c>
+      <c r="G770" s="1" t="n">
+        <v>0.0854</v>
+      </c>
+      <c r="H770" s="1" t="n">
+        <v>0.0254</v>
+      </c>
+      <c r="I770" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J770" s="1" t="n">
+        <v>0.0177</v>
+      </c>
+      <c r="K770" s="1" t="n">
+        <v>0.0359</v>
+      </c>
+      <c r="L770" s="1" t="n">
+        <v>0.0309</v>
+      </c>
+      <c r="M770" s="1" t="n">
+        <v>0.0166</v>
+      </c>
+      <c r="N770" s="1" t="n">
+        <v>0.0087</v>
+      </c>
+      <c r="O770" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P770" s="1" t="n">
         <f aca="false">SUM(F770:O770)</f>
-        <v>0</v>
+        <v>0.316</v>
       </c>
       <c r="R770" s="1" t="n">
         <v>11</v>
@@ -34736,9 +35121,39 @@
       <c r="E771" s="1" t="n">
         <v>2600</v>
       </c>
+      <c r="F771" s="1" t="n">
+        <v>0.0973</v>
+      </c>
+      <c r="G771" s="1" t="n">
+        <v>0.091</v>
+      </c>
+      <c r="H771" s="1" t="n">
+        <v>0.0413</v>
+      </c>
+      <c r="I771" s="1" t="n">
+        <v>0.0608</v>
+      </c>
+      <c r="J771" s="1" t="n">
+        <v>0.0739</v>
+      </c>
+      <c r="K771" s="1" t="n">
+        <v>0.0378</v>
+      </c>
+      <c r="L771" s="1" t="n">
+        <v>0.0362</v>
+      </c>
+      <c r="M771" s="1" t="n">
+        <v>0.0338</v>
+      </c>
+      <c r="N771" s="1" t="n">
+        <v>0.0647</v>
+      </c>
+      <c r="O771" s="1" t="n">
+        <v>0.0721</v>
+      </c>
       <c r="P771" s="1" t="n">
         <f aca="false">SUM(F771:O771)</f>
-        <v>0</v>
+        <v>0.6089</v>
       </c>
       <c r="R771" s="1" t="n">
         <v>11</v>
@@ -34785,6 +35200,9 @@
         <f aca="false">SUM(F773:O773)</f>
         <v>0</v>
       </c>
+      <c r="Q773" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R773" s="1" t="n">
         <v>11</v>
       </c>
@@ -34806,6 +35224,9 @@
         <f aca="false">SUM(F774:O774)</f>
         <v>0</v>
       </c>
+      <c r="Q774" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R774" s="1" t="n">
         <v>11</v>
       </c>
@@ -34833,6 +35254,9 @@
         <f aca="false">SUM(F775:O775)</f>
         <v>0</v>
       </c>
+      <c r="Q775" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R775" s="1" t="n">
         <v>11</v>
       </c>
@@ -34850,9 +35274,39 @@
       <c r="C776" s="1" t="n">
         <v>600</v>
       </c>
+      <c r="F776" s="1" t="n">
+        <v>0.0131</v>
+      </c>
+      <c r="G776" s="1" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="H776" s="1" t="n">
+        <v>0.0282</v>
+      </c>
+      <c r="I776" s="1" t="n">
+        <v>0.0244</v>
+      </c>
+      <c r="J776" s="1" t="n">
+        <v>0.0287</v>
+      </c>
+      <c r="K776" s="1" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="L776" s="1" t="n">
+        <v>0.0243</v>
+      </c>
+      <c r="M776" s="1" t="n">
+        <v>0.0866</v>
+      </c>
+      <c r="N776" s="1" t="n">
+        <v>0.057</v>
+      </c>
+      <c r="O776" s="1" t="n">
+        <v>0.0196</v>
+      </c>
       <c r="P776" s="1" t="n">
         <f aca="false">SUM(F776:O776)</f>
-        <v>0</v>
+        <v>0.3169</v>
       </c>
       <c r="R776" s="1" t="n">
         <v>11</v>
@@ -34881,6 +35335,9 @@
         <f aca="false">SUM(F777:O777)</f>
         <v>0</v>
       </c>
+      <c r="Q777" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R777" s="1" t="n">
         <v>11</v>
       </c>
@@ -34902,6 +35359,9 @@
         <f aca="false">SUM(F778:O778)</f>
         <v>0</v>
       </c>
+      <c r="Q778" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R778" s="1" t="n">
         <v>11</v>
       </c>
@@ -34929,6 +35389,9 @@
         <f aca="false">SUM(F779:O779)</f>
         <v>0</v>
       </c>
+      <c r="Q779" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R779" s="1" t="n">
         <v>11</v>
       </c>
@@ -34950,6 +35413,9 @@
         <f aca="false">SUM(F780:O780)</f>
         <v>0</v>
       </c>
+      <c r="Q780" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R780" s="1" t="n">
         <v>11</v>
       </c>
@@ -34977,6 +35443,9 @@
         <f aca="false">SUM(F781:O781)</f>
         <v>0</v>
       </c>
+      <c r="Q781" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R781" s="1" t="n">
         <v>11</v>
       </c>
@@ -35018,9 +35487,36 @@
       <c r="E783" s="1" t="n">
         <v>1100</v>
       </c>
+      <c r="F783" s="1" t="n">
+        <v>0.0549</v>
+      </c>
+      <c r="G783" s="1" t="n">
+        <v>0.0931</v>
+      </c>
+      <c r="H783" s="1" t="n">
+        <v>0.0744</v>
+      </c>
+      <c r="I783" s="1" t="n">
+        <v>0.0314</v>
+      </c>
+      <c r="J783" s="1" t="n">
+        <v>0.0265</v>
+      </c>
+      <c r="K783" s="1" t="n">
+        <v>0.0641</v>
+      </c>
+      <c r="L783" s="1" t="n">
+        <v>0.1434</v>
+      </c>
+      <c r="M783" s="1" t="n">
+        <v>0.1097</v>
+      </c>
+      <c r="N783" s="1" t="n">
+        <v>0.0368</v>
+      </c>
       <c r="P783" s="1" t="n">
         <f aca="false">SUM(F783:O783)</f>
-        <v>0</v>
+        <v>0.6343</v>
       </c>
       <c r="R783" s="1" t="n">
         <v>11</v>
@@ -35063,9 +35559,39 @@
       <c r="E785" s="1" t="n">
         <v>1100</v>
       </c>
+      <c r="F785" s="1" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="G785" s="1" t="n">
+        <v>0.053</v>
+      </c>
+      <c r="H785" s="1" t="n">
+        <v>0.0589</v>
+      </c>
+      <c r="I785" s="1" t="n">
+        <v>0.0477</v>
+      </c>
+      <c r="J785" s="1" t="n">
+        <v>0.0403</v>
+      </c>
+      <c r="K785" s="1" t="n">
+        <v>0.0388</v>
+      </c>
+      <c r="L785" s="1" t="n">
+        <v>0.1003</v>
+      </c>
+      <c r="M785" s="1" t="n">
+        <v>0.1251</v>
+      </c>
+      <c r="N785" s="1" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="O785" s="1" t="n">
+        <v>0.0362</v>
+      </c>
       <c r="P785" s="1" t="n">
         <f aca="false">SUM(F785:O785)</f>
-        <v>0</v>
+        <v>0.6483</v>
       </c>
       <c r="R785" s="1" t="n">
         <v>11</v>
@@ -35108,9 +35634,39 @@
       <c r="E787" s="1" t="n">
         <v>2600</v>
       </c>
+      <c r="F787" s="1" t="n">
+        <v>0.0798</v>
+      </c>
+      <c r="G787" s="1" t="n">
+        <v>0.0659</v>
+      </c>
+      <c r="H787" s="1" t="n">
+        <v>0.0489</v>
+      </c>
+      <c r="I787" s="1" t="n">
+        <v>0.0405</v>
+      </c>
+      <c r="J787" s="1" t="n">
+        <v>0.0375</v>
+      </c>
+      <c r="K787" s="1" t="n">
+        <v>0.0926</v>
+      </c>
+      <c r="L787" s="1" t="n">
+        <v>0.0671</v>
+      </c>
+      <c r="M787" s="1" t="n">
+        <v>0.0818</v>
+      </c>
+      <c r="N787" s="1" t="n">
+        <v>0.1055</v>
+      </c>
+      <c r="O787" s="1" t="n">
+        <v>0.0326</v>
+      </c>
       <c r="P787" s="1" t="n">
         <f aca="false">SUM(F787:O787)</f>
-        <v>0</v>
+        <v>0.6522</v>
       </c>
       <c r="R787" s="1" t="n">
         <v>11</v>
@@ -35153,9 +35709,39 @@
       <c r="E789" s="1" t="n">
         <v>2100</v>
       </c>
+      <c r="F789" s="1" t="n">
+        <v>0.0885</v>
+      </c>
+      <c r="G789" s="1" t="n">
+        <v>0.0843</v>
+      </c>
+      <c r="H789" s="1" t="n">
+        <v>0.0706</v>
+      </c>
+      <c r="I789" s="1" t="n">
+        <v>0.0378</v>
+      </c>
+      <c r="J789" s="1" t="n">
+        <v>0.0305</v>
+      </c>
+      <c r="K789" s="1" t="n">
+        <v>0.1019</v>
+      </c>
+      <c r="L789" s="1" t="n">
+        <v>0.087</v>
+      </c>
+      <c r="M789" s="1" t="n">
+        <v>0.0924</v>
+      </c>
+      <c r="N789" s="1" t="n">
+        <v>0.0445</v>
+      </c>
+      <c r="O789" s="1" t="n">
+        <v>0.0192</v>
+      </c>
       <c r="P789" s="1" t="n">
         <f aca="false">SUM(F789:O789)</f>
-        <v>0</v>
+        <v>0.6567</v>
       </c>
       <c r="R789" s="1" t="n">
         <v>11</v>
@@ -35174,9 +35760,39 @@
       <c r="C790" s="1" t="n">
         <v>2100</v>
       </c>
+      <c r="F790" s="1" t="n">
+        <v>0.0195</v>
+      </c>
+      <c r="G790" s="1" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="H790" s="1" t="n">
+        <v>0.0526</v>
+      </c>
+      <c r="I790" s="1" t="n">
+        <v>0.0316</v>
+      </c>
+      <c r="J790" s="1" t="n">
+        <v>0.0281</v>
+      </c>
+      <c r="K790" s="1" t="n">
+        <v>0.0189</v>
+      </c>
+      <c r="L790" s="1" t="n">
+        <v>0.0404</v>
+      </c>
+      <c r="M790" s="1" t="n">
+        <v>0.0748</v>
+      </c>
+      <c r="N790" s="1" t="n">
+        <v>0.0385</v>
+      </c>
+      <c r="O790" s="1" t="n">
+        <v>0.0166</v>
+      </c>
       <c r="P790" s="1" t="n">
         <f aca="false">SUM(F790:O790)</f>
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="R790" s="1" t="n">
         <v>11</v>
@@ -35201,9 +35817,39 @@
       <c r="E791" s="1" t="n">
         <v>1350</v>
       </c>
+      <c r="F791" s="1" t="n">
+        <v>0.0252</v>
+      </c>
+      <c r="G791" s="1" t="n">
+        <v>0.0536</v>
+      </c>
+      <c r="H791" s="1" t="n">
+        <v>0.0806</v>
+      </c>
+      <c r="I791" s="1" t="n">
+        <v>0.0624</v>
+      </c>
+      <c r="J791" s="1" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="K791" s="1" t="n">
+        <v>0.0251</v>
+      </c>
+      <c r="L791" s="1" t="n">
+        <v>0.0578</v>
+      </c>
+      <c r="M791" s="1" t="n">
+        <v>0.145</v>
+      </c>
+      <c r="N791" s="1" t="n">
+        <v>0.1083</v>
+      </c>
+      <c r="O791" s="1" t="n">
+        <v>0.0382</v>
+      </c>
       <c r="P791" s="1" t="n">
         <f aca="false">SUM(F791:O791)</f>
-        <v>0</v>
+        <v>0.6402</v>
       </c>
       <c r="R791" s="1" t="n">
         <v>11</v>
@@ -35222,9 +35868,39 @@
       <c r="C792" s="1" t="n">
         <v>1350</v>
       </c>
+      <c r="F792" s="1" t="n">
+        <v>0.0136</v>
+      </c>
+      <c r="G792" s="1" t="n">
+        <v>0.0248</v>
+      </c>
+      <c r="H792" s="1" t="n">
+        <v>0.0356</v>
+      </c>
+      <c r="I792" s="1" t="n">
+        <v>0.0346</v>
+      </c>
+      <c r="J792" s="1" t="n">
+        <v>0.0337</v>
+      </c>
+      <c r="K792" s="1" t="n">
+        <v>0.0123</v>
+      </c>
+      <c r="L792" s="1" t="n">
+        <v>0.0253</v>
+      </c>
+      <c r="M792" s="1" t="n">
+        <v>0.0757</v>
+      </c>
+      <c r="N792" s="1" t="n">
+        <v>0.0747</v>
+      </c>
+      <c r="O792" s="1" t="n">
+        <v>0.0255</v>
+      </c>
       <c r="P792" s="1" t="n">
         <f aca="false">SUM(F792:O792)</f>
-        <v>0</v>
+        <v>0.3558</v>
       </c>
       <c r="R792" s="1" t="n">
         <v>11</v>
@@ -35253,6 +35929,9 @@
         <f aca="false">SUM(F793:O793)</f>
         <v>0</v>
       </c>
+      <c r="Q793" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R793" s="1" t="n">
         <v>11</v>
       </c>
@@ -35274,6 +35953,9 @@
         <f aca="false">SUM(F794:O794)</f>
         <v>0</v>
       </c>
+      <c r="Q794" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R794" s="1" t="n">
         <v>11</v>
       </c>
@@ -35301,6 +35983,9 @@
         <f aca="false">SUM(F795:O795)</f>
         <v>0</v>
       </c>
+      <c r="Q795" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R795" s="1" t="n">
         <v>11</v>
       </c>
@@ -35318,9 +36003,39 @@
       <c r="C796" s="1" t="n">
         <v>350</v>
       </c>
+      <c r="F796" s="1" t="n">
+        <v>0.0223</v>
+      </c>
+      <c r="G796" s="1" t="n">
+        <v>0.0342</v>
+      </c>
+      <c r="H796" s="1" t="n">
+        <v>0.0302</v>
+      </c>
+      <c r="I796" s="1" t="n">
+        <v>0.0158</v>
+      </c>
+      <c r="J796" s="1" t="n">
+        <v>0.0231</v>
+      </c>
+      <c r="K796" s="1" t="n">
+        <v>0.0285</v>
+      </c>
+      <c r="L796" s="1" t="n">
+        <v>0.1052</v>
+      </c>
+      <c r="M796" s="1" t="n">
+        <v>0.0725</v>
+      </c>
+      <c r="N796" s="1" t="n">
+        <v>0.0208</v>
+      </c>
+      <c r="O796" s="1" t="n">
+        <v>0.0102</v>
+      </c>
       <c r="P796" s="1" t="n">
         <f aca="false">SUM(F796:O796)</f>
-        <v>0</v>
+        <v>0.3628</v>
       </c>
       <c r="R796" s="1" t="n">
         <v>11</v>
@@ -35345,9 +36060,39 @@
       <c r="E797" s="1" t="n">
         <v>850</v>
       </c>
+      <c r="F797" s="1" t="n">
+        <v>0.0414</v>
+      </c>
+      <c r="G797" s="1" t="n">
+        <v>0.0628</v>
+      </c>
+      <c r="H797" s="1" t="n">
+        <v>0.053</v>
+      </c>
+      <c r="I797" s="1" t="n">
+        <v>0.0251</v>
+      </c>
+      <c r="J797" s="1" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="K797" s="1" t="n">
+        <v>0.0571</v>
+      </c>
+      <c r="L797" s="1" t="n">
+        <v>0.1975</v>
+      </c>
+      <c r="M797" s="1" t="n">
+        <v>0.126</v>
+      </c>
+      <c r="N797" s="1" t="n">
+        <v>0.0336</v>
+      </c>
+      <c r="O797" s="1" t="n">
+        <v>0.0126</v>
+      </c>
       <c r="P797" s="1" t="n">
         <f aca="false">SUM(F797:O797)</f>
-        <v>0</v>
+        <v>0.6331</v>
       </c>
       <c r="R797" s="1" t="n">
         <v>11</v>
@@ -35366,9 +36111,39 @@
       <c r="C798" s="1" t="n">
         <v>850</v>
       </c>
+      <c r="F798" s="1" t="n">
+        <v>0.0277</v>
+      </c>
+      <c r="G798" s="1" t="n">
+        <v>0.0397</v>
+      </c>
+      <c r="H798" s="1" t="n">
+        <v>0.0327</v>
+      </c>
+      <c r="I798" s="1" t="n">
+        <v>0.0165</v>
+      </c>
+      <c r="J798" s="1" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="K798" s="1" t="n">
+        <v>0.0355</v>
+      </c>
+      <c r="L798" s="1" t="n">
+        <v>0.1025</v>
+      </c>
+      <c r="M798" s="1" t="n">
+        <v>0.0607</v>
+      </c>
+      <c r="N798" s="1" t="n">
+        <v>0.0204</v>
+      </c>
+      <c r="O798" s="1" t="n">
+        <v>0.0103</v>
+      </c>
       <c r="P798" s="1" t="n">
         <f aca="false">SUM(F798:O798)</f>
-        <v>0</v>
+        <v>0.369</v>
       </c>
       <c r="R798" s="1" t="n">
         <v>11</v>
@@ -35393,9 +36168,39 @@
       <c r="E799" s="1" t="n">
         <v>4600</v>
       </c>
+      <c r="F799" s="1" t="n">
+        <v>0.0548</v>
+      </c>
+      <c r="G799" s="1" t="n">
+        <v>0.1802</v>
+      </c>
+      <c r="H799" s="1" t="n">
+        <v>0.0796</v>
+      </c>
+      <c r="I799" s="1" t="n">
+        <v>0.0254</v>
+      </c>
+      <c r="J799" s="1" t="n">
+        <v>0.0234</v>
+      </c>
+      <c r="K799" s="1" t="n">
+        <v>0.0518</v>
+      </c>
+      <c r="L799" s="1" t="n">
+        <v>0.1246</v>
+      </c>
+      <c r="M799" s="1" t="n">
+        <v>0.0784</v>
+      </c>
+      <c r="N799" s="1" t="n">
+        <v>0.0273</v>
+      </c>
+      <c r="O799" s="1" t="n">
+        <v>0.0112</v>
+      </c>
       <c r="P799" s="1" t="n">
         <f aca="false">SUM(F799:O799)</f>
-        <v>0</v>
+        <v>0.6567</v>
       </c>
       <c r="R799" s="1" t="n">
         <v>11</v>
@@ -35414,9 +36219,39 @@
       <c r="C800" s="1" t="n">
         <v>4600</v>
       </c>
+      <c r="F800" s="1" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G800" s="1" t="n">
+        <v>0.1548</v>
+      </c>
+      <c r="H800" s="1" t="n">
+        <v>0.0595</v>
+      </c>
+      <c r="I800" s="1" t="n">
+        <v>0.0178</v>
+      </c>
+      <c r="J800" s="1" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="K800" s="1" t="n">
+        <v>0.0289</v>
+      </c>
+      <c r="L800" s="1" t="n">
+        <v>0.0346</v>
+      </c>
+      <c r="M800" s="1" t="n">
+        <v>0.0271</v>
+      </c>
+      <c r="N800" s="1" t="n">
+        <v>0.0164</v>
+      </c>
+      <c r="O800" s="1" t="n">
+        <v>0.0097</v>
+      </c>
       <c r="P800" s="1" t="n">
         <f aca="false">SUM(F800:O800)</f>
-        <v>0</v>
+        <v>0.4118</v>
       </c>
       <c r="R800" s="1" t="n">
         <v>11</v>
@@ -35441,9 +36276,39 @@
       <c r="E801" s="1" t="n">
         <v>4600</v>
       </c>
+      <c r="F801" s="1" t="n">
+        <v>0.0832</v>
+      </c>
+      <c r="G801" s="1" t="n">
+        <v>0.2678</v>
+      </c>
+      <c r="H801" s="1" t="n">
+        <v>0.0812</v>
+      </c>
+      <c r="I801" s="1" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="J801" s="1" t="n">
+        <v>0.0218</v>
+      </c>
+      <c r="K801" s="1" t="n">
+        <v>0.0479</v>
+      </c>
+      <c r="L801" s="1" t="n">
+        <v>0.0542</v>
+      </c>
+      <c r="M801" s="1" t="n">
+        <v>0.0379</v>
+      </c>
+      <c r="N801" s="1" t="n">
+        <v>0.0189</v>
+      </c>
+      <c r="O801" s="1" t="n">
+        <v>0.0087</v>
+      </c>
       <c r="P801" s="1" t="n">
         <f aca="false">SUM(F801:O801)</f>
-        <v>0</v>
+        <v>0.6426</v>
       </c>
       <c r="R801" s="1" t="n">
         <v>11</v>
@@ -35462,9 +36327,39 @@
       <c r="C802" s="1" t="n">
         <v>4600</v>
       </c>
+      <c r="F802" s="1" t="n">
+        <v>0.0581</v>
+      </c>
+      <c r="G802" s="1" t="n">
+        <v>0.1311</v>
+      </c>
+      <c r="H802" s="1" t="n">
+        <v>0.0368</v>
+      </c>
+      <c r="I802" s="1" t="n">
+        <v>0.0138</v>
+      </c>
+      <c r="J802" s="1" t="n">
+        <v>0.0215</v>
+      </c>
+      <c r="K802" s="1" t="n">
+        <v>0.0344</v>
+      </c>
+      <c r="L802" s="1" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="M802" s="1" t="n">
+        <v>0.0347</v>
+      </c>
+      <c r="N802" s="1" t="n">
+        <v>0.0137</v>
+      </c>
+      <c r="O802" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P802" s="1" t="n">
         <f aca="false">SUM(F802:O802)</f>
-        <v>0</v>
+        <v>0.3791</v>
       </c>
       <c r="R802" s="1" t="n">
         <v>11</v>
@@ -35489,9 +36384,39 @@
       <c r="E803" s="1" t="n">
         <v>2100</v>
       </c>
+      <c r="F803" s="1" t="n">
+        <v>0.0995</v>
+      </c>
+      <c r="G803" s="1" t="n">
+        <v>0.1733</v>
+      </c>
+      <c r="H803" s="1" t="n">
+        <v>0.0572</v>
+      </c>
+      <c r="I803" s="1" t="n">
+        <v>0.0197</v>
+      </c>
+      <c r="J803" s="1" t="n">
+        <v>0.0226</v>
+      </c>
+      <c r="K803" s="1" t="n">
+        <v>0.0917</v>
+      </c>
+      <c r="L803" s="1" t="n">
+        <v>0.0986</v>
+      </c>
+      <c r="M803" s="1" t="n">
+        <v>0.0463</v>
+      </c>
+      <c r="N803" s="1" t="n">
+        <v>0.0202</v>
+      </c>
+      <c r="O803" s="1" t="n">
+        <v>0.0098</v>
+      </c>
       <c r="P803" s="1" t="n">
         <f aca="false">SUM(F803:O803)</f>
-        <v>0</v>
+        <v>0.6389</v>
       </c>
       <c r="R803" s="1" t="n">
         <v>11</v>
@@ -35510,9 +36435,39 @@
       <c r="C804" s="1" t="n">
         <v>2100</v>
       </c>
+      <c r="F804" s="1" t="n">
+        <v>0.0513</v>
+      </c>
+      <c r="G804" s="1" t="n">
+        <v>0.0556</v>
+      </c>
+      <c r="H804" s="1" t="n">
+        <v>0.0313</v>
+      </c>
+      <c r="I804" s="1" t="n">
+        <v>0.0133</v>
+      </c>
+      <c r="J804" s="1" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="K804" s="1" t="n">
+        <v>0.0661</v>
+      </c>
+      <c r="L804" s="1" t="n">
+        <v>0.0739</v>
+      </c>
+      <c r="M804" s="1" t="n">
+        <v>0.0315</v>
+      </c>
+      <c r="N804" s="1" t="n">
+        <v>0.0144</v>
+      </c>
+      <c r="O804" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P804" s="1" t="n">
         <f aca="false">SUM(F804:O804)</f>
-        <v>0</v>
+        <v>0.3584</v>
       </c>
       <c r="R804" s="1" t="n">
         <v>11</v>
@@ -35537,9 +36492,39 @@
       <c r="E805" s="1" t="n">
         <v>1850</v>
       </c>
+      <c r="F805" s="1" t="n">
+        <v>0.0557</v>
+      </c>
+      <c r="G805" s="1" t="n">
+        <v>0.0673</v>
+      </c>
+      <c r="H805" s="1" t="n">
+        <v>0.0577</v>
+      </c>
+      <c r="I805" s="1" t="n">
+        <v>0.053</v>
+      </c>
+      <c r="J805" s="1" t="n">
+        <v>0.0429</v>
+      </c>
+      <c r="K805" s="1" t="n">
+        <v>0.0709</v>
+      </c>
+      <c r="L805" s="1" t="n">
+        <v>0.0863</v>
+      </c>
+      <c r="M805" s="1" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="N805" s="1" t="n">
+        <v>0.0934</v>
+      </c>
+      <c r="O805" s="1" t="n">
+        <v>0.0376</v>
+      </c>
       <c r="P805" s="1" t="n">
         <f aca="false">SUM(F805:O805)</f>
-        <v>0</v>
+        <v>0.6398</v>
       </c>
       <c r="R805" s="1" t="n">
         <v>11</v>
@@ -35558,9 +36543,39 @@
       <c r="C806" s="1" t="n">
         <v>1850</v>
       </c>
+      <c r="F806" s="1" t="n">
+        <v>0.0128</v>
+      </c>
+      <c r="G806" s="1" t="n">
+        <v>0.0219</v>
+      </c>
+      <c r="H806" s="1" t="n">
+        <v>0.0359</v>
+      </c>
+      <c r="I806" s="1" t="n">
+        <v>0.0458</v>
+      </c>
+      <c r="J806" s="1" t="n">
+        <v>0.0408</v>
+      </c>
+      <c r="K806" s="1" t="n">
+        <v>0.0121</v>
+      </c>
+      <c r="L806" s="1" t="n">
+        <v>0.0214</v>
+      </c>
+      <c r="M806" s="1" t="n">
+        <v>0.0502</v>
+      </c>
+      <c r="N806" s="1" t="n">
+        <v>0.0858</v>
+      </c>
+      <c r="O806" s="1" t="n">
+        <v>0.035</v>
+      </c>
       <c r="P806" s="1" t="n">
         <f aca="false">SUM(F806:O806)</f>
-        <v>0</v>
+        <v>0.3617</v>
       </c>
       <c r="R806" s="1" t="n">
         <v>11</v>
@@ -35589,6 +36604,9 @@
         <f aca="false">SUM(F807:O807)</f>
         <v>0</v>
       </c>
+      <c r="Q807" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R807" s="1" t="n">
         <v>11</v>
       </c>
@@ -35610,6 +36628,9 @@
         <f aca="false">SUM(F808:O808)</f>
         <v>0</v>
       </c>
+      <c r="Q808" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R808" s="1" t="n">
         <v>11</v>
       </c>
@@ -35637,6 +36658,9 @@
         <f aca="false">SUM(F809:O809)</f>
         <v>0</v>
       </c>
+      <c r="Q809" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R809" s="1" t="n">
         <v>11</v>
       </c>
@@ -35654,9 +36678,39 @@
       <c r="C810" s="1" t="n">
         <v>3100</v>
       </c>
+      <c r="F810" s="1" t="n">
+        <v>0.0558</v>
+      </c>
+      <c r="G810" s="1" t="n">
+        <v>0.0715</v>
+      </c>
+      <c r="H810" s="1" t="n">
+        <v>0.0341</v>
+      </c>
+      <c r="I810" s="1" t="n">
+        <v>0.0127</v>
+      </c>
+      <c r="J810" s="1" t="n">
+        <v>0.0208</v>
+      </c>
+      <c r="K810" s="1" t="n">
+        <v>0.0472</v>
+      </c>
+      <c r="L810" s="1" t="n">
+        <v>0.0515</v>
+      </c>
+      <c r="M810" s="1" t="n">
+        <v>0.0272</v>
+      </c>
+      <c r="N810" s="1" t="n">
+        <v>0.0132</v>
+      </c>
+      <c r="O810" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P810" s="1" t="n">
         <f aca="false">SUM(F810:O810)</f>
-        <v>0</v>
+        <v>0.334</v>
       </c>
       <c r="R810" s="1" t="n">
         <v>11</v>
@@ -35681,9 +36735,39 @@
       <c r="E811" s="1" t="n">
         <v>3350</v>
       </c>
+      <c r="F811" s="1" t="n">
+        <v>0.0578</v>
+      </c>
+      <c r="G811" s="1" t="n">
+        <v>0.076</v>
+      </c>
+      <c r="H811" s="1" t="n">
+        <v>0.0456</v>
+      </c>
+      <c r="I811" s="1" t="n">
+        <v>0.0644</v>
+      </c>
+      <c r="J811" s="1" t="n">
+        <v>0.1295</v>
+      </c>
+      <c r="K811" s="1" t="n">
+        <v>0.0495</v>
+      </c>
+      <c r="L811" s="1" t="n">
+        <v>0.0555</v>
+      </c>
+      <c r="M811" s="1" t="n">
+        <v>0.0382</v>
+      </c>
+      <c r="N811" s="1" t="n">
+        <v>0.0475</v>
+      </c>
+      <c r="O811" s="1" t="n">
+        <v>0.0782</v>
+      </c>
       <c r="P811" s="1" t="n">
         <f aca="false">SUM(F811:O811)</f>
-        <v>0</v>
+        <v>0.6422</v>
       </c>
       <c r="R811" s="1" t="n">
         <v>11</v>
@@ -35702,9 +36786,39 @@
       <c r="C812" s="1" t="n">
         <v>3350</v>
       </c>
+      <c r="F812" s="1" t="n">
+        <v>0.0087</v>
+      </c>
+      <c r="G812" s="1" t="n">
+        <v>0.0132</v>
+      </c>
+      <c r="H812" s="1" t="n">
+        <v>0.0199</v>
+      </c>
+      <c r="I812" s="1" t="n">
+        <v>0.0566</v>
+      </c>
+      <c r="J812" s="1" t="n">
+        <v>0.1268</v>
+      </c>
+      <c r="K812" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L812" s="1" t="n">
+        <v>0.0121</v>
+      </c>
+      <c r="M812" s="1" t="n">
+        <v>0.0161</v>
+      </c>
+      <c r="N812" s="1" t="n">
+        <v>0.0397</v>
+      </c>
+      <c r="O812" s="1" t="n">
+        <v>0.0751</v>
+      </c>
       <c r="P812" s="1" t="n">
         <f aca="false">SUM(F812:O812)</f>
-        <v>0</v>
+        <v>0.3682</v>
       </c>
       <c r="R812" s="1" t="n">
         <v>11</v>
@@ -35729,9 +36843,39 @@
       <c r="E813" s="1" t="n">
         <v>100</v>
       </c>
+      <c r="F813" s="1" t="n">
+        <v>0.0188</v>
+      </c>
+      <c r="G813" s="1" t="n">
+        <v>0.0173</v>
+      </c>
+      <c r="H813" s="1" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="I813" s="1" t="n">
+        <v>0.0561</v>
+      </c>
+      <c r="J813" s="1" t="n">
+        <v>0.1266</v>
+      </c>
+      <c r="K813" s="1" t="n">
+        <v>0.196</v>
+      </c>
+      <c r="L813" s="1" t="n">
+        <v>0.0314</v>
+      </c>
+      <c r="M813" s="1" t="n">
+        <v>0.0181</v>
+      </c>
+      <c r="N813" s="1" t="n">
+        <v>0.0395</v>
+      </c>
+      <c r="O813" s="1" t="n">
+        <v>0.0748</v>
+      </c>
       <c r="P813" s="1" t="n">
         <f aca="false">SUM(F813:O813)</f>
-        <v>0</v>
+        <v>0.5986</v>
       </c>
       <c r="R813" s="1" t="n">
         <v>11</v>
@@ -35774,9 +36918,39 @@
       <c r="E815" s="1" t="n">
         <v>850</v>
       </c>
+      <c r="F815" s="1" t="n">
+        <v>0.0651</v>
+      </c>
+      <c r="G815" s="1" t="n">
+        <v>0.0454</v>
+      </c>
+      <c r="H815" s="1" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="I815" s="1" t="n">
+        <v>0.0104</v>
+      </c>
+      <c r="J815" s="1" t="n">
+        <v>0.0222</v>
+      </c>
+      <c r="K815" s="1" t="n">
+        <v>0.3553</v>
+      </c>
+      <c r="L815" s="1" t="n">
+        <v>0.0707</v>
+      </c>
+      <c r="M815" s="1" t="n">
+        <v>0.0228</v>
+      </c>
+      <c r="N815" s="1" t="n">
+        <v>0.0114</v>
+      </c>
+      <c r="O815" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P815" s="1" t="n">
         <f aca="false">SUM(F815:O815)</f>
-        <v>0</v>
+        <v>0.6263</v>
       </c>
       <c r="R815" s="1" t="n">
         <v>11</v>
@@ -35795,9 +36969,39 @@
       <c r="C816" s="1" t="n">
         <v>850</v>
       </c>
+      <c r="F816" s="1" t="n">
+        <v>0.0481</v>
+      </c>
+      <c r="G816" s="1" t="n">
+        <v>0.0344</v>
+      </c>
+      <c r="H816" s="1" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="I816" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J816" s="1" t="n">
+        <v>0.0187</v>
+      </c>
+      <c r="K816" s="1" t="n">
+        <v>0.1611</v>
+      </c>
+      <c r="L816" s="1" t="n">
+        <v>0.0454</v>
+      </c>
+      <c r="M816" s="1" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="N816" s="1" t="n">
+        <v>0.0091</v>
+      </c>
+      <c r="O816" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P816" s="1" t="n">
         <f aca="false">SUM(F816:O816)</f>
-        <v>0</v>
+        <v>0.3528</v>
       </c>
       <c r="R816" s="1" t="n">
         <v>11</v>
@@ -35826,6 +37030,9 @@
         <f aca="false">SUM(F817:O817)</f>
         <v>0</v>
       </c>
+      <c r="Q817" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R817" s="1" t="n">
         <v>11</v>
       </c>
@@ -35847,6 +37054,9 @@
         <f aca="false">SUM(F818:O818)</f>
         <v>0</v>
       </c>
+      <c r="Q818" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R818" s="1" t="n">
         <v>11</v>
       </c>
@@ -35874,6 +37084,9 @@
         <f aca="false">SUM(F819:O819)</f>
         <v>0</v>
       </c>
+      <c r="Q819" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R819" s="1" t="n">
         <v>11</v>
       </c>
@@ -35891,9 +37104,39 @@
       <c r="C820" s="1" t="n">
         <v>1600</v>
       </c>
+      <c r="F820" s="1" t="n">
+        <v>0.0424</v>
+      </c>
+      <c r="G820" s="1" t="n">
+        <v>0.0469</v>
+      </c>
+      <c r="H820" s="1" t="n">
+        <v>0.0283</v>
+      </c>
+      <c r="I820" s="1" t="n">
+        <v>0.0105</v>
+      </c>
+      <c r="J820" s="1" t="n">
+        <v>0.0183</v>
+      </c>
+      <c r="K820" s="1" t="n">
+        <v>0.0617</v>
+      </c>
+      <c r="L820" s="1" t="n">
+        <v>0.0902</v>
+      </c>
+      <c r="M820" s="1" t="n">
+        <v>0.033</v>
+      </c>
+      <c r="N820" s="1" t="n">
+        <v>0.0126</v>
+      </c>
+      <c r="O820" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P820" s="1" t="n">
         <f aca="false">SUM(F820:O820)</f>
-        <v>0</v>
+        <v>0.3439</v>
       </c>
       <c r="R820" s="1" t="n">
         <v>11</v>
@@ -35922,6 +37165,9 @@
         <f aca="false">SUM(F821:O821)</f>
         <v>0</v>
       </c>
+      <c r="Q821" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R821" s="1" t="n">
         <v>11</v>
       </c>
@@ -35967,6 +37213,9 @@
         <f aca="false">SUM(F823:O823)</f>
         <v>0</v>
       </c>
+      <c r="Q823" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R823" s="1" t="n">
         <v>11</v>
       </c>
@@ -35984,9 +37233,39 @@
       <c r="C824" s="1" t="n">
         <v>4600</v>
       </c>
+      <c r="F824" s="1" t="n">
+        <v>0.0133</v>
+      </c>
+      <c r="G824" s="1" t="n">
+        <v>0.0288</v>
+      </c>
+      <c r="H824" s="1" t="n">
+        <v>0.0966</v>
+      </c>
+      <c r="I824" s="1" t="n">
+        <v>0.0698</v>
+      </c>
+      <c r="J824" s="1" t="n">
+        <v>0.0333</v>
+      </c>
+      <c r="K824" s="1" t="n">
+        <v>0.0103</v>
+      </c>
+      <c r="L824" s="1" t="n">
+        <v>0.0199</v>
+      </c>
+      <c r="M824" s="1" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="N824" s="1" t="n">
+        <v>0.0301</v>
+      </c>
+      <c r="O824" s="1" t="n">
+        <v>0.019</v>
+      </c>
       <c r="P824" s="1" t="n">
         <f aca="false">SUM(F824:O824)</f>
-        <v>0</v>
+        <v>0.3501</v>
       </c>
       <c r="R824" s="1" t="n">
         <v>11</v>
@@ -36015,6 +37294,9 @@
         <f aca="false">SUM(F825:O825)</f>
         <v>0</v>
       </c>
+      <c r="Q825" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R825" s="1" t="n">
         <v>11</v>
       </c>
@@ -36036,6 +37318,9 @@
         <f aca="false">SUM(F826:O826)</f>
         <v>0</v>
       </c>
+      <c r="Q826" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R826" s="1" t="n">
         <v>11</v>
       </c>
@@ -36063,6 +37348,9 @@
         <f aca="false">SUM(F827:O827)</f>
         <v>0</v>
       </c>
+      <c r="Q827" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R827" s="1" t="n">
         <v>11</v>
       </c>
@@ -36108,6 +37396,9 @@
         <f aca="false">SUM(F829:O829)</f>
         <v>0</v>
       </c>
+      <c r="Q829" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R829" s="1" t="n">
         <v>11</v>
       </c>
@@ -36129,6 +37420,9 @@
         <f aca="false">SUM(F830:O830)</f>
         <v>0</v>
       </c>
+      <c r="Q830" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R830" s="1" t="n">
         <v>11</v>
       </c>
@@ -36156,6 +37450,9 @@
         <f aca="false">SUM(F831:O831)</f>
         <v>0</v>
       </c>
+      <c r="Q831" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R831" s="1" t="n">
         <v>11</v>
       </c>
@@ -36173,9 +37470,39 @@
       <c r="C832" s="1" t="n">
         <v>600</v>
       </c>
+      <c r="F832" s="1" t="n">
+        <v>0.0123</v>
+      </c>
+      <c r="G832" s="1" t="n">
+        <v>0.0219</v>
+      </c>
+      <c r="H832" s="1" t="n">
+        <v>0.0272</v>
+      </c>
+      <c r="I832" s="1" t="n">
+        <v>0.0198</v>
+      </c>
+      <c r="J832" s="1" t="n">
+        <v>0.0254</v>
+      </c>
+      <c r="K832" s="1" t="n">
+        <v>0.0112</v>
+      </c>
+      <c r="L832" s="1" t="n">
+        <v>0.0344</v>
+      </c>
+      <c r="M832" s="1" t="n">
+        <v>0.1488</v>
+      </c>
+      <c r="N832" s="1" t="n">
+        <v>0.0308</v>
+      </c>
+      <c r="O832" s="1" t="n">
+        <v>0.0138</v>
+      </c>
       <c r="P832" s="1" t="n">
         <f aca="false">SUM(F832:O832)</f>
-        <v>0</v>
+        <v>0.3456</v>
       </c>
       <c r="R832" s="1" t="n">
         <v>11</v>
@@ -36200,9 +37527,39 @@
       <c r="E833" s="1" t="n">
         <v>3100</v>
       </c>
+      <c r="F833" s="1" t="n">
+        <v>0.0825</v>
+      </c>
+      <c r="G833" s="1" t="n">
+        <v>0.0769</v>
+      </c>
+      <c r="H833" s="1" t="n">
+        <v>0.0466</v>
+      </c>
+      <c r="I833" s="1" t="n">
+        <v>0.0241</v>
+      </c>
+      <c r="J833" s="1" t="n">
+        <v>0.0245</v>
+      </c>
+      <c r="K833" s="1" t="n">
+        <v>0.0705</v>
+      </c>
+      <c r="L833" s="1" t="n">
+        <v>0.0775</v>
+      </c>
+      <c r="M833" s="1" t="n">
+        <v>0.1643</v>
+      </c>
+      <c r="N833" s="1" t="n">
+        <v>0.0354</v>
+      </c>
+      <c r="O833" s="1" t="n">
+        <v>0.0138</v>
+      </c>
       <c r="P833" s="1" t="n">
         <f aca="false">SUM(F833:O833)</f>
-        <v>0</v>
+        <v>0.6161</v>
       </c>
       <c r="R833" s="1" t="n">
         <v>11</v>
@@ -36245,9 +37602,39 @@
       <c r="E835" s="1" t="n">
         <v>350</v>
       </c>
+      <c r="F835" s="1" t="n">
+        <v>0.0928</v>
+      </c>
+      <c r="G835" s="1" t="n">
+        <v>0.0856</v>
+      </c>
+      <c r="H835" s="1" t="n">
+        <v>0.0454</v>
+      </c>
+      <c r="I835" s="1" t="n">
+        <v>0.0198</v>
+      </c>
+      <c r="J835" s="1" t="n">
+        <v>0.0236</v>
+      </c>
+      <c r="K835" s="1" t="n">
+        <v>0.0902</v>
+      </c>
+      <c r="L835" s="1" t="n">
+        <v>0.1933</v>
+      </c>
+      <c r="M835" s="1" t="n">
+        <v>0.0604</v>
+      </c>
+      <c r="N835" s="1" t="n">
+        <v>0.0221</v>
+      </c>
+      <c r="O835" s="1" t="n">
+        <v>0.0111</v>
+      </c>
       <c r="P835" s="1" t="n">
         <f aca="false">SUM(F835:O835)</f>
-        <v>0</v>
+        <v>0.6443</v>
       </c>
       <c r="R835" s="1" t="n">
         <v>11</v>
@@ -36266,9 +37653,39 @@
       <c r="C836" s="1" t="n">
         <v>350</v>
       </c>
+      <c r="F836" s="1" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="G836" s="1" t="n">
+        <v>0.0316</v>
+      </c>
+      <c r="H836" s="1" t="n">
+        <v>0.0257</v>
+      </c>
+      <c r="I836" s="1" t="n">
+        <v>0.0136</v>
+      </c>
+      <c r="J836" s="1" t="n">
+        <v>0.0215</v>
+      </c>
+      <c r="K836" s="1" t="n">
+        <v>0.0338</v>
+      </c>
+      <c r="L836" s="1" t="n">
+        <v>0.1505</v>
+      </c>
+      <c r="M836" s="1" t="n">
+        <v>0.0426</v>
+      </c>
+      <c r="N836" s="1" t="n">
+        <v>0.0161</v>
+      </c>
+      <c r="O836" s="1" t="n">
+        <v>0.007</v>
+      </c>
       <c r="P836" s="1" t="n">
         <f aca="false">SUM(F836:O836)</f>
-        <v>0</v>
+        <v>0.3674</v>
       </c>
       <c r="R836" s="1" t="n">
         <v>11</v>
@@ -36297,6 +37714,9 @@
         <f aca="false">SUM(F837:O837)</f>
         <v>0</v>
       </c>
+      <c r="Q837" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R837" s="1" t="n">
         <v>11</v>
       </c>
@@ -36318,6 +37738,9 @@
         <f aca="false">SUM(F838:O838)</f>
         <v>0</v>
       </c>
+      <c r="Q838" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R838" s="1" t="n">
         <v>11</v>
       </c>
@@ -36345,6 +37768,9 @@
         <f aca="false">SUM(F839:O839)</f>
         <v>0</v>
       </c>
+      <c r="Q839" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R839" s="1" t="n">
         <v>11</v>
       </c>
@@ -36366,6 +37792,9 @@
         <f aca="false">SUM(F840:O840)</f>
         <v>0</v>
       </c>
+      <c r="Q840" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R840" s="1" t="n">
         <v>11</v>
       </c>
@@ -36393,6 +37822,9 @@
         <f aca="false">SUM(F841:O841)</f>
         <v>0</v>
       </c>
+      <c r="Q841" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="S841" s="1" t="n">
         <v>2</v>
       </c>
@@ -36407,9 +37839,39 @@
       <c r="C842" s="1" t="n">
         <v>2600</v>
       </c>
+      <c r="F842" s="1" t="n">
+        <v>0.0762</v>
+      </c>
+      <c r="G842" s="1" t="n">
+        <v>0.0448</v>
+      </c>
+      <c r="H842" s="1" t="n">
+        <v>0.0212</v>
+      </c>
+      <c r="I842" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J842" s="1" t="n">
+        <v>0.0184</v>
+      </c>
+      <c r="K842" s="1" t="n">
+        <v>0.109</v>
+      </c>
+      <c r="L842" s="1" t="n">
+        <v>0.0468</v>
+      </c>
+      <c r="M842" s="1" t="n">
+        <v>0.0175</v>
+      </c>
+      <c r="N842" s="1" t="n">
+        <v>0.0091</v>
+      </c>
+      <c r="O842" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P842" s="1" t="n">
         <f aca="false">SUM(F842:O842)</f>
-        <v>0</v>
+        <v>0.343</v>
       </c>
       <c r="S842" s="1" t="n">
         <v>1</v>
@@ -36431,9 +37893,39 @@
       <c r="E843" s="1" t="n">
         <v>1600</v>
       </c>
+      <c r="F843" s="1" t="n">
+        <v>0.0835</v>
+      </c>
+      <c r="G843" s="1" t="n">
+        <v>0.0618</v>
+      </c>
+      <c r="H843" s="1" t="n">
+        <v>0.0527</v>
+      </c>
+      <c r="I843" s="1" t="n">
+        <v>0.041</v>
+      </c>
+      <c r="J843" s="1" t="n">
+        <v>0.0329</v>
+      </c>
+      <c r="K843" s="1" t="n">
+        <v>0.1173</v>
+      </c>
+      <c r="L843" s="1" t="n">
+        <v>0.0666</v>
+      </c>
+      <c r="M843" s="1" t="n">
+        <v>0.0879</v>
+      </c>
+      <c r="N843" s="1" t="n">
+        <v>0.0681</v>
+      </c>
+      <c r="O843" s="1" t="n">
+        <v>0.0253</v>
+      </c>
       <c r="P843" s="1" t="n">
         <f aca="false">SUM(F843:O843)</f>
-        <v>0</v>
+        <v>0.6371</v>
       </c>
       <c r="S843" s="1" t="n">
         <v>2</v>
@@ -36470,9 +37962,39 @@
       <c r="E845" s="1" t="n">
         <v>1600</v>
       </c>
+      <c r="F845" s="1" t="n">
+        <v>0.0641</v>
+      </c>
+      <c r="G845" s="1" t="n">
+        <v>0.0601</v>
+      </c>
+      <c r="H845" s="1" t="n">
+        <v>0.0548</v>
+      </c>
+      <c r="I845" s="1" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="J845" s="1" t="n">
+        <v>0.0354</v>
+      </c>
+      <c r="K845" s="1" t="n">
+        <v>0.1301</v>
+      </c>
+      <c r="L845" s="1" t="n">
+        <v>0.0787</v>
+      </c>
+      <c r="M845" s="1" t="n">
+        <v>0.091</v>
+      </c>
+      <c r="N845" s="1" t="n">
+        <v>0.0698</v>
+      </c>
+      <c r="O845" s="1" t="n">
+        <v>0.027</v>
+      </c>
       <c r="P845" s="1" t="n">
         <f aca="false">SUM(F845:O845)</f>
-        <v>0</v>
+        <v>0.654</v>
       </c>
       <c r="S845" s="1" t="n">
         <v>2</v>
@@ -36488,9 +38010,39 @@
       <c r="C846" s="1" t="n">
         <v>1600</v>
       </c>
+      <c r="F846" s="1" t="n">
+        <v>0.0561</v>
+      </c>
+      <c r="G846" s="1" t="n">
+        <v>0.0422</v>
+      </c>
+      <c r="H846" s="1" t="n">
+        <v>0.0232</v>
+      </c>
+      <c r="I846" s="1" t="n">
+        <v>0.0113</v>
+      </c>
+      <c r="J846" s="1" t="n">
+        <v>0.0214</v>
+      </c>
+      <c r="K846" s="1" t="n">
+        <v>0.1212</v>
+      </c>
+      <c r="L846" s="1" t="n">
+        <v>0.0583</v>
+      </c>
+      <c r="M846" s="1" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="N846" s="1" t="n">
+        <v>0.0118</v>
+      </c>
+      <c r="O846" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P846" s="1" t="n">
         <f aca="false">SUM(F846:O846)</f>
-        <v>0</v>
+        <v>0.3665</v>
       </c>
       <c r="S846" s="1" t="n">
         <v>1</v>
@@ -36512,9 +38064,39 @@
       <c r="E847" s="1" t="n">
         <v>4600</v>
       </c>
+      <c r="F847" s="1" t="n">
+        <v>0.096</v>
+      </c>
+      <c r="G847" s="1" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="H847" s="1" t="n">
+        <v>0.0491</v>
+      </c>
+      <c r="I847" s="1" t="n">
+        <v>0.0159</v>
+      </c>
+      <c r="J847" s="1" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="K847" s="1" t="n">
+        <v>0.1429</v>
+      </c>
+      <c r="L847" s="1" t="n">
+        <v>0.0806</v>
+      </c>
+      <c r="M847" s="1" t="n">
+        <v>0.0341</v>
+      </c>
+      <c r="N847" s="1" t="n">
+        <v>0.0154</v>
+      </c>
+      <c r="O847" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P847" s="1" t="n">
         <f aca="false">SUM(F847:O847)</f>
-        <v>0</v>
+        <v>0.624</v>
       </c>
       <c r="S847" s="1" t="n">
         <v>2</v>
@@ -36530,9 +38112,39 @@
       <c r="C848" s="1" t="n">
         <v>4600</v>
       </c>
+      <c r="F848" s="1" t="n">
+        <v>0.0489</v>
+      </c>
+      <c r="G848" s="1" t="n">
+        <v>0.1383</v>
+      </c>
+      <c r="H848" s="1" t="n">
+        <v>0.0371</v>
+      </c>
+      <c r="I848" s="1" t="n">
+        <v>0.0135</v>
+      </c>
+      <c r="J848" s="1" t="n">
+        <v>0.0205</v>
+      </c>
+      <c r="K848" s="1" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="L848" s="1" t="n">
+        <v>0.0318</v>
+      </c>
+      <c r="M848" s="1" t="n">
+        <v>0.0204</v>
+      </c>
+      <c r="N848" s="1" t="n">
+        <v>0.0127</v>
+      </c>
+      <c r="O848" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P848" s="1" t="n">
         <f aca="false">SUM(F848:O848)</f>
-        <v>0</v>
+        <v>0.3532</v>
       </c>
       <c r="S848" s="1" t="n">
         <v>1</v>
@@ -36554,9 +38166,39 @@
       <c r="E849" s="1" t="n">
         <v>4600</v>
       </c>
+      <c r="F849" s="1" t="n">
+        <v>0.0475</v>
+      </c>
+      <c r="G849" s="1" t="n">
+        <v>0.1402</v>
+      </c>
+      <c r="H849" s="1" t="n">
+        <v>0.0505</v>
+      </c>
+      <c r="I849" s="1" t="n">
+        <v>0.1178</v>
+      </c>
+      <c r="J849" s="1" t="n">
+        <v>0.0962</v>
+      </c>
+      <c r="K849" s="1" t="n">
+        <v>0.0275</v>
+      </c>
+      <c r="L849" s="1" t="n">
+        <v>0.0325</v>
+      </c>
+      <c r="M849" s="1" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N849" s="1" t="n">
+        <v>0.0409</v>
+      </c>
+      <c r="O849" s="1" t="n">
+        <v>0.0482</v>
+      </c>
       <c r="P849" s="1" t="n">
         <f aca="false">SUM(F849:O849)</f>
-        <v>0</v>
+        <v>0.6313</v>
       </c>
       <c r="S849" s="1" t="n">
         <v>2</v>
@@ -36572,9 +38214,39 @@
       <c r="C850" s="1" t="n">
         <v>4600</v>
       </c>
+      <c r="F850" s="1" t="n">
+        <v>0.0093</v>
+      </c>
+      <c r="G850" s="1" t="n">
+        <v>0.0141</v>
+      </c>
+      <c r="H850" s="1" t="n">
+        <v>0.0248</v>
+      </c>
+      <c r="I850" s="1" t="n">
+        <v>0.1116</v>
+      </c>
+      <c r="J850" s="1" t="n">
+        <v>0.0947</v>
+      </c>
+      <c r="K850" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L850" s="1" t="n">
+        <v>0.0125</v>
+      </c>
+      <c r="M850" s="1" t="n">
+        <v>0.0171</v>
+      </c>
+      <c r="N850" s="1" t="n">
+        <v>0.0357</v>
+      </c>
+      <c r="O850" s="1" t="n">
+        <v>0.0462</v>
+      </c>
       <c r="P850" s="1" t="n">
         <f aca="false">SUM(F850:O850)</f>
-        <v>0</v>
+        <v>0.366</v>
       </c>
       <c r="S850" s="1" t="n">
         <v>1</v>
@@ -36600,6 +38272,9 @@
         <f aca="false">SUM(F851:O851)</f>
         <v>0</v>
       </c>
+      <c r="Q851" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="S851" s="1" t="n">
         <v>2</v>
       </c>
@@ -36618,6 +38293,9 @@
         <f aca="false">SUM(F852:O852)</f>
         <v>0</v>
       </c>
+      <c r="Q852" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="S852" s="1" t="n">
         <v>1</v>
       </c>
@@ -36642,6 +38320,9 @@
         <f aca="false">SUM(F853:O853)</f>
         <v>0</v>
       </c>
+      <c r="Q853" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="S853" s="1" t="n">
         <v>2</v>
       </c>
@@ -36656,9 +38337,39 @@
       <c r="C854" s="1" t="n">
         <v>3100</v>
       </c>
+      <c r="F854" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G854" s="1" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="H854" s="1" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="I854" s="1" t="n">
+        <v>0.0534</v>
+      </c>
+      <c r="J854" s="1" t="n">
+        <v>0.0783</v>
+      </c>
+      <c r="K854" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L854" s="1" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M854" s="1" t="n">
+        <v>0.0193</v>
+      </c>
+      <c r="N854" s="1" t="n">
+        <v>0.0647</v>
+      </c>
+      <c r="O854" s="1" t="n">
+        <v>0.087</v>
+      </c>
       <c r="P854" s="1" t="n">
         <f aca="false">SUM(F854:O854)</f>
-        <v>0</v>
+        <v>0.3447</v>
       </c>
       <c r="S854" s="1" t="n">
         <v>1</v>
@@ -36680,9 +38391,39 @@
       <c r="E855" s="1" t="n">
         <v>2350</v>
       </c>
+      <c r="F855" s="1" t="n">
+        <v>0.0265</v>
+      </c>
+      <c r="G855" s="1" t="n">
+        <v>0.0609</v>
+      </c>
+      <c r="H855" s="1" t="n">
+        <v>0.0794</v>
+      </c>
+      <c r="I855" s="1" t="n">
+        <v>0.0794</v>
+      </c>
+      <c r="J855" s="1" t="n">
+        <v>0.0852</v>
+      </c>
+      <c r="K855" s="1" t="n">
+        <v>0.0235</v>
+      </c>
+      <c r="L855" s="1" t="n">
+        <v>0.0445</v>
+      </c>
+      <c r="M855" s="1" t="n">
+        <v>0.0603</v>
+      </c>
+      <c r="N855" s="1" t="n">
+        <v>0.0845</v>
+      </c>
+      <c r="O855" s="1" t="n">
+        <v>0.0951</v>
+      </c>
       <c r="P855" s="1" t="n">
         <f aca="false">SUM(F855:O855)</f>
-        <v>0</v>
+        <v>0.6393</v>
       </c>
       <c r="S855" s="1" t="n">
         <v>2</v>
@@ -36698,9 +38439,39 @@
       <c r="C856" s="1" t="n">
         <v>2350</v>
       </c>
+      <c r="F856" s="1" t="n">
+        <v>0.0257</v>
+      </c>
+      <c r="G856" s="1" t="n">
+        <v>0.0561</v>
+      </c>
+      <c r="H856" s="1" t="n">
+        <v>0.0652</v>
+      </c>
+      <c r="I856" s="1" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="J856" s="1" t="n">
+        <v>0.0258</v>
+      </c>
+      <c r="K856" s="1" t="n">
+        <v>0.0228</v>
+      </c>
+      <c r="L856" s="1" t="n">
+        <v>0.0402</v>
+      </c>
+      <c r="M856" s="1" t="n">
+        <v>0.0441</v>
+      </c>
+      <c r="N856" s="1" t="n">
+        <v>0.0248</v>
+      </c>
+      <c r="O856" s="1" t="n">
+        <v>0.0133</v>
+      </c>
       <c r="P856" s="1" t="n">
         <f aca="false">SUM(F856:O856)</f>
-        <v>0</v>
+        <v>0.345</v>
       </c>
       <c r="S856" s="1" t="n">
         <v>1</v>
@@ -36722,9 +38493,39 @@
       <c r="E857" s="1" t="n">
         <v>2100</v>
       </c>
+      <c r="F857" s="1" t="n">
+        <v>0.086</v>
+      </c>
+      <c r="G857" s="1" t="n">
+        <v>0.0909</v>
+      </c>
+      <c r="H857" s="1" t="n">
+        <v>0.0784</v>
+      </c>
+      <c r="I857" s="1" t="n">
+        <v>0.0309</v>
+      </c>
+      <c r="J857" s="1" t="n">
+        <v>0.0259</v>
+      </c>
+      <c r="K857" s="1" t="n">
+        <v>0.145</v>
+      </c>
+      <c r="L857" s="1" t="n">
+        <v>0.0822</v>
+      </c>
+      <c r="M857" s="1" t="n">
+        <v>0.0581</v>
+      </c>
+      <c r="N857" s="1" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="O857" s="1" t="n">
+        <v>0.0136</v>
+      </c>
       <c r="P857" s="1" t="n">
         <f aca="false">SUM(F857:O857)</f>
-        <v>0</v>
+        <v>0.64</v>
       </c>
       <c r="S857" s="1" t="n">
         <v>2</v>
@@ -36740,9 +38541,39 @@
       <c r="C858" s="1" t="n">
         <v>2100</v>
       </c>
+      <c r="F858" s="1" t="n">
+        <v>0.0656</v>
+      </c>
+      <c r="G858" s="1" t="n">
+        <v>0.041</v>
+      </c>
+      <c r="H858" s="1" t="n">
+        <v>0.0206</v>
+      </c>
+      <c r="I858" s="1" t="n">
+        <v>0.0089</v>
+      </c>
+      <c r="J858" s="1" t="n">
+        <v>0.0195</v>
+      </c>
+      <c r="K858" s="1" t="n">
+        <v>0.1271</v>
+      </c>
+      <c r="L858" s="1" t="n">
+        <v>0.0474</v>
+      </c>
+      <c r="M858" s="1" t="n">
+        <v>0.0175</v>
+      </c>
+      <c r="N858" s="1" t="n">
+        <v>0.0095</v>
+      </c>
+      <c r="O858" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P858" s="1" t="n">
         <f aca="false">SUM(F858:O858)</f>
-        <v>0</v>
+        <v>0.3571</v>
       </c>
       <c r="S858" s="1" t="n">
         <v>1</v>
@@ -36768,6 +38599,9 @@
         <f aca="false">SUM(F859:O859)</f>
         <v>0</v>
       </c>
+      <c r="Q859" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="S859" s="1" t="n">
         <v>2</v>
       </c>
@@ -36807,6 +38641,9 @@
         <f aca="false">SUM(F861:O861)</f>
         <v>0</v>
       </c>
+      <c r="Q861" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="S861" s="1" t="n">
         <v>2</v>
       </c>
@@ -36825,6 +38662,9 @@
         <f aca="false">SUM(F862:O862)</f>
         <v>0</v>
       </c>
+      <c r="Q862" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="S862" s="1" t="n">
         <v>1</v>
       </c>
@@ -36849,6 +38689,9 @@
         <f aca="false">SUM(F863:O863)</f>
         <v>0</v>
       </c>
+      <c r="Q863" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="S863" s="1" t="n">
         <v>2</v>
       </c>
@@ -36863,9 +38706,39 @@
       <c r="C864" s="1" t="n">
         <v>2850</v>
       </c>
+      <c r="F864" s="1" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="G864" s="1" t="n">
+        <v>0.057</v>
+      </c>
+      <c r="H864" s="1" t="n">
+        <v>0.0267</v>
+      </c>
+      <c r="I864" s="1" t="n">
+        <v>0.0104</v>
+      </c>
+      <c r="J864" s="1" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="K864" s="1" t="n">
+        <v>0.0654</v>
+      </c>
+      <c r="L864" s="1" t="n">
+        <v>0.0515</v>
+      </c>
+      <c r="M864" s="1" t="n">
+        <v>0.0223</v>
+      </c>
+      <c r="N864" s="1" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="O864" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="P864" s="1" t="n">
         <f aca="false">SUM(F864:O864)</f>
-        <v>0</v>
+        <v>0.3313</v>
       </c>
       <c r="S864" s="1" t="n">
         <v>1</v>

</xml_diff>